<commit_message>
- implemented multiple Deathrattles - implemented debug behaviours - implemented Young Priestess, Feral Spirit and Soul of the Forest
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -874,9 +874,6 @@
     <t>SI:7 Agent</t>
   </si>
   <si>
-    <t>Siphon Sould</t>
-  </si>
-  <si>
     <t>Stampeding Kodo</t>
   </si>
   <si>
@@ -1238,6 +1235,9 @@
   </si>
   <si>
     <t>Missing</t>
+  </si>
+  <si>
+    <t>Siphon Soul</t>
   </si>
 </sst>
 </file>
@@ -1828,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="A264" sqref="A264"/>
+    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
+      <selection activeCell="A381" sqref="A381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,11 +1852,11 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F1" s="1"/>
       <c r="J1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K1">
         <f>COUNTIF(B:B,"Free")</f>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="F2" s="2"/>
       <c r="J2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K2">
         <f>COUNTIF(B:B,"Common")</f>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="J3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K3">
         <f>COUNTIF(B:B,"Rare")</f>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="F4" s="2"/>
       <c r="J4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K4">
         <f>COUNTIF(B:B,"Epic")</f>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="J5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K5">
         <f>COUNTIF(B:B,"Legendary")</f>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="F6" s="2"/>
       <c r="J6" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K6" s="1">
         <f>SUM(K1:K5)</f>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="J8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="F9" s="2"/>
       <c r="J9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
@@ -2100,7 +2100,7 @@
         <v>Implemented</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -2116,7 +2116,7 @@
         <v>Implemented</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -2132,7 +2132,7 @@
         <v>Implemented</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -2324,7 +2324,7 @@
         <v>Implemented</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -2356,7 +2356,7 @@
         <v>Implemented</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -2372,7 +2372,7 @@
         <v>Implemented</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F30" s="2"/>
     </row>
@@ -2388,7 +2388,7 @@
         <v>Implemented</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -2404,7 +2404,7 @@
         <v>Implemented</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -2676,7 +2676,7 @@
         <v>Implemented</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -2708,7 +2708,7 @@
         <v>Implemented</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -2724,7 +2724,7 @@
         <v>Implemented</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -2740,7 +2740,7 @@
         <v>Implemented</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -3108,7 +3108,7 @@
         <v>Implemented</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F76" s="2"/>
     </row>
@@ -3418,7 +3418,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
@@ -3434,7 +3434,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B97" t="s">
         <v>6</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B98" t="s">
         <v>6</v>
@@ -3466,7 +3466,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B99" t="s">
         <v>6</v>
@@ -3482,7 +3482,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B100" t="s">
         <v>6</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B101" t="s">
         <v>6</v>
@@ -3514,7 +3514,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B103" t="s">
         <v>6</v>
@@ -3546,7 +3546,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B104" t="s">
         <v>6</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
@@ -3578,7 +3578,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B106" t="s">
         <v>6</v>
@@ -3594,7 +3594,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B107" t="s">
         <v>6</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B108" t="s">
         <v>6</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B109" t="s">
         <v>6</v>
@@ -3642,7 +3642,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B110" t="s">
         <v>6</v>
@@ -3658,7 +3658,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
@@ -3674,7 +3674,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
@@ -3690,7 +3690,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B114" t="s">
         <v>6</v>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B115" t="s">
         <v>6</v>
@@ -3738,7 +3738,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B116" t="s">
         <v>6</v>
@@ -3754,7 +3754,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B117" t="s">
         <v>6</v>
@@ -3770,7 +3770,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
@@ -3802,7 +3802,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B123" t="s">
         <v>6</v>
@@ -3866,7 +3866,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B124" t="s">
         <v>6</v>
@@ -3882,7 +3882,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
@@ -3898,7 +3898,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
@@ -3914,7 +3914,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
@@ -3930,7 +3930,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
@@ -3946,7 +3946,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B129" t="s">
         <v>6</v>
@@ -3962,7 +3962,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
@@ -3978,7 +3978,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B131" t="s">
         <v>6</v>
@@ -3994,7 +3994,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B132" t="s">
         <v>6</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B133" t="s">
         <v>6</v>
@@ -4020,7 +4020,7 @@
         <v>Missing</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -4116,7 +4116,7 @@
         <v>Implemented</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -4132,7 +4132,7 @@
         <v>Implemented</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -4148,7 +4148,7 @@
         <v>Implemented</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -4164,7 +4164,7 @@
         <v>Implemented</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -4244,7 +4244,7 @@
         <v>Implemented</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4260,7 +4260,7 @@
         <v>Implemented</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4307,7 +4307,7 @@
         <v>Implemented</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4592,7 +4592,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4847,7 +4847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -5057,7 +5057,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -5072,7 +5072,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5267,7 +5267,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5297,7 +5297,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5312,7 +5312,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5523,7 +5523,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5555,7 +5555,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5641,7 +5641,7 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B240" t="s">
         <v>8</v>
@@ -5657,7 +5657,7 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B241" t="s">
         <v>8</v>
@@ -5673,7 +5673,7 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B242" t="s">
         <v>8</v>
@@ -5689,7 +5689,7 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B243" t="s">
         <v>8</v>
@@ -5699,13 +5699,13 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F243" s="2"/>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B244" t="s">
         <v>8</v>
@@ -5721,7 +5721,7 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B245" t="s">
         <v>8</v>
@@ -5737,7 +5737,7 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B246" t="s">
         <v>8</v>
@@ -5753,7 +5753,7 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B247" t="s">
         <v>8</v>
@@ -5769,7 +5769,7 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B248" t="s">
         <v>8</v>
@@ -5785,7 +5785,7 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B249" t="s">
         <v>8</v>
@@ -5801,7 +5801,7 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B250" t="s">
         <v>8</v>
@@ -5811,13 +5811,13 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F250" s="2"/>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B251" t="s">
         <v>8</v>
@@ -5827,13 +5827,13 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F251" s="2"/>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B252" t="s">
         <v>8</v>
@@ -5849,7 +5849,7 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B253" t="s">
         <v>8</v>
@@ -5865,7 +5865,7 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B254" t="s">
         <v>8</v>
@@ -5881,7 +5881,7 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B255" t="s">
         <v>8</v>
@@ -5897,7 +5897,7 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B256" t="s">
         <v>8</v>
@@ -5913,7 +5913,7 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B257" t="s">
         <v>8</v>
@@ -5923,13 +5923,13 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F257" s="2"/>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B258" t="s">
         <v>8</v>
@@ -5945,7 +5945,7 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B259" t="s">
         <v>8</v>
@@ -5961,7 +5961,7 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B260" t="s">
         <v>8</v>
@@ -5977,7 +5977,7 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B261" t="s">
         <v>8</v>
@@ -5993,7 +5993,7 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B262" t="s">
         <v>8</v>
@@ -6009,7 +6009,7 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B263" t="s">
         <v>8</v>
@@ -6041,7 +6041,7 @@
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B265" t="s">
         <v>8</v>
@@ -6057,7 +6057,7 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B266" t="s">
         <v>8</v>
@@ -6073,7 +6073,7 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B267" t="s">
         <v>7</v>
@@ -6121,7 +6121,7 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B270" t="s">
         <v>7</v>
@@ -6137,7 +6137,7 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B271" t="s">
         <v>7</v>
@@ -6153,7 +6153,7 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B272" t="s">
         <v>7</v>
@@ -6169,7 +6169,7 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B273" t="s">
         <v>7</v>
@@ -6182,7 +6182,7 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B274" t="s">
         <v>7</v>
@@ -6195,7 +6195,7 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B275" t="s">
         <v>7</v>
@@ -6211,7 +6211,7 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B276" t="s">
         <v>7</v>
@@ -6227,7 +6227,7 @@
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B277" t="s">
         <v>7</v>
@@ -6243,7 +6243,7 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B278" t="s">
         <v>7</v>
@@ -6259,7 +6259,7 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B279" t="s">
         <v>7</v>
@@ -6272,7 +6272,7 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B280" t="s">
         <v>7</v>
@@ -6285,7 +6285,7 @@
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B281" t="s">
         <v>7</v>
@@ -6298,7 +6298,7 @@
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B282" t="s">
         <v>7</v>
@@ -6311,7 +6311,7 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B283" t="s">
         <v>7</v>
@@ -6324,7 +6324,7 @@
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B284" t="s">
         <v>7</v>
@@ -6337,7 +6337,7 @@
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B285" t="s">
         <v>7</v>
@@ -6350,7 +6350,7 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B286" t="s">
         <v>7</v>
@@ -6363,7 +6363,7 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B287" t="s">
         <v>7</v>
@@ -6376,7 +6376,7 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B288" t="s">
         <v>7</v>
@@ -6389,7 +6389,7 @@
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B289" t="s">
         <v>7</v>
@@ -6402,7 +6402,7 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B290" t="s">
         <v>7</v>
@@ -6415,7 +6415,7 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B291" t="s">
         <v>7</v>
@@ -6428,7 +6428,7 @@
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B292" t="s">
         <v>7</v>
@@ -6441,7 +6441,7 @@
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B293" t="s">
         <v>7</v>
@@ -6454,7 +6454,7 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B294" t="s">
         <v>7</v>
@@ -6467,7 +6467,7 @@
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B295" t="s">
         <v>7</v>
@@ -6480,7 +6480,7 @@
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B296" t="s">
         <v>7</v>
@@ -6493,7 +6493,7 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B297" t="s">
         <v>7</v>
@@ -6506,7 +6506,7 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B298" t="s">
         <v>7</v>
@@ -6519,7 +6519,7 @@
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B299" t="s">
         <v>7</v>
@@ -6532,7 +6532,7 @@
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B300" t="s">
         <v>7</v>
@@ -6545,7 +6545,7 @@
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B301" t="s">
         <v>7</v>
@@ -6558,7 +6558,7 @@
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B302" t="s">
         <v>7</v>
@@ -6835,7 +6835,7 @@
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B321" t="s">
         <v>5</v>
@@ -6845,7 +6845,7 @@
         <v>Implemented</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -7029,7 +7029,7 @@
         <v>Missing</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
@@ -7505,7 +7505,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>280</v>
+        <v>401</v>
       </c>
       <c r="B373" t="s">
         <v>5</v>
@@ -7517,7 +7517,7 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B374" t="s">
         <v>5</v>
@@ -7529,7 +7529,7 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B375" t="s">
         <v>5</v>
@@ -7541,7 +7541,7 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B376" t="s">
         <v>5</v>
@@ -7553,7 +7553,7 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B377" t="s">
         <v>5</v>
@@ -7565,7 +7565,7 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B378" t="s">
         <v>5</v>
@@ -7577,7 +7577,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B379" t="s">
         <v>5</v>
@@ -7589,7 +7589,7 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B380" t="s">
         <v>5</v>
@@ -7601,7 +7601,7 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B381" t="s">
         <v>5</v>
@@ -7613,7 +7613,7 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B382" t="s">
         <v>5</v>
@@ -7625,7 +7625,7 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B383" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
- added EntityReference.EVENT_TARGET as possible target - refactored a lot in the process
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$251</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$253</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="401">
   <si>
     <t>Cardname</t>
   </si>
@@ -1223,9 +1223,6 @@
   </si>
   <si>
     <t>Stormwind Knight</t>
-  </si>
-  <si>
-    <t>Assasinate</t>
   </si>
   <si>
     <t>PowerOverwhelming</t>
@@ -1289,225 +1286,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1828,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="A381" sqref="A381"/>
+    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
+      <selection activeCell="A325" sqref="A325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2010,11 +1789,11 @@
       </c>
       <c r="F8" s="2"/>
       <c r="J8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2033,11 +1812,11 @@
       </c>
       <c r="F9" s="2"/>
       <c r="J9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -4352,7 +4131,7 @@
         <v>Implemented</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>213</v>
+        <v>290</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4367,7 +4146,7 @@
         <v>Implemented</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>125</v>
+        <v>213</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4382,7 +4161,7 @@
         <v>Implemented</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4397,7 +4176,7 @@
         <v>Implemented</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4412,7 +4191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>129</v>
+        <v>21</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4427,7 +4206,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4442,7 +4221,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>150</v>
+        <v>31</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4457,7 +4236,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>57</v>
+        <v>150</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4472,7 +4251,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4487,7 +4266,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4502,7 +4281,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4517,7 +4296,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4532,7 +4311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4547,7 +4326,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>175</v>
+        <v>78</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4562,7 +4341,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4577,7 +4356,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4592,7 +4371,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>375</v>
+        <v>182</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4607,7 +4386,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>132</v>
+        <v>375</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4622,7 +4401,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4637,7 +4416,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4652,7 +4431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4667,7 +4446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>161</v>
+        <v>67</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4682,7 +4461,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4697,7 +4476,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>82</v>
+        <v>167</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4712,7 +4491,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4727,7 +4506,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4742,7 +4521,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4757,7 +4536,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4772,7 +4551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4787,7 +4566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4802,7 +4581,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>188</v>
+        <v>109</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4817,7 +4596,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4832,7 +4611,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4847,7 +4626,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>397</v>
+        <v>203</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4862,7 +4641,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4877,7 +4656,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4892,7 +4671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>128</v>
+        <v>19</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4907,7 +4686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4922,7 +4701,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4937,7 +4716,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4952,7 +4731,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>140</v>
+        <v>36</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4967,7 +4746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4982,7 +4761,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4997,7 +4776,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -5012,7 +4791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>186</v>
+        <v>104</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -5027,7 +4806,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>112</v>
+        <v>186</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -5042,7 +4821,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -5057,7 +4836,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>364</v>
+        <v>113</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -5072,7 +4851,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5087,7 +4866,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>9</v>
+        <v>377</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -5102,7 +4881,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5117,7 +4896,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>145</v>
+        <v>23</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -5132,7 +4911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -5147,7 +4926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -5162,7 +4941,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>48</v>
+        <v>243</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -5177,7 +4956,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -5192,7 +4971,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5207,7 +4986,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>64</v>
+        <v>155</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5222,7 +5001,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>166</v>
+        <v>50</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5237,7 +5016,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5252,7 +5031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5267,7 +5046,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>373</v>
+        <v>102</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5282,7 +5061,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5297,7 +5076,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5312,7 +5091,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>386</v>
+        <v>205</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5327,7 +5106,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>130</v>
+        <v>385</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5342,7 +5121,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>33</v>
+        <v>386</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5357,7 +5136,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5372,7 +5151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5387,7 +5166,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>40</v>
+        <v>141</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5402,7 +5181,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>153</v>
+        <v>39</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5417,7 +5196,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5432,7 +5211,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5447,7 +5226,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>177</v>
+        <v>62</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5462,7 +5241,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5477,7 +5256,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5492,7 +5271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5507,7 +5286,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>114</v>
+        <v>185</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5523,7 +5302,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>370</v>
+        <v>107</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5539,7 +5318,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>200</v>
+        <v>114</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5555,7 +5334,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5571,7 +5350,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>124</v>
+        <v>200</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5587,7 +5366,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>15</v>
+        <v>378</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5603,7 +5382,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5619,7 +5398,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5635,7 +5414,7 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>30</v>
+        <v>127</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5651,7 +5430,7 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5667,7 +5446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5683,7 +5462,7 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="F242" s="2"/>
     </row>
@@ -5699,7 +5478,7 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>336</v>
+        <v>42</v>
       </c>
       <c r="F243" s="2"/>
     </row>
@@ -5715,7 +5494,7 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="F244" s="2"/>
     </row>
@@ -5731,7 +5510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>162</v>
+        <v>336</v>
       </c>
       <c r="F245" s="2"/>
     </row>
@@ -5747,7 +5526,7 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="F246" s="2"/>
     </row>
@@ -5763,7 +5542,7 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="F247" s="2"/>
     </row>
@@ -5779,7 +5558,7 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="F248" s="2"/>
     </row>
@@ -5795,7 +5574,7 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F249" s="2"/>
     </row>
@@ -5811,7 +5590,7 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>381</v>
+        <v>111</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5827,7 +5606,7 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>383</v>
+        <v>191</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5843,7 +5622,7 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>32</v>
+        <v>381</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5859,7 +5638,7 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>137</v>
+        <v>383</v>
       </c>
       <c r="F253" s="2"/>
     </row>
@@ -5875,7 +5654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>151</v>
+        <v>32</v>
       </c>
       <c r="F254" s="2"/>
     </row>
@@ -5891,7 +5670,7 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>246</v>
+        <v>137</v>
       </c>
       <c r="F255" s="2"/>
     </row>
@@ -5907,7 +5686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>198</v>
+        <v>151</v>
       </c>
       <c r="F256" s="2"/>
     </row>
@@ -5923,7 +5702,7 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>398</v>
+        <v>246</v>
       </c>
       <c r="F257" s="2"/>
     </row>
@@ -5939,7 +5718,7 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>114</v>
+        <v>198</v>
       </c>
       <c r="F258" s="2"/>
     </row>
@@ -5955,7 +5734,7 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>44</v>
+        <v>397</v>
       </c>
       <c r="F259" s="2"/>
     </row>
@@ -5971,7 +5750,7 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="F260" s="2"/>
     </row>
@@ -5987,7 +5766,7 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>122</v>
+        <v>44</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -6003,7 +5782,7 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>228</v>
+        <v>63</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -6019,7 +5798,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -6032,10 +5811,10 @@
       </c>
       <c r="C264" t="str">
         <f>IF(COUNTIF(D:D,$A264)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>173</v>
+        <v>228</v>
       </c>
       <c r="F264" s="2"/>
     </row>
@@ -6051,7 +5830,7 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F265" s="2"/>
     </row>
@@ -6067,7 +5846,7 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -6083,7 +5862,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>203</v>
+        <v>150</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -6099,7 +5878,7 @@
         <v>Missing</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -6115,7 +5894,7 @@
         <v>Missing</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>134</v>
+        <v>203</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -6131,7 +5910,7 @@
         <v>Missing</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -6147,7 +5926,7 @@
         <v>Missing</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -6163,7 +5942,7 @@
         <v>Missing</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -6178,6 +5957,9 @@
         <f>IF(COUNTIF(D:D,$A273)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D273" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="F273" s="2"/>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
@@ -6191,6 +5973,9 @@
         <f>IF(COUNTIF(D:D,$A274)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D274" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="F274" s="2"/>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
@@ -6204,9 +5989,6 @@
         <f>IF(COUNTIF(D:D,$A275)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-      <c r="D275" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="F275" s="2"/>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
@@ -6220,9 +6002,6 @@
         <f>IF(COUNTIF(D:D,$A276)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-      <c r="D276" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="F276" s="2"/>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
@@ -6237,7 +6016,7 @@
         <v>Missing</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>234</v>
+        <v>101</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -6253,7 +6032,7 @@
         <v>Missing</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>106</v>
+        <v>160</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -6268,6 +6047,9 @@
         <f>IF(COUNTIF(D:D,$A279)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D279" s="2" t="s">
+        <v>234</v>
+      </c>
       <c r="F279" s="2"/>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
@@ -6281,6 +6063,9 @@
         <f>IF(COUNTIF(D:D,$A280)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D280" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="F280" s="2"/>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
@@ -6684,9 +6469,6 @@
         <f>IF(COUNTIF(D:D,$A311)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D311" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="F311" s="2"/>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.25">
@@ -6700,9 +6482,6 @@
         <f>IF(COUNTIF(D:D,$A312)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D312" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F312" s="2"/>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.25">
@@ -6717,7 +6496,7 @@
         <v>Implemented</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>65</v>
+        <v>231</v>
       </c>
       <c r="F313" s="2"/>
     </row>
@@ -6733,7 +6512,7 @@
         <v>Implemented</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="F314" s="2"/>
     </row>
@@ -6749,7 +6528,7 @@
         <v>Implemented</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="F315" s="2"/>
     </row>
@@ -6765,7 +6544,7 @@
         <v>Implemented</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="F316" s="2"/>
     </row>
@@ -6781,7 +6560,7 @@
         <v>Implemented</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="F317" s="2"/>
     </row>
@@ -6797,7 +6576,7 @@
         <v>Implemented</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>115</v>
+        <v>54</v>
       </c>
       <c r="F318" s="2"/>
     </row>
@@ -6813,7 +6592,7 @@
         <v>Implemented</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="F319" s="2"/>
     </row>
@@ -6829,7 +6608,7 @@
         <v>Implemented</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="F320" s="2"/>
     </row>
@@ -6845,7 +6624,7 @@
         <v>Implemented</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>384</v>
+        <v>37</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -6861,7 +6640,7 @@
         <v>Missing</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6877,7 +6656,7 @@
         <v>Missing</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>215</v>
+        <v>384</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6893,7 +6672,7 @@
         <v>Missing</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>254</v>
+        <v>156</v>
       </c>
       <c r="F324" s="2"/>
     </row>
@@ -6909,7 +6688,7 @@
         <v>Missing</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>132</v>
+        <v>215</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
@@ -6924,7 +6703,7 @@
         <v>Missing</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>167</v>
+        <v>254</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
@@ -6939,7 +6718,7 @@
         <v>Missing</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>43</v>
+        <v>132</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -6954,7 +6733,7 @@
         <v>Missing</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
@@ -6969,7 +6748,7 @@
         <v>Missing</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>227</v>
+        <v>43</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -6984,7 +6763,7 @@
         <v>Missing</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>85</v>
+        <v>155</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
@@ -6999,7 +6778,7 @@
         <v>Missing</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>123</v>
+        <v>227</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -7014,7 +6793,7 @@
         <v>Missing</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>238</v>
+        <v>85</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
@@ -7029,7 +6808,7 @@
         <v>Missing</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>368</v>
+        <v>123</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
@@ -7044,7 +6823,7 @@
         <v>Missing</v>
       </c>
       <c r="D334" s="2" t="s">
-        <v>104</v>
+        <v>238</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
@@ -7058,6 +6837,9 @@
         <f>IF(COUNTIF(D:D,$A335)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D335" s="2" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
@@ -7070,6 +6852,9 @@
         <f>IF(COUNTIF(D:D,$A336)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D336" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
@@ -7128,7 +6913,7 @@
       </c>
       <c r="C341" t="str">
         <f>IF(COUNTIF(D:D,$A341)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
@@ -7505,7 +7290,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B373" t="s">
         <v>5</v>
@@ -7632,7 +7417,7 @@
       </c>
       <c r="C383" t="str">
         <f>IF(COUNTIF(D:D,$A383)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- changed project to Java 8 and JavaFX 8 - upgraded to Eclipse Luna - added BlessedChampion
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$253</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$261</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="401">
   <si>
     <t>Cardname</t>
   </si>
@@ -1607,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="A325" sqref="A325"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D324" sqref="D324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,7 +1654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>223</v>
       </c>
       <c r="F2" s="2"/>
       <c r="J2" t="s">
@@ -1677,7 +1677,7 @@
         <v>Implemented</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2"/>
       <c r="J3" t="s">
@@ -1700,7 +1700,7 @@
         <v>Implemented</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>61</v>
+        <v>144</v>
       </c>
       <c r="F4" s="2"/>
       <c r="J4" t="s">
@@ -1723,7 +1723,7 @@
         <v>Implemented</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F5" s="2"/>
       <c r="J5" t="s">
@@ -1746,7 +1746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="2"/>
       <c r="J6" s="1" t="s">
@@ -1769,7 +1769,7 @@
         <v>Implemented</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>171</v>
+        <v>72</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1785,7 +1785,7 @@
         <v>Implemented</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>81</v>
+        <v>171</v>
       </c>
       <c r="F8" s="2"/>
       <c r="J8" t="s">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
         <v>Implemented</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F9" s="2"/>
       <c r="J9" t="s">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1831,7 +1831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>174</v>
+        <v>86</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1847,7 +1847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1863,7 +1863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>105</v>
+        <v>176</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -1879,7 +1879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>365</v>
+        <v>105</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -1895,7 +1895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>371</v>
+        <v>194</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1911,7 +1911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1927,7 +1927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>211</v>
+        <v>371</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -1943,7 +1943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>384</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1959,7 +1959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -1975,7 +1975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1991,7 +1991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>149</v>
+        <v>14</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -2007,7 +2007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -2023,7 +2023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -2039,7 +2039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -2055,7 +2055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -2071,7 +2071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -2087,7 +2087,7 @@
         <v>Implemented</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>184</v>
+        <v>75</v>
       </c>
       <c r="F26" s="2"/>
     </row>
@@ -2103,7 +2103,7 @@
         <v>Implemented</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>323</v>
+        <v>88</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -2119,7 +2119,7 @@
         <v>Implemented</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -2135,7 +2135,7 @@
         <v>Implemented</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>366</v>
+        <v>323</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -2151,7 +2151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>372</v>
+        <v>192</v>
       </c>
       <c r="F30" s="2"/>
     </row>
@@ -2167,7 +2167,7 @@
         <v>Implemented</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -2183,7 +2183,7 @@
         <v>Implemented</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -2199,7 +2199,7 @@
         <v>Implemented</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>206</v>
+        <v>374</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -2215,7 +2215,7 @@
         <v>Implemented</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>11</v>
+        <v>376</v>
       </c>
       <c r="F34" s="2"/>
     </row>
@@ -2231,7 +2231,7 @@
         <v>Implemented</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>12</v>
+        <v>206</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -2247,7 +2247,7 @@
         <v>Implemented</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F36" s="2"/>
     </row>
@@ -2263,7 +2263,7 @@
         <v>Implemented</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
       <c r="F37" s="2"/>
     </row>
@@ -2279,7 +2279,7 @@
         <v>Implemented</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>231</v>
+        <v>13</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -2295,7 +2295,7 @@
         <v>Implemented</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -2311,7 +2311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -2327,7 +2327,7 @@
         <v>Implemented</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -2343,7 +2343,7 @@
         <v>Implemented</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -2359,7 +2359,7 @@
         <v>Implemented</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -2375,7 +2375,7 @@
         <v>Implemented</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>160</v>
+        <v>49</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -2391,7 +2391,7 @@
         <v>Implemented</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -2407,7 +2407,7 @@
         <v>Implemented</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -2423,7 +2423,7 @@
         <v>Implemented</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -2439,7 +2439,7 @@
         <v>Implemented</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -2455,7 +2455,7 @@
         <v>Implemented</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>319</v>
+        <v>85</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -2471,7 +2471,7 @@
         <v>Implemented</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>193</v>
+        <v>96</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -2487,7 +2487,7 @@
         <v>Implemented</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -2503,7 +2503,7 @@
         <v>Implemented</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>286</v>
+        <v>193</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -2519,7 +2519,7 @@
         <v>Implemented</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>382</v>
+        <v>325</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -2535,7 +2535,7 @@
         <v>Implemented</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>115</v>
+        <v>286</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -2551,7 +2551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>121</v>
+        <v>382</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -2567,7 +2567,7 @@
         <v>Implemented</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="F56" s="2"/>
     </row>
@@ -2583,7 +2583,7 @@
         <v>Implemented</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F57" s="2"/>
     </row>
@@ -2599,7 +2599,7 @@
         <v>Implemented</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="F58" s="2"/>
     </row>
@@ -2615,7 +2615,7 @@
         <v>Implemented</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -2631,7 +2631,7 @@
         <v>Implemented</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>215</v>
+        <v>120</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -2647,7 +2647,7 @@
         <v>Implemented</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>216</v>
+        <v>123</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -2663,7 +2663,7 @@
         <v>Implemented</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F62" s="2"/>
     </row>
@@ -2679,7 +2679,7 @@
         <v>Implemented</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F63" s="2"/>
     </row>
@@ -2695,7 +2695,7 @@
         <v>Implemented</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="F64" s="2"/>
     </row>
@@ -2711,7 +2711,7 @@
         <v>Implemented</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F65" s="2"/>
     </row>
@@ -2727,7 +2727,7 @@
         <v>Implemented</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -2743,7 +2743,7 @@
         <v>Implemented</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -2759,7 +2759,7 @@
         <v>Implemented</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="F68" s="2"/>
     </row>
@@ -2775,7 +2775,7 @@
         <v>Implemented</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -2791,7 +2791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="F70" s="2"/>
     </row>
@@ -2807,7 +2807,7 @@
         <v>Implemented</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>24</v>
+        <v>227</v>
       </c>
       <c r="F71" s="2"/>
     </row>
@@ -2823,7 +2823,7 @@
         <v>Implemented</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>25</v>
+        <v>131</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -2839,7 +2839,7 @@
         <v>Implemented</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F73" s="2"/>
     </row>
@@ -2855,7 +2855,7 @@
         <v>Implemented</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F74" s="2"/>
     </row>
@@ -2871,7 +2871,7 @@
         <v>Implemented</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>228</v>
+        <v>26</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -2887,7 +2887,7 @@
         <v>Implemented</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>394</v>
+        <v>28</v>
       </c>
       <c r="F76" s="2"/>
     </row>
@@ -2903,7 +2903,7 @@
         <v>Implemented</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
       <c r="F77" s="2"/>
     </row>
@@ -2919,7 +2919,7 @@
         <v>Implemented</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>137</v>
+        <v>394</v>
       </c>
       <c r="F78" s="2"/>
     </row>
@@ -2935,7 +2935,7 @@
         <v>Implemented</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F79" s="2"/>
     </row>
@@ -2951,7 +2951,7 @@
         <v>Implemented</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F80" s="2"/>
     </row>
@@ -2967,7 +2967,7 @@
         <v>Implemented</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F81" s="2"/>
     </row>
@@ -2983,7 +2983,7 @@
         <v>Implemented</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>233</v>
+        <v>138</v>
       </c>
       <c r="F82" s="2"/>
     </row>
@@ -2999,7 +2999,7 @@
         <v>Implemented</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>234</v>
+        <v>35</v>
       </c>
       <c r="F83" s="2"/>
     </row>
@@ -3015,7 +3015,7 @@
         <v>Implemented</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>142</v>
+        <v>233</v>
       </c>
       <c r="F84" s="2"/>
     </row>
@@ -3031,7 +3031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>38</v>
+        <v>234</v>
       </c>
       <c r="F85" s="2"/>
     </row>
@@ -3047,7 +3047,7 @@
         <v>Implemented</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F86" s="2"/>
     </row>
@@ -3063,7 +3063,7 @@
         <v>Implemented</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="F87" s="2"/>
     </row>
@@ -3079,7 +3079,7 @@
         <v>Implemented</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="F88" s="2"/>
     </row>
@@ -3095,7 +3095,7 @@
         <v>Implemented</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>238</v>
+        <v>147</v>
       </c>
       <c r="F89" s="2"/>
     </row>
@@ -3111,7 +3111,7 @@
         <v>Implemented</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="F90" s="2"/>
     </row>
@@ -3127,7 +3127,7 @@
         <v>Implemented</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="F91" s="2"/>
     </row>
@@ -3143,7 +3143,7 @@
         <v>Implemented</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F92" s="2"/>
     </row>
@@ -3156,10 +3156,10 @@
       </c>
       <c r="C93" t="str">
         <f>IF(COUNTIF(D:D,$A93)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F93" s="2"/>
     </row>
@@ -3175,7 +3175,7 @@
         <v>Implemented</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>52</v>
+        <v>154</v>
       </c>
       <c r="F94" s="2"/>
     </row>
@@ -3191,7 +3191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>53</v>
+        <v>157</v>
       </c>
       <c r="F95" s="2"/>
     </row>
@@ -3207,7 +3207,7 @@
         <v>Implemented</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>246</v>
+        <v>52</v>
       </c>
       <c r="F96" s="2"/>
     </row>
@@ -3223,7 +3223,7 @@
         <v>Implemented</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F97" s="2"/>
     </row>
@@ -3239,7 +3239,7 @@
         <v>Missing</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>55</v>
+        <v>246</v>
       </c>
       <c r="F98" s="2"/>
     </row>
@@ -3255,7 +3255,7 @@
         <v>Missing</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F99" s="2"/>
     </row>
@@ -3271,7 +3271,7 @@
         <v>Missing</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F100" s="2"/>
     </row>
@@ -3287,7 +3287,7 @@
         <v>Missing</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>158</v>
+        <v>56</v>
       </c>
       <c r="F101" s="2"/>
     </row>
@@ -3303,7 +3303,7 @@
         <v>Missing</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>250</v>
+        <v>58</v>
       </c>
       <c r="F102" s="2"/>
     </row>
@@ -3319,7 +3319,7 @@
         <v>Missing</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>251</v>
+        <v>158</v>
       </c>
       <c r="F103" s="2"/>
     </row>
@@ -3335,7 +3335,7 @@
         <v>Missing</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>163</v>
+        <v>250</v>
       </c>
       <c r="F104" s="2"/>
     </row>
@@ -3351,7 +3351,7 @@
         <v>Missing</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>73</v>
+        <v>251</v>
       </c>
       <c r="F105" s="2"/>
     </row>
@@ -3367,7 +3367,7 @@
         <v>Missing</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="F106" s="2"/>
     </row>
@@ -3383,7 +3383,7 @@
         <v>Missing</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>164</v>
+        <v>73</v>
       </c>
       <c r="F107" s="2"/>
     </row>
@@ -3399,7 +3399,7 @@
         <v>Missing</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>254</v>
+        <v>74</v>
       </c>
       <c r="F108" s="2"/>
     </row>
@@ -3415,7 +3415,7 @@
         <v>Missing</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="F109" s="2"/>
     </row>
@@ -3431,7 +3431,7 @@
         <v>Missing</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>165</v>
+        <v>254</v>
       </c>
       <c r="F110" s="2"/>
     </row>
@@ -3447,7 +3447,7 @@
         <v>Missing</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>257</v>
+        <v>76</v>
       </c>
       <c r="F111" s="2"/>
     </row>
@@ -3463,7 +3463,7 @@
         <v>Missing</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F112" s="2"/>
     </row>
@@ -3479,7 +3479,7 @@
         <v>Missing</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>79</v>
+        <v>257</v>
       </c>
       <c r="F113" s="2"/>
     </row>
@@ -3495,7 +3495,7 @@
         <v>Missing</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F114" s="2"/>
     </row>
@@ -3511,7 +3511,7 @@
         <v>Missing</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F115" s="2"/>
     </row>
@@ -3527,7 +3527,7 @@
         <v>Missing</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F116" s="2"/>
     </row>
@@ -3543,7 +3543,7 @@
         <v>Missing</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F117" s="2"/>
     </row>
@@ -3559,7 +3559,7 @@
         <v>Missing</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>90</v>
+        <v>173</v>
       </c>
       <c r="F118" s="2"/>
     </row>
@@ -3575,7 +3575,7 @@
         <v>Missing</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F119" s="2"/>
     </row>
@@ -3591,7 +3591,7 @@
         <v>Missing</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F120" s="2"/>
     </row>
@@ -3607,7 +3607,7 @@
         <v>Missing</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F121" s="2"/>
     </row>
@@ -3623,7 +3623,7 @@
         <v>Missing</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F122" s="2"/>
     </row>
@@ -3639,7 +3639,7 @@
         <v>Missing</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>178</v>
+        <v>94</v>
       </c>
       <c r="F123" s="2"/>
     </row>
@@ -3655,7 +3655,7 @@
         <v>Missing</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>179</v>
+        <v>95</v>
       </c>
       <c r="F124" s="2"/>
     </row>
@@ -3671,7 +3671,7 @@
         <v>Missing</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>98</v>
+        <v>178</v>
       </c>
       <c r="F125" s="2"/>
     </row>
@@ -3687,7 +3687,7 @@
         <v>Missing</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>99</v>
+        <v>272</v>
       </c>
       <c r="F126" s="2"/>
     </row>
@@ -3703,7 +3703,7 @@
         <v>Missing</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>100</v>
+        <v>179</v>
       </c>
       <c r="F127" s="2"/>
     </row>
@@ -3719,7 +3719,7 @@
         <v>Missing</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F128" s="2"/>
     </row>
@@ -3735,7 +3735,7 @@
         <v>Missing</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>183</v>
+        <v>99</v>
       </c>
       <c r="F129" s="2"/>
     </row>
@@ -3751,7 +3751,7 @@
         <v>Missing</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F130" s="2"/>
     </row>
@@ -3767,7 +3767,7 @@
         <v>Implemented</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F131" s="2"/>
     </row>
@@ -3783,7 +3783,7 @@
         <v>Missing</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F132" s="2"/>
     </row>
@@ -3799,7 +3799,7 @@
         <v>Missing</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>395</v>
+        <v>106</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -3815,7 +3815,7 @@
         <v>Implemented</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>189</v>
+        <v>110</v>
       </c>
       <c r="F134" s="2"/>
     </row>
@@ -3831,7 +3831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F135" s="2"/>
     </row>
@@ -3847,7 +3847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>195</v>
+        <v>395</v>
       </c>
       <c r="F136" s="2"/>
     </row>
@@ -3863,7 +3863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -3879,7 +3879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -3895,7 +3895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>367</v>
+        <v>195</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -3911,7 +3911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>368</v>
+        <v>196</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -3927,7 +3927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>369</v>
+        <v>197</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -3943,7 +3943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>396</v>
+        <v>367</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -3959,7 +3959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>199</v>
+        <v>368</v>
       </c>
       <c r="F143" s="2"/>
     </row>
@@ -3975,7 +3975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>201</v>
+        <v>369</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -3991,7 +3991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>204</v>
+        <v>396</v>
       </c>
       <c r="F145" s="2"/>
     </row>
@@ -4007,7 +4007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F146" s="2"/>
     </row>
@@ -4023,7 +4023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>379</v>
+        <v>201</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4039,7 +4039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>380</v>
+        <v>204</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4055,7 +4055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F149" s="2"/>
     </row>
@@ -4071,7 +4071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>209</v>
+        <v>379</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4086,7 +4086,7 @@
         <v>Implemented</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>Implemented</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4116,7 +4116,7 @@
         <v>Implemented</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4131,7 +4131,7 @@
         <v>Implemented</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>290</v>
+        <v>387</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4146,7 +4146,7 @@
         <v>Implemented</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
         <v>Implemented</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4176,7 +4176,7 @@
         <v>Implemented</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>20</v>
+        <v>290</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>21</v>
+        <v>213</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4206,7 +4206,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>31</v>
+        <v>225</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>150</v>
+        <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4251,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,7 +4296,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,7 +4326,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>175</v>
+        <v>60</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4356,7 +4356,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>181</v>
+        <v>65</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,7 +4371,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>182</v>
+        <v>69</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,7 +4386,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>375</v>
+        <v>78</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>37</v>
+        <v>181</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,7 +4431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>66</v>
+        <v>182</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4446,7 +4446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>67</v>
+        <v>375</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4491,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4506,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4521,7 +4521,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4536,7 +4536,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>92</v>
+        <v>167</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,7 +4551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,7 +4566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>188</v>
+        <v>92</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +4611,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>202</v>
+        <v>97</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>203</v>
+        <v>108</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +4641,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,7 +4656,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>19</v>
+        <v>202</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>128</v>
+        <v>203</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +4701,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>133</v>
+        <v>18</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4716,7 +4716,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>134</v>
+        <v>17</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4731,7 +4731,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4746,7 +4746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4761,7 +4761,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4776,7 +4776,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>43</v>
+        <v>134</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>104</v>
+        <v>36</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>186</v>
+        <v>140</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,7 +4821,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4836,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4851,7 +4851,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>364</v>
+        <v>104</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4866,7 +4866,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>377</v>
+        <v>186</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,7 +4881,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>9</v>
+        <v>112</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4896,7 +4896,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4911,7 +4911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>145</v>
+        <v>364</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>146</v>
+        <v>377</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4941,7 +4941,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>243</v>
+        <v>9</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>45</v>
+        <v>214</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4971,7 +4971,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,7 +4986,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,7 +5001,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>50</v>
+        <v>146</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5016,7 +5016,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>64</v>
+        <v>243</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5031,7 +5031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>166</v>
+        <v>45</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5061,7 +5061,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,7 +5076,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>373</v>
+        <v>50</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,7 +5091,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>205</v>
+        <v>64</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>385</v>
+        <v>255</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,7 +5121,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>386</v>
+        <v>166</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,7 +5136,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5166,7 +5166,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>141</v>
+        <v>373</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,7 +5181,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>39</v>
+        <v>205</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>40</v>
+        <v>385</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5211,7 +5211,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>153</v>
+        <v>386</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5226,7 +5226,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,7 +5256,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5271,7 +5271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>103</v>
+        <v>236</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>185</v>
+        <v>39</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5302,7 +5302,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5318,7 +5318,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5334,7 +5334,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>370</v>
+        <v>62</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5350,7 +5350,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>200</v>
+        <v>87</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5366,7 +5366,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>378</v>
+        <v>177</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5382,7 +5382,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5398,7 +5398,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5414,7 +5414,7 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5430,7 +5430,7 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5446,7 +5446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>30</v>
+        <v>370</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5462,7 +5462,7 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>136</v>
+        <v>200</v>
       </c>
       <c r="F242" s="2"/>
     </row>
@@ -5478,7 +5478,7 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>42</v>
+        <v>378</v>
       </c>
       <c r="F243" s="2"/>
     </row>
@@ -5494,7 +5494,7 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="F244" s="2"/>
     </row>
@@ -5510,7 +5510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>336</v>
+        <v>15</v>
       </c>
       <c r="F245" s="2"/>
     </row>
@@ -5526,7 +5526,7 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
       <c r="F246" s="2"/>
     </row>
@@ -5542,7 +5542,7 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="F247" s="2"/>
     </row>
@@ -5558,7 +5558,7 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="F248" s="2"/>
     </row>
@@ -5574,7 +5574,7 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>180</v>
+        <v>30</v>
       </c>
       <c r="F249" s="2"/>
     </row>
@@ -5590,7 +5590,7 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5606,7 +5606,7 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>191</v>
+        <v>42</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5622,7 +5622,7 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>381</v>
+        <v>44</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5638,7 +5638,7 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>383</v>
+        <v>336</v>
       </c>
       <c r="F253" s="2"/>
     </row>
@@ -5654,7 +5654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="F254" s="2"/>
     </row>
@@ -5670,7 +5670,7 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="F255" s="2"/>
     </row>
@@ -5686,7 +5686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="F256" s="2"/>
     </row>
@@ -5702,7 +5702,7 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>246</v>
+        <v>180</v>
       </c>
       <c r="F257" s="2"/>
     </row>
@@ -5718,7 +5718,7 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>198</v>
+        <v>111</v>
       </c>
       <c r="F258" s="2"/>
     </row>
@@ -5734,7 +5734,7 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>397</v>
+        <v>191</v>
       </c>
       <c r="F259" s="2"/>
     </row>
@@ -5750,7 +5750,7 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>114</v>
+        <v>381</v>
       </c>
       <c r="F260" s="2"/>
     </row>
@@ -5766,7 +5766,7 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>44</v>
+        <v>383</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -5782,7 +5782,7 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -5798,7 +5798,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5814,7 +5814,7 @@
         <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>228</v>
+        <v>151</v>
       </c>
       <c r="F264" s="2"/>
     </row>
@@ -5830,7 +5830,7 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>154</v>
+        <v>246</v>
       </c>
       <c r="F265" s="2"/>
     </row>
@@ -5846,7 +5846,7 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -5862,7 +5862,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>150</v>
+        <v>397</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5878,7 +5878,7 @@
         <v>Missing</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5894,7 +5894,7 @@
         <v>Missing</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>203</v>
+        <v>44</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -5910,7 +5910,7 @@
         <v>Missing</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>133</v>
+        <v>63</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -5926,7 +5926,7 @@
         <v>Missing</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -5942,7 +5942,7 @@
         <v>Missing</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>130</v>
+        <v>228</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -5958,7 +5958,7 @@
         <v>Missing</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -5974,7 +5974,7 @@
         <v>Missing</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>92</v>
+        <v>173</v>
       </c>
       <c r="F274" s="2"/>
     </row>
@@ -5989,6 +5989,9 @@
         <f>IF(COUNTIF(D:D,$A275)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D275" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="F275" s="2"/>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
@@ -6002,6 +6005,9 @@
         <f>IF(COUNTIF(D:D,$A276)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D276" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="F276" s="2"/>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
@@ -6016,7 +6022,7 @@
         <v>Missing</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -6032,7 +6038,7 @@
         <v>Missing</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -6048,7 +6054,7 @@
         <v>Missing</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>234</v>
+        <v>134</v>
       </c>
       <c r="F279" s="2"/>
     </row>
@@ -6064,7 +6070,7 @@
         <v>Missing</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="F280" s="2"/>
     </row>
@@ -6079,6 +6085,9 @@
         <f>IF(COUNTIF(D:D,$A281)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D281" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="F281" s="2"/>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
@@ -6092,6 +6101,9 @@
         <f>IF(COUNTIF(D:D,$A282)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D282" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="F282" s="2"/>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
@@ -6131,6 +6143,9 @@
         <f>IF(COUNTIF(D:D,$A285)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D285" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="F285" s="2"/>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
@@ -6144,6 +6159,9 @@
         <f>IF(COUNTIF(D:D,$A286)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D286" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="F286" s="2"/>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
@@ -6157,6 +6175,9 @@
         <f>IF(COUNTIF(D:D,$A287)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D287" s="2" t="s">
+        <v>234</v>
+      </c>
       <c r="F287" s="2"/>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
@@ -6170,6 +6191,9 @@
         <f>IF(COUNTIF(D:D,$A288)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D288" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="F288" s="2"/>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
@@ -6495,9 +6519,6 @@
         <f>IF(COUNTIF(D:D,$A313)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D313" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="F313" s="2"/>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">
@@ -6511,9 +6532,6 @@
         <f>IF(COUNTIF(D:D,$A314)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D314" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F314" s="2"/>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">
@@ -6527,9 +6545,6 @@
         <f>IF(COUNTIF(D:D,$A315)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D315" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="F315" s="2"/>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
@@ -6543,9 +6558,6 @@
         <f>IF(COUNTIF(D:D,$A316)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D316" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="F316" s="2"/>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
@@ -6559,9 +6571,6 @@
         <f>IF(COUNTIF(D:D,$A317)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D317" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="F317" s="2"/>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
@@ -6575,9 +6584,6 @@
         <f>IF(COUNTIF(D:D,$A318)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D318" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F318" s="2"/>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
@@ -6591,9 +6597,6 @@
         <f>IF(COUNTIF(D:D,$A319)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D319" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="F319" s="2"/>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
@@ -6607,9 +6610,6 @@
         <f>IF(COUNTIF(D:D,$A320)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D320" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="F320" s="2"/>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
@@ -6624,7 +6624,7 @@
         <v>Implemented</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>37</v>
+        <v>231</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -6640,7 +6640,7 @@
         <v>Missing</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6656,7 +6656,7 @@
         <v>Missing</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>384</v>
+        <v>65</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6669,10 +6669,10 @@
       </c>
       <c r="C324" t="str">
         <f>IF(COUNTIF(D:D,$A324)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>156</v>
+        <v>66</v>
       </c>
       <c r="F324" s="2"/>
     </row>
@@ -6685,10 +6685,10 @@
       </c>
       <c r="C325" t="str">
         <f>IF(COUNTIF(D:D,$A325)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>215</v>
+        <v>42</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
@@ -6703,7 +6703,7 @@
         <v>Missing</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>254</v>
+        <v>54</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
@@ -6715,10 +6715,10 @@
       </c>
       <c r="C327" t="str">
         <f>IF(COUNTIF(D:D,$A327)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>132</v>
+        <v>57</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -6733,7 +6733,7 @@
         <v>Missing</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>167</v>
+        <v>115</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
@@ -6745,10 +6745,10 @@
       </c>
       <c r="C329" t="str">
         <f>IF(COUNTIF(D:D,$A329)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -6763,7 +6763,7 @@
         <v>Missing</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
@@ -6778,7 +6778,7 @@
         <v>Missing</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>227</v>
+        <v>384</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -6793,7 +6793,7 @@
         <v>Missing</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>85</v>
+        <v>156</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
@@ -6808,7 +6808,7 @@
         <v>Missing</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>123</v>
+        <v>215</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
@@ -6823,7 +6823,7 @@
         <v>Missing</v>
       </c>
       <c r="D334" s="2" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
@@ -6835,10 +6835,10 @@
       </c>
       <c r="C335" t="str">
         <f>IF(COUNTIF(D:D,$A335)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D335" s="2" t="s">
-        <v>368</v>
+        <v>132</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
@@ -6853,10 +6853,10 @@
         <v>Missing</v>
       </c>
       <c r="D336" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>239</v>
       </c>
@@ -6867,8 +6867,11 @@
         <f>IF(COUNTIF(D:D,$A337)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D337" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>240</v>
       </c>
@@ -6879,8 +6882,11 @@
         <f>IF(COUNTIF(D:D,$A338)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D338" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>241</v>
       </c>
@@ -6891,8 +6897,11 @@
         <f>IF(COUNTIF(D:D,$A339)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D339" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>242</v>
       </c>
@@ -6903,8 +6912,11 @@
         <f>IF(COUNTIF(D:D,$A340)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D340" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>243</v>
       </c>
@@ -6915,8 +6927,11 @@
         <f>IF(COUNTIF(D:D,$A341)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D341" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>244</v>
       </c>
@@ -6927,8 +6942,11 @@
         <f>IF(COUNTIF(D:D,$A342)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D342" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>245</v>
       </c>
@@ -6939,8 +6957,11 @@
         <f>IF(COUNTIF(D:D,$A343)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D343" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>247</v>
       </c>
@@ -6951,8 +6972,11 @@
         <f>IF(COUNTIF(D:D,$A344)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D344" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>248</v>
       </c>
@@ -6964,7 +6988,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>249</v>
       </c>
@@ -6976,7 +7000,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>252</v>
       </c>
@@ -6988,7 +7012,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>253</v>
       </c>
@@ -7000,7 +7024,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>255</v>
       </c>
@@ -7009,10 +7033,10 @@
       </c>
       <c r="C349" t="str">
         <f>IF(COUNTIF(D:D,$A349)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
-      </c>
-    </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Implemented</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>256</v>
       </c>
@@ -7024,7 +7048,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>258</v>
       </c>
@@ -7036,7 +7060,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>259</v>
       </c>
@@ -7201,7 +7225,7 @@
       </c>
       <c r="C365" t="str">
         <f>IF(COUNTIF(D:D,$A365)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- implemented the following rare cards: Eaglehorn Bow, Explosive Shot, Ethereal Arcanist, Equality, Felguard
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$261</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$268</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="401">
   <si>
     <t>Cardname</t>
   </si>
@@ -1216,9 +1216,6 @@
     <t>Implemented Cards</t>
   </si>
   <si>
-    <t>ColdlightSeer</t>
-  </si>
-  <si>
     <t>Silverback Patriarch</t>
   </si>
   <si>
@@ -1235,6 +1232,9 @@
   </si>
   <si>
     <t>Siphon Soul</t>
+  </si>
+  <si>
+    <t>Alarm-o-bot</t>
   </si>
 </sst>
 </file>
@@ -1608,7 +1608,7 @@
   <dimension ref="A1:K383"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D324" sqref="D324"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,11 +1789,11 @@
       </c>
       <c r="F8" s="2"/>
       <c r="J8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>259</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1812,11 +1812,11 @@
       </c>
       <c r="F9" s="2"/>
       <c r="J9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2295,7 +2295,7 @@
         <v>Implemented</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>135</v>
+        <v>226</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -2311,7 +2311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>231</v>
+        <v>135</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -2327,7 +2327,7 @@
         <v>Implemented</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>46</v>
+        <v>231</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -2343,7 +2343,7 @@
         <v>Implemented</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -2359,7 +2359,7 @@
         <v>Implemented</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -2375,7 +2375,7 @@
         <v>Implemented</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -2391,7 +2391,7 @@
         <v>Implemented</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>159</v>
+        <v>49</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -2407,7 +2407,7 @@
         <v>Implemented</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -2423,7 +2423,7 @@
         <v>Implemented</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -2439,7 +2439,7 @@
         <v>Implemented</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -2455,7 +2455,7 @@
         <v>Implemented</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>85</v>
+        <v>172</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -2471,7 +2471,7 @@
         <v>Implemented</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -2487,7 +2487,7 @@
         <v>Implemented</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>319</v>
+        <v>96</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -2503,7 +2503,7 @@
         <v>Implemented</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>193</v>
+        <v>319</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -2519,7 +2519,7 @@
         <v>Implemented</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>325</v>
+        <v>193</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -2535,7 +2535,7 @@
         <v>Implemented</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>286</v>
+        <v>325</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -2551,7 +2551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>382</v>
+        <v>286</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -2567,7 +2567,7 @@
         <v>Implemented</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>115</v>
+        <v>382</v>
       </c>
       <c r="F56" s="2"/>
     </row>
@@ -2583,7 +2583,7 @@
         <v>Implemented</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F57" s="2"/>
     </row>
@@ -2599,7 +2599,7 @@
         <v>Implemented</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>3</v>
+        <v>121</v>
       </c>
       <c r="F58" s="2"/>
     </row>
@@ -2615,7 +2615,7 @@
         <v>Implemented</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>122</v>
+        <v>3</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -2631,7 +2631,7 @@
         <v>Implemented</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -2647,7 +2647,7 @@
         <v>Implemented</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>123</v>
+        <v>400</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -2663,7 +2663,7 @@
         <v>Implemented</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>215</v>
+        <v>120</v>
       </c>
       <c r="F62" s="2"/>
     </row>
@@ -2679,7 +2679,7 @@
         <v>Implemented</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>216</v>
+        <v>123</v>
       </c>
       <c r="F63" s="2"/>
     </row>
@@ -2695,7 +2695,7 @@
         <v>Implemented</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F64" s="2"/>
     </row>
@@ -2711,7 +2711,7 @@
         <v>Implemented</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F65" s="2"/>
     </row>
@@ -2727,7 +2727,7 @@
         <v>Implemented</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -2743,7 +2743,7 @@
         <v>Implemented</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -2759,7 +2759,7 @@
         <v>Implemented</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="F68" s="2"/>
     </row>
@@ -2775,7 +2775,7 @@
         <v>Implemented</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -2791,7 +2791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="F70" s="2"/>
     </row>
@@ -2807,7 +2807,7 @@
         <v>Implemented</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F71" s="2"/>
     </row>
@@ -2823,7 +2823,7 @@
         <v>Implemented</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -2839,7 +2839,7 @@
         <v>Implemented</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>24</v>
+        <v>227</v>
       </c>
       <c r="F73" s="2"/>
     </row>
@@ -2855,7 +2855,7 @@
         <v>Implemented</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>25</v>
+        <v>131</v>
       </c>
       <c r="F74" s="2"/>
     </row>
@@ -2871,7 +2871,7 @@
         <v>Implemented</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -2887,7 +2887,7 @@
         <v>Implemented</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F76" s="2"/>
     </row>
@@ -2903,7 +2903,7 @@
         <v>Implemented</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>228</v>
+        <v>26</v>
       </c>
       <c r="F77" s="2"/>
     </row>
@@ -2919,7 +2919,7 @@
         <v>Implemented</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>394</v>
+        <v>28</v>
       </c>
       <c r="F78" s="2"/>
     </row>
@@ -2935,7 +2935,7 @@
         <v>Implemented</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
       <c r="F79" s="2"/>
     </row>
@@ -2951,7 +2951,7 @@
         <v>Implemented</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="F80" s="2"/>
     </row>
@@ -2967,7 +2967,7 @@
         <v>Implemented</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F81" s="2"/>
     </row>
@@ -2983,7 +2983,7 @@
         <v>Implemented</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F82" s="2"/>
     </row>
@@ -2999,7 +2999,7 @@
         <v>Implemented</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F83" s="2"/>
     </row>
@@ -3015,7 +3015,7 @@
         <v>Implemented</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>233</v>
+        <v>138</v>
       </c>
       <c r="F84" s="2"/>
     </row>
@@ -3031,7 +3031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>234</v>
+        <v>35</v>
       </c>
       <c r="F85" s="2"/>
     </row>
@@ -3047,7 +3047,7 @@
         <v>Implemented</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>142</v>
+        <v>233</v>
       </c>
       <c r="F86" s="2"/>
     </row>
@@ -3063,7 +3063,7 @@
         <v>Implemented</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>38</v>
+        <v>234</v>
       </c>
       <c r="F87" s="2"/>
     </row>
@@ -3079,7 +3079,7 @@
         <v>Implemented</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F88" s="2"/>
     </row>
@@ -3095,7 +3095,7 @@
         <v>Implemented</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="F89" s="2"/>
     </row>
@@ -3111,7 +3111,7 @@
         <v>Implemented</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="F90" s="2"/>
     </row>
@@ -3127,7 +3127,7 @@
         <v>Implemented</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>238</v>
+        <v>147</v>
       </c>
       <c r="F91" s="2"/>
     </row>
@@ -3143,7 +3143,7 @@
         <v>Implemented</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="F92" s="2"/>
     </row>
@@ -3159,7 +3159,7 @@
         <v>Implemented</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="F93" s="2"/>
     </row>
@@ -3175,7 +3175,7 @@
         <v>Implemented</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F94" s="2"/>
     </row>
@@ -3191,7 +3191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F95" s="2"/>
     </row>
@@ -3207,7 +3207,7 @@
         <v>Implemented</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>52</v>
+        <v>154</v>
       </c>
       <c r="F96" s="2"/>
     </row>
@@ -3223,7 +3223,7 @@
         <v>Implemented</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>53</v>
+        <v>157</v>
       </c>
       <c r="F97" s="2"/>
     </row>
@@ -3239,7 +3239,7 @@
         <v>Missing</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>246</v>
+        <v>52</v>
       </c>
       <c r="F98" s="2"/>
     </row>
@@ -3255,7 +3255,7 @@
         <v>Missing</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F99" s="2"/>
     </row>
@@ -3271,7 +3271,7 @@
         <v>Missing</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>55</v>
+        <v>246</v>
       </c>
       <c r="F100" s="2"/>
     </row>
@@ -3287,7 +3287,7 @@
         <v>Missing</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F101" s="2"/>
     </row>
@@ -3303,7 +3303,7 @@
         <v>Missing</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F102" s="2"/>
     </row>
@@ -3319,7 +3319,7 @@
         <v>Missing</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>158</v>
+        <v>56</v>
       </c>
       <c r="F103" s="2"/>
     </row>
@@ -3335,7 +3335,7 @@
         <v>Missing</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>250</v>
+        <v>58</v>
       </c>
       <c r="F104" s="2"/>
     </row>
@@ -3351,7 +3351,7 @@
         <v>Missing</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>251</v>
+        <v>158</v>
       </c>
       <c r="F105" s="2"/>
     </row>
@@ -3367,7 +3367,7 @@
         <v>Missing</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>163</v>
+        <v>250</v>
       </c>
       <c r="F106" s="2"/>
     </row>
@@ -3383,7 +3383,7 @@
         <v>Missing</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>73</v>
+        <v>251</v>
       </c>
       <c r="F107" s="2"/>
     </row>
@@ -3399,7 +3399,7 @@
         <v>Missing</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="F108" s="2"/>
     </row>
@@ -3415,7 +3415,7 @@
         <v>Missing</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>164</v>
+        <v>73</v>
       </c>
       <c r="F109" s="2"/>
     </row>
@@ -3431,7 +3431,7 @@
         <v>Missing</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>254</v>
+        <v>74</v>
       </c>
       <c r="F110" s="2"/>
     </row>
@@ -3447,7 +3447,7 @@
         <v>Missing</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="F111" s="2"/>
     </row>
@@ -3463,7 +3463,7 @@
         <v>Missing</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>165</v>
+        <v>254</v>
       </c>
       <c r="F112" s="2"/>
     </row>
@@ -3479,7 +3479,7 @@
         <v>Missing</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>257</v>
+        <v>76</v>
       </c>
       <c r="F113" s="2"/>
     </row>
@@ -3495,7 +3495,7 @@
         <v>Missing</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F114" s="2"/>
     </row>
@@ -3511,7 +3511,7 @@
         <v>Missing</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>79</v>
+        <v>257</v>
       </c>
       <c r="F115" s="2"/>
     </row>
@@ -3527,7 +3527,7 @@
         <v>Missing</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F116" s="2"/>
     </row>
@@ -3543,7 +3543,7 @@
         <v>Missing</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F117" s="2"/>
     </row>
@@ -3559,7 +3559,7 @@
         <v>Missing</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F118" s="2"/>
     </row>
@@ -3575,7 +3575,7 @@
         <v>Missing</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F119" s="2"/>
     </row>
@@ -3591,7 +3591,7 @@
         <v>Missing</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>90</v>
+        <v>173</v>
       </c>
       <c r="F120" s="2"/>
     </row>
@@ -3607,7 +3607,7 @@
         <v>Missing</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F121" s="2"/>
     </row>
@@ -3623,7 +3623,7 @@
         <v>Missing</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F122" s="2"/>
     </row>
@@ -3639,7 +3639,7 @@
         <v>Missing</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F123" s="2"/>
     </row>
@@ -3655,7 +3655,7 @@
         <v>Missing</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F124" s="2"/>
     </row>
@@ -3671,7 +3671,7 @@
         <v>Missing</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>178</v>
+        <v>94</v>
       </c>
       <c r="F125" s="2"/>
     </row>
@@ -3687,7 +3687,7 @@
         <v>Missing</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>272</v>
+        <v>95</v>
       </c>
       <c r="F126" s="2"/>
     </row>
@@ -3703,7 +3703,7 @@
         <v>Missing</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F127" s="2"/>
     </row>
@@ -3719,7 +3719,7 @@
         <v>Missing</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>98</v>
+        <v>272</v>
       </c>
       <c r="F128" s="2"/>
     </row>
@@ -3735,7 +3735,7 @@
         <v>Missing</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="F129" s="2"/>
     </row>
@@ -3751,7 +3751,7 @@
         <v>Missing</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F130" s="2"/>
     </row>
@@ -3767,7 +3767,7 @@
         <v>Implemented</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F131" s="2"/>
     </row>
@@ -3783,7 +3783,7 @@
         <v>Missing</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>183</v>
+        <v>100</v>
       </c>
       <c r="F132" s="2"/>
     </row>
@@ -3799,7 +3799,7 @@
         <v>Missing</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -3815,7 +3815,7 @@
         <v>Implemented</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="F134" s="2"/>
     </row>
@@ -3831,7 +3831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>187</v>
+        <v>106</v>
       </c>
       <c r="F135" s="2"/>
     </row>
@@ -3847,7 +3847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>395</v>
+        <v>110</v>
       </c>
       <c r="F136" s="2"/>
     </row>
@@ -3863,7 +3863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -3879,7 +3879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>190</v>
+        <v>394</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -3895,7 +3895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -3911,7 +3911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -3927,7 +3927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -3943,7 +3943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>367</v>
+        <v>196</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -3959,7 +3959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>368</v>
+        <v>197</v>
       </c>
       <c r="F143" s="2"/>
     </row>
@@ -3975,7 +3975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -3991,7 +3991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>396</v>
+        <v>368</v>
       </c>
       <c r="F145" s="2"/>
     </row>
@@ -4007,7 +4007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>199</v>
+        <v>369</v>
       </c>
       <c r="F146" s="2"/>
     </row>
@@ -4023,7 +4023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>201</v>
+        <v>395</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4039,7 +4039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4055,7 +4055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F149" s="2"/>
     </row>
@@ -4071,7 +4071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>379</v>
+        <v>204</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4086,7 +4086,7 @@
         <v>Implemented</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>380</v>
+        <v>207</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>Implemented</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>208</v>
+        <v>379</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4116,7 +4116,7 @@
         <v>Implemented</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>209</v>
+        <v>380</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4131,7 +4131,7 @@
         <v>Implemented</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>387</v>
+        <v>208</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4146,7 +4146,7 @@
         <v>Implemented</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
         <v>Implemented</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>212</v>
+        <v>387</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4176,7 +4176,7 @@
         <v>Implemented</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>290</v>
+        <v>210</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4206,7 +4206,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>125</v>
+        <v>290</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4251,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>129</v>
+        <v>225</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,7 +4296,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>150</v>
+        <v>21</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,7 +4326,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>60</v>
+        <v>235</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4356,7 +4356,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,7 +4371,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,7 +4386,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>175</v>
+        <v>60</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>181</v>
+        <v>65</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,7 +4431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>182</v>
+        <v>69</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4446,7 +4446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>375</v>
+        <v>78</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>37</v>
+        <v>181</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4491,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>66</v>
+        <v>182</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4506,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>67</v>
+        <v>375</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4521,7 +4521,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>161</v>
+        <v>221</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4536,7 +4536,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,7 +4551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,7 +4566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>92</v>
+        <v>161</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +4611,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>97</v>
+        <v>167</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +4641,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,7 +4656,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>188</v>
+        <v>84</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>202</v>
+        <v>92</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>203</v>
+        <v>97</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +4701,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4716,7 +4716,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4731,7 +4731,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>19</v>
+        <v>188</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4746,7 +4746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>128</v>
+        <v>202</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4761,7 +4761,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>133</v>
+        <v>203</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4776,7 +4776,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,7 +4821,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4836,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>43</v>
+        <v>224</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4851,7 +4851,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4866,7 +4866,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>186</v>
+        <v>134</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,7 +4881,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4896,7 +4896,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4911,7 +4911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>364</v>
+        <v>148</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>377</v>
+        <v>43</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4941,7 +4941,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4971,7 +4971,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>23</v>
+        <v>112</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,7 +4986,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,7 +5001,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>146</v>
+        <v>364</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5016,7 +5016,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>243</v>
+        <v>377</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5031,7 +5031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>48</v>
+        <v>214</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5061,7 +5061,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>155</v>
+        <v>23</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,7 +5076,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,7 +5091,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,7 +5121,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>166</v>
+        <v>45</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,7 +5136,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5166,7 +5166,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>373</v>
+        <v>50</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,7 +5181,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>205</v>
+        <v>64</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>385</v>
+        <v>255</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5211,7 +5211,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>386</v>
+        <v>166</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5226,7 +5226,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,7 +5256,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>141</v>
+        <v>373</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5271,7 +5271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>39</v>
+        <v>385</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5302,7 +5302,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>40</v>
+        <v>386</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5318,7 +5318,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5334,7 +5334,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5350,7 +5350,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5366,7 +5366,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>177</v>
+        <v>236</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5382,7 +5382,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5398,7 +5398,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>185</v>
+        <v>40</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5414,7 +5414,7 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>107</v>
+        <v>153</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5430,7 +5430,7 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5446,7 +5446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>370</v>
+        <v>87</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5462,7 +5462,7 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="F242" s="2"/>
     </row>
@@ -5478,7 +5478,7 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>378</v>
+        <v>103</v>
       </c>
       <c r="F243" s="2"/>
     </row>
@@ -5494,7 +5494,7 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>124</v>
+        <v>185</v>
       </c>
       <c r="F244" s="2"/>
     </row>
@@ -5510,7 +5510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="F245" s="2"/>
     </row>
@@ -5526,7 +5526,7 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>220</v>
+        <v>114</v>
       </c>
       <c r="F246" s="2"/>
     </row>
@@ -5542,7 +5542,7 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>127</v>
+        <v>370</v>
       </c>
       <c r="F247" s="2"/>
     </row>
@@ -5558,7 +5558,7 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>27</v>
+        <v>200</v>
       </c>
       <c r="F248" s="2"/>
     </row>
@@ -5574,7 +5574,7 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>30</v>
+        <v>378</v>
       </c>
       <c r="F249" s="2"/>
     </row>
@@ -5590,7 +5590,7 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5606,7 +5606,7 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5622,7 +5622,7 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>44</v>
+        <v>220</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5638,7 +5638,7 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>336</v>
+        <v>127</v>
       </c>
       <c r="F253" s="2"/>
     </row>
@@ -5654,7 +5654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="F254" s="2"/>
     </row>
@@ -5670,7 +5670,7 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="F255" s="2"/>
     </row>
@@ -5686,7 +5686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>77</v>
+        <v>230</v>
       </c>
       <c r="F256" s="2"/>
     </row>
@@ -5702,7 +5702,7 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>180</v>
+        <v>136</v>
       </c>
       <c r="F257" s="2"/>
     </row>
@@ -5718,7 +5718,7 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="F258" s="2"/>
     </row>
@@ -5734,7 +5734,7 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>191</v>
+        <v>44</v>
       </c>
       <c r="F259" s="2"/>
     </row>
@@ -5750,7 +5750,7 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>381</v>
+        <v>336</v>
       </c>
       <c r="F260" s="2"/>
     </row>
@@ -5766,7 +5766,7 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>383</v>
+        <v>63</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -5782,7 +5782,7 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -5798,7 +5798,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5814,13 +5814,13 @@
         <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
       <c r="F264" s="2"/>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B265" t="s">
         <v>8</v>
@@ -5830,13 +5830,13 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>246</v>
+        <v>111</v>
       </c>
       <c r="F265" s="2"/>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B266" t="s">
         <v>8</v>
@@ -5846,7 +5846,7 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -5862,7 +5862,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5878,7 +5878,7 @@
         <v>Missing</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>114</v>
+        <v>383</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5894,7 +5894,7 @@
         <v>Missing</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -5910,7 +5910,7 @@
         <v>Missing</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -5926,7 +5926,7 @@
         <v>Missing</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -5942,7 +5942,7 @@
         <v>Missing</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -5958,7 +5958,7 @@
         <v>Missing</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>154</v>
+        <v>198</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -5974,7 +5974,7 @@
         <v>Missing</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>173</v>
+        <v>396</v>
       </c>
       <c r="F274" s="2"/>
     </row>
@@ -5990,7 +5990,7 @@
         <v>Missing</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="F275" s="2"/>
     </row>
@@ -6006,7 +6006,7 @@
         <v>Missing</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>161</v>
+        <v>44</v>
       </c>
       <c r="F276" s="2"/>
     </row>
@@ -6022,7 +6022,7 @@
         <v>Missing</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>203</v>
+        <v>63</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -6038,7 +6038,7 @@
         <v>Missing</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -6054,7 +6054,7 @@
         <v>Missing</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>134</v>
+        <v>228</v>
       </c>
       <c r="F279" s="2"/>
     </row>
@@ -6070,7 +6070,7 @@
         <v>Missing</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="F280" s="2"/>
     </row>
@@ -6086,7 +6086,7 @@
         <v>Missing</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
       <c r="F281" s="2"/>
     </row>
@@ -6102,7 +6102,7 @@
         <v>Missing</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="F282" s="2"/>
     </row>
@@ -6117,6 +6117,9 @@
         <f>IF(COUNTIF(D:D,$A283)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D283" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="F283" s="2"/>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
@@ -6130,6 +6133,9 @@
         <f>IF(COUNTIF(D:D,$A284)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D284" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="F284" s="2"/>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
@@ -6144,7 +6150,7 @@
         <v>Missing</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="F285" s="2"/>
     </row>
@@ -6160,7 +6166,7 @@
         <v>Missing</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="F286" s="2"/>
     </row>
@@ -6176,7 +6182,7 @@
         <v>Missing</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>234</v>
+        <v>130</v>
       </c>
       <c r="F287" s="2"/>
     </row>
@@ -6192,7 +6198,7 @@
         <v>Missing</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="F288" s="2"/>
     </row>
@@ -6207,6 +6213,9 @@
         <f>IF(COUNTIF(D:D,$A289)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D289" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="F289" s="2"/>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
@@ -6246,6 +6255,9 @@
         <f>IF(COUNTIF(D:D,$A292)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D292" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="F292" s="2"/>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
@@ -6259,6 +6271,9 @@
         <f>IF(COUNTIF(D:D,$A293)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D293" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="F293" s="2"/>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
@@ -6272,6 +6287,9 @@
         <f>IF(COUNTIF(D:D,$A294)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D294" s="2" t="s">
+        <v>234</v>
+      </c>
       <c r="F294" s="2"/>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
@@ -6285,6 +6303,9 @@
         <f>IF(COUNTIF(D:D,$A295)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D295" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="F295" s="2"/>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
@@ -6623,9 +6644,6 @@
         <f>IF(COUNTIF(D:D,$A321)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D321" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="F321" s="2"/>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
@@ -6637,10 +6655,7 @@
       </c>
       <c r="C322" t="str">
         <f>IF(COUNTIF(D:D,$A322)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
-      </c>
-      <c r="D322" s="2" t="s">
-        <v>31</v>
+        <v>Implemented</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6653,10 +6668,7 @@
       </c>
       <c r="C323" t="str">
         <f>IF(COUNTIF(D:D,$A323)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
-      </c>
-      <c r="D323" s="2" t="s">
-        <v>65</v>
+        <v>Implemented</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6671,9 +6683,6 @@
         <f>IF(COUNTIF(D:D,$A324)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D324" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="F324" s="2"/>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
@@ -6687,9 +6696,6 @@
         <f>IF(COUNTIF(D:D,$A325)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D325" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
@@ -6700,10 +6706,7 @@
       </c>
       <c r="C326" t="str">
         <f>IF(COUNTIF(D:D,$A326)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
-      </c>
-      <c r="D326" s="2" t="s">
-        <v>54</v>
+        <v>Implemented</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
@@ -6717,9 +6720,6 @@
         <f>IF(COUNTIF(D:D,$A327)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D327" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
@@ -6730,10 +6730,10 @@
       </c>
       <c r="C328" t="str">
         <f>IF(COUNTIF(D:D,$A328)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>115</v>
+        <v>231</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
@@ -6748,7 +6748,7 @@
         <v>Implemented</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -6760,10 +6760,10 @@
       </c>
       <c r="C330" t="str">
         <f>IF(COUNTIF(D:D,$A330)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>144</v>
+        <v>65</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
@@ -6775,10 +6775,10 @@
       </c>
       <c r="C331" t="str">
         <f>IF(COUNTIF(D:D,$A331)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>384</v>
+        <v>66</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -6790,10 +6790,10 @@
       </c>
       <c r="C332" t="str">
         <f>IF(COUNTIF(D:D,$A332)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>156</v>
+        <v>42</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
@@ -6808,7 +6808,7 @@
         <v>Missing</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>215</v>
+        <v>54</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
@@ -6820,10 +6820,10 @@
       </c>
       <c r="C334" t="str">
         <f>IF(COUNTIF(D:D,$A334)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D334" s="2" t="s">
-        <v>254</v>
+        <v>57</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
@@ -6838,7 +6838,7 @@
         <v>Implemented</v>
       </c>
       <c r="D335" s="2" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
@@ -6853,7 +6853,7 @@
         <v>Missing</v>
       </c>
       <c r="D336" s="2" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -6868,7 +6868,7 @@
         <v>Missing</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -6883,7 +6883,7 @@
         <v>Missing</v>
       </c>
       <c r="D338" s="2" t="s">
-        <v>155</v>
+        <v>384</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -6898,7 +6898,7 @@
         <v>Missing</v>
       </c>
       <c r="D339" s="2" t="s">
-        <v>227</v>
+        <v>156</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -6913,7 +6913,7 @@
         <v>Missing</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>85</v>
+        <v>215</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -6928,7 +6928,7 @@
         <v>Implemented</v>
       </c>
       <c r="D341" s="2" t="s">
-        <v>123</v>
+        <v>254</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -6943,7 +6943,7 @@
         <v>Missing</v>
       </c>
       <c r="D342" s="2" t="s">
-        <v>238</v>
+        <v>132</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -6958,7 +6958,7 @@
         <v>Missing</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>368</v>
+        <v>167</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -6973,7 +6973,7 @@
         <v>Missing</v>
       </c>
       <c r="D344" s="2" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -6987,6 +6987,9 @@
         <f>IF(COUNTIF(D:D,$A345)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D345" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
@@ -6999,6 +7002,9 @@
         <f>IF(COUNTIF(D:D,$A346)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D346" s="2" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
@@ -7011,6 +7017,9 @@
         <f>IF(COUNTIF(D:D,$A347)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D347" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
@@ -7023,6 +7032,9 @@
         <f>IF(COUNTIF(D:D,$A348)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D348" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
@@ -7035,6 +7047,9 @@
         <f>IF(COUNTIF(D:D,$A349)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D349" s="2" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
@@ -7047,6 +7062,9 @@
         <f>IF(COUNTIF(D:D,$A350)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D350" s="2" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
@@ -7059,6 +7077,9 @@
         <f>IF(COUNTIF(D:D,$A351)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D351" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
@@ -7314,7 +7335,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B373" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
- implemented the following rare cards: Flare, Holy Wrath, Holy Fire, Headcrack, Frothing Berserker
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$268</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$278</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="401">
   <si>
     <t>Cardname</t>
   </si>
@@ -754,9 +754,6 @@
     <t>Equality</t>
   </si>
   <si>
-    <t>Etheral Arcanist</t>
-  </si>
-  <si>
     <t>Explosive Shot</t>
   </si>
   <si>
@@ -1235,6 +1232,9 @@
   </si>
   <si>
     <t>Alarm-o-bot</t>
+  </si>
+  <si>
+    <t>Ethereal Arcanist</t>
   </si>
 </sst>
 </file>
@@ -1607,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K383"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,11 +1631,11 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F1" s="1"/>
       <c r="J1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K1">
         <f>COUNTIF(B:B,"Free")</f>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="F2" s="2"/>
       <c r="J2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K2">
         <f>COUNTIF(B:B,"Common")</f>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="J3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K3">
         <f>COUNTIF(B:B,"Rare")</f>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="F4" s="2"/>
       <c r="J4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K4">
         <f>COUNTIF(B:B,"Epic")</f>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="J5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K5">
         <f>COUNTIF(B:B,"Legendary")</f>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="F6" s="2"/>
       <c r="J6" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K6" s="1">
         <f>SUM(K1:K5)</f>
@@ -1789,11 +1789,11 @@
       </c>
       <c r="F8" s="2"/>
       <c r="J8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1812,11 +1812,11 @@
       </c>
       <c r="F9" s="2"/>
       <c r="J9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1927,7 +1927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -1943,7 +1943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -2023,7 +2023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -2039,7 +2039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>156</v>
+        <v>240</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -2055,7 +2055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -2071,7 +2071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>70</v>
+        <v>243</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -2087,7 +2087,7 @@
         <v>Implemented</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>75</v>
+        <v>156</v>
       </c>
       <c r="F26" s="2"/>
     </row>
@@ -2103,7 +2103,7 @@
         <v>Implemented</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -2119,7 +2119,7 @@
         <v>Implemented</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>184</v>
+        <v>70</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -2135,7 +2135,7 @@
         <v>Implemented</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>323</v>
+        <v>75</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -2151,7 +2151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>192</v>
+        <v>88</v>
       </c>
       <c r="F30" s="2"/>
     </row>
@@ -2167,7 +2167,7 @@
         <v>Implemented</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>366</v>
+        <v>184</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -2183,7 +2183,7 @@
         <v>Implemented</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -2199,7 +2199,7 @@
         <v>Implemented</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>374</v>
+        <v>192</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -2215,7 +2215,7 @@
         <v>Implemented</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="F34" s="2"/>
     </row>
@@ -2231,7 +2231,7 @@
         <v>Implemented</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>206</v>
+        <v>371</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -2247,7 +2247,7 @@
         <v>Implemented</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>11</v>
+        <v>373</v>
       </c>
       <c r="F36" s="2"/>
     </row>
@@ -2263,7 +2263,7 @@
         <v>Implemented</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>12</v>
+        <v>375</v>
       </c>
       <c r="F37" s="2"/>
     </row>
@@ -2279,7 +2279,7 @@
         <v>Implemented</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>13</v>
+        <v>206</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -2295,7 +2295,7 @@
         <v>Implemented</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>226</v>
+        <v>11</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -2311,7 +2311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -2327,7 +2327,7 @@
         <v>Implemented</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>231</v>
+        <v>13</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -2343,7 +2343,7 @@
         <v>Implemented</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>46</v>
+        <v>226</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -2359,7 +2359,7 @@
         <v>Implemented</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>47</v>
+        <v>135</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -2375,7 +2375,7 @@
         <v>Implemented</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>51</v>
+        <v>231</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -2391,7 +2391,7 @@
         <v>Implemented</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>49</v>
+        <v>400</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -2407,7 +2407,7 @@
         <v>Implemented</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>159</v>
+        <v>46</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -2423,7 +2423,7 @@
         <v>Implemented</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>160</v>
+        <v>47</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -2439,7 +2439,7 @@
         <v>Implemented</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>170</v>
+        <v>51</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -2455,7 +2455,7 @@
         <v>Implemented</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>172</v>
+        <v>49</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -2471,7 +2471,7 @@
         <v>Implemented</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -2487,7 +2487,7 @@
         <v>Implemented</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -2503,7 +2503,7 @@
         <v>Implemented</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>319</v>
+        <v>170</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -2519,7 +2519,7 @@
         <v>Implemented</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -2535,7 +2535,7 @@
         <v>Implemented</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>325</v>
+        <v>85</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -2551,7 +2551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>286</v>
+        <v>96</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -2567,7 +2567,7 @@
         <v>Implemented</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>382</v>
+        <v>318</v>
       </c>
       <c r="F56" s="2"/>
     </row>
@@ -2583,7 +2583,7 @@
         <v>Implemented</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>115</v>
+        <v>193</v>
       </c>
       <c r="F57" s="2"/>
     </row>
@@ -2599,7 +2599,7 @@
         <v>Implemented</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>121</v>
+        <v>324</v>
       </c>
       <c r="F58" s="2"/>
     </row>
@@ -2615,7 +2615,7 @@
         <v>Implemented</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>3</v>
+        <v>285</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -2631,7 +2631,7 @@
         <v>Implemented</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>122</v>
+        <v>381</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -2647,7 +2647,7 @@
         <v>Implemented</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>400</v>
+        <v>115</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -2663,7 +2663,7 @@
         <v>Implemented</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F62" s="2"/>
     </row>
@@ -2679,7 +2679,7 @@
         <v>Implemented</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="F63" s="2"/>
     </row>
@@ -2695,7 +2695,7 @@
         <v>Implemented</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>215</v>
+        <v>122</v>
       </c>
       <c r="F64" s="2"/>
     </row>
@@ -2711,7 +2711,7 @@
         <v>Implemented</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>216</v>
+        <v>399</v>
       </c>
       <c r="F65" s="2"/>
     </row>
@@ -2727,7 +2727,7 @@
         <v>Implemented</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>217</v>
+        <v>120</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -2743,7 +2743,7 @@
         <v>Implemented</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -2759,7 +2759,7 @@
         <v>Implemented</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="F68" s="2"/>
     </row>
@@ -2775,7 +2775,7 @@
         <v>Implemented</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -2791,7 +2791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>126</v>
+        <v>217</v>
       </c>
       <c r="F70" s="2"/>
     </row>
@@ -2807,7 +2807,7 @@
         <v>Implemented</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F71" s="2"/>
     </row>
@@ -2823,7 +2823,7 @@
         <v>Implemented</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -2839,7 +2839,7 @@
         <v>Implemented</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F73" s="2"/>
     </row>
@@ -2855,7 +2855,7 @@
         <v>Implemented</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F74" s="2"/>
     </row>
@@ -2871,7 +2871,7 @@
         <v>Implemented</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>24</v>
+        <v>222</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -2887,7 +2887,7 @@
         <v>Implemented</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F76" s="2"/>
     </row>
@@ -2903,7 +2903,7 @@
         <v>Implemented</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>26</v>
+        <v>227</v>
       </c>
       <c r="F77" s="2"/>
     </row>
@@ -2919,7 +2919,7 @@
         <v>Implemented</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
       <c r="F78" s="2"/>
     </row>
@@ -2935,7 +2935,7 @@
         <v>Implemented</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>228</v>
+        <v>24</v>
       </c>
       <c r="F79" s="2"/>
     </row>
@@ -2951,7 +2951,7 @@
         <v>Implemented</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>229</v>
+        <v>25</v>
       </c>
       <c r="F80" s="2"/>
     </row>
@@ -2967,7 +2967,7 @@
         <v>Implemented</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F81" s="2"/>
     </row>
@@ -2983,7 +2983,7 @@
         <v>Implemented</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
       <c r="F82" s="2"/>
     </row>
@@ -2999,7 +2999,7 @@
         <v>Implemented</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>34</v>
+        <v>228</v>
       </c>
       <c r="F83" s="2"/>
     </row>
@@ -3015,7 +3015,7 @@
         <v>Implemented</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>138</v>
+        <v>229</v>
       </c>
       <c r="F84" s="2"/>
     </row>
@@ -3031,7 +3031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F85" s="2"/>
     </row>
@@ -3047,7 +3047,7 @@
         <v>Implemented</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>233</v>
+        <v>137</v>
       </c>
       <c r="F86" s="2"/>
     </row>
@@ -3063,7 +3063,7 @@
         <v>Implemented</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>234</v>
+        <v>34</v>
       </c>
       <c r="F87" s="2"/>
     </row>
@@ -3079,7 +3079,7 @@
         <v>Implemented</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F88" s="2"/>
     </row>
@@ -3095,7 +3095,7 @@
         <v>Implemented</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F89" s="2"/>
     </row>
@@ -3111,7 +3111,7 @@
         <v>Implemented</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>143</v>
+        <v>233</v>
       </c>
       <c r="F90" s="2"/>
     </row>
@@ -3127,7 +3127,7 @@
         <v>Implemented</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>147</v>
+        <v>234</v>
       </c>
       <c r="F91" s="2"/>
     </row>
@@ -3143,7 +3143,7 @@
         <v>Implemented</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="F92" s="2"/>
     </row>
@@ -3159,7 +3159,7 @@
         <v>Implemented</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>238</v>
+        <v>38</v>
       </c>
       <c r="F93" s="2"/>
     </row>
@@ -3175,7 +3175,7 @@
         <v>Implemented</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F94" s="2"/>
     </row>
@@ -3191,13 +3191,13 @@
         <v>Implemented</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
@@ -3207,13 +3207,13 @@
         <v>Implemented</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>154</v>
+        <v>41</v>
       </c>
       <c r="F96" s="2"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B97" t="s">
         <v>6</v>
@@ -3223,13 +3223,13 @@
         <v>Implemented</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>157</v>
+        <v>238</v>
       </c>
       <c r="F97" s="2"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B98" t="s">
         <v>6</v>
@@ -3239,13 +3239,13 @@
         <v>Missing</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>52</v>
+        <v>151</v>
       </c>
       <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B99" t="s">
         <v>6</v>
@@ -3255,13 +3255,13 @@
         <v>Missing</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>53</v>
+        <v>152</v>
       </c>
       <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B100" t="s">
         <v>6</v>
@@ -3271,13 +3271,13 @@
         <v>Missing</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>246</v>
+        <v>154</v>
       </c>
       <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B101" t="s">
         <v>6</v>
@@ -3287,13 +3287,13 @@
         <v>Missing</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
@@ -3303,13 +3303,13 @@
         <v>Missing</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B103" t="s">
         <v>6</v>
@@ -3319,13 +3319,13 @@
         <v>Missing</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B104" t="s">
         <v>6</v>
@@ -3335,13 +3335,13 @@
         <v>Missing</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>58</v>
+        <v>245</v>
       </c>
       <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
@@ -3351,13 +3351,13 @@
         <v>Missing</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
       <c r="F105" s="2"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B106" t="s">
         <v>6</v>
@@ -3367,13 +3367,13 @@
         <v>Missing</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>250</v>
+        <v>55</v>
       </c>
       <c r="F106" s="2"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B107" t="s">
         <v>6</v>
@@ -3383,13 +3383,13 @@
         <v>Missing</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>251</v>
+        <v>56</v>
       </c>
       <c r="F107" s="2"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B108" t="s">
         <v>6</v>
@@ -3399,13 +3399,13 @@
         <v>Missing</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>163</v>
+        <v>58</v>
       </c>
       <c r="F108" s="2"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B109" t="s">
         <v>6</v>
@@ -3415,13 +3415,13 @@
         <v>Missing</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="F109" s="2"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B110" t="s">
         <v>6</v>
@@ -3431,13 +3431,13 @@
         <v>Missing</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>74</v>
+        <v>249</v>
       </c>
       <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
@@ -3447,13 +3447,13 @@
         <v>Missing</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>164</v>
+        <v>250</v>
       </c>
       <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
@@ -3463,13 +3463,13 @@
         <v>Missing</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>254</v>
+        <v>163</v>
       </c>
       <c r="F112" s="2"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
@@ -3479,13 +3479,13 @@
         <v>Missing</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F113" s="2"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B114" t="s">
         <v>6</v>
@@ -3495,13 +3495,13 @@
         <v>Missing</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
       <c r="F114" s="2"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B115" t="s">
         <v>6</v>
@@ -3511,13 +3511,13 @@
         <v>Missing</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>257</v>
+        <v>164</v>
       </c>
       <c r="F115" s="2"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B116" t="s">
         <v>6</v>
@@ -3527,13 +3527,13 @@
         <v>Missing</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>168</v>
+        <v>253</v>
       </c>
       <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B117" t="s">
         <v>6</v>
@@ -3543,13 +3543,13 @@
         <v>Missing</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F117" s="2"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
@@ -3559,13 +3559,13 @@
         <v>Missing</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F118" s="2"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
@@ -3575,13 +3575,13 @@
         <v>Missing</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>80</v>
+        <v>256</v>
       </c>
       <c r="F119" s="2"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
@@ -3591,13 +3591,13 @@
         <v>Missing</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F120" s="2"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
@@ -3607,13 +3607,13 @@
         <v>Missing</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="F121" s="2"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
@@ -3623,13 +3623,13 @@
         <v>Missing</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>90</v>
+        <v>169</v>
       </c>
       <c r="F122" s="2"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B123" t="s">
         <v>6</v>
@@ -3639,13 +3639,13 @@
         <v>Missing</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F123" s="2"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B124" t="s">
         <v>6</v>
@@ -3655,13 +3655,13 @@
         <v>Missing</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="F124" s="2"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
@@ -3671,13 +3671,13 @@
         <v>Missing</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F125" s="2"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
@@ -3687,13 +3687,13 @@
         <v>Missing</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F126" s="2"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
@@ -3703,13 +3703,13 @@
         <v>Missing</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>178</v>
+        <v>91</v>
       </c>
       <c r="F127" s="2"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
@@ -3719,13 +3719,13 @@
         <v>Missing</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>272</v>
+        <v>93</v>
       </c>
       <c r="F128" s="2"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B129" t="s">
         <v>6</v>
@@ -3735,13 +3735,13 @@
         <v>Missing</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>179</v>
+        <v>94</v>
       </c>
       <c r="F129" s="2"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
@@ -3751,13 +3751,13 @@
         <v>Missing</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F130" s="2"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B131" t="s">
         <v>6</v>
@@ -3767,13 +3767,13 @@
         <v>Implemented</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>99</v>
+        <v>178</v>
       </c>
       <c r="F131" s="2"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B132" t="s">
         <v>6</v>
@@ -3783,13 +3783,13 @@
         <v>Missing</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>100</v>
+        <v>271</v>
       </c>
       <c r="F132" s="2"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B133" t="s">
         <v>6</v>
@@ -3799,7 +3799,7 @@
         <v>Missing</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -3815,7 +3815,7 @@
         <v>Implemented</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>183</v>
+        <v>98</v>
       </c>
       <c r="F134" s="2"/>
     </row>
@@ -3831,7 +3831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F135" s="2"/>
     </row>
@@ -3847,7 +3847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F136" s="2"/>
     </row>
@@ -3863,7 +3863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>187</v>
+        <v>101</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -3879,7 +3879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>394</v>
+        <v>183</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -3895,7 +3895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>189</v>
+        <v>106</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -3911,7 +3911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>190</v>
+        <v>110</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -3927,7 +3927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -3943,7 +3943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>196</v>
+        <v>393</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -3959,7 +3959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F143" s="2"/>
     </row>
@@ -3975,7 +3975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>367</v>
+        <v>190</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -3991,7 +3991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>368</v>
+        <v>195</v>
       </c>
       <c r="F145" s="2"/>
     </row>
@@ -4007,7 +4007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>369</v>
+        <v>196</v>
       </c>
       <c r="F146" s="2"/>
     </row>
@@ -4023,7 +4023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>395</v>
+        <v>197</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4039,7 +4039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>199</v>
+        <v>366</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4055,7 +4055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>201</v>
+        <v>367</v>
       </c>
       <c r="F149" s="2"/>
     </row>
@@ -4071,7 +4071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>204</v>
+        <v>368</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4086,7 +4086,7 @@
         <v>Implemented</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>207</v>
+        <v>394</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>Implemented</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>379</v>
+        <v>199</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4116,7 +4116,7 @@
         <v>Implemented</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>380</v>
+        <v>201</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4131,7 +4131,7 @@
         <v>Implemented</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4146,7 +4146,7 @@
         <v>Implemented</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
         <v>Implemented</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4176,7 +4176,7 @@
         <v>Implemented</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>210</v>
+        <v>379</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4206,7 +4206,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>290</v>
+        <v>209</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>213</v>
+        <v>386</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4251,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>225</v>
+        <v>289</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>20</v>
+        <v>213</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,7 +4296,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,7 +4326,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>31</v>
+        <v>225</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>235</v>
+        <v>20</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4356,7 +4356,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>150</v>
+        <v>21</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,7 +4371,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,7 +4386,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>60</v>
+        <v>235</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>65</v>
+        <v>239</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,7 +4431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4446,7 +4446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4491,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4506,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>375</v>
+        <v>248</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4521,7 +4521,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>221</v>
+        <v>69</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4536,7 +4536,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>132</v>
+        <v>78</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,7 +4551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,7 +4566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>66</v>
+        <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>67</v>
+        <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>161</v>
+        <v>374</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +4611,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>167</v>
+        <v>221</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +4641,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,7 +4656,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>84</v>
+        <v>247</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +4701,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>108</v>
+        <v>161</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4716,7 +4716,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4731,7 +4731,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>188</v>
+        <v>82</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4746,7 +4746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>202</v>
+        <v>83</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4761,7 +4761,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>203</v>
+        <v>84</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4776,7 +4776,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,7 +4821,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4836,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4851,7 +4851,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>133</v>
+        <v>202</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4866,7 +4866,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>134</v>
+        <v>203</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,7 +4881,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4896,7 +4896,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4911,7 +4911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>148</v>
+        <v>19</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4941,7 +4941,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>104</v>
+        <v>224</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>186</v>
+        <v>133</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4971,7 +4971,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,7 +4986,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>113</v>
+        <v>36</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,7 +5001,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>364</v>
+        <v>140</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5016,7 +5016,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>377</v>
+        <v>148</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5031,7 +5031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5061,7 +5061,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,7 +5076,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,7 +5091,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>243</v>
+        <v>113</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,7 +5121,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>45</v>
+        <v>363</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,7 +5136,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>48</v>
+        <v>376</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>155</v>
+        <v>9</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5166,7 +5166,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>50</v>
+        <v>214</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,7 +5181,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>255</v>
+        <v>145</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5211,7 +5211,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5226,7 +5226,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>102</v>
+        <v>242</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>198</v>
+        <v>45</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,7 +5256,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>373</v>
+        <v>48</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5271,7 +5271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>385</v>
+        <v>50</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5302,7 +5302,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>386</v>
+        <v>64</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5318,7 +5318,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>130</v>
+        <v>254</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5334,7 +5334,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5350,7 +5350,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>141</v>
+        <v>102</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5366,7 +5366,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5382,7 +5382,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>39</v>
+        <v>372</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5398,7 +5398,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>40</v>
+        <v>205</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5414,13 +5414,13 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>153</v>
+        <v>384</v>
       </c>
       <c r="F239" s="2"/>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B240" t="s">
         <v>8</v>
@@ -5430,13 +5430,13 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>62</v>
+        <v>385</v>
       </c>
       <c r="F240" s="2"/>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B241" t="s">
         <v>8</v>
@@ -5446,13 +5446,13 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="F241" s="2"/>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B242" t="s">
         <v>8</v>
@@ -5462,13 +5462,13 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>177</v>
+        <v>33</v>
       </c>
       <c r="F242" s="2"/>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B243" t="s">
         <v>8</v>
@@ -5478,13 +5478,13 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="F243" s="2"/>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B244" t="s">
         <v>8</v>
@@ -5494,13 +5494,13 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>185</v>
+        <v>236</v>
       </c>
       <c r="F244" s="2"/>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B245" t="s">
         <v>8</v>
@@ -5510,13 +5510,13 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="F245" s="2"/>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B246" t="s">
         <v>8</v>
@@ -5526,13 +5526,13 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="F246" s="2"/>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B247" t="s">
         <v>8</v>
@@ -5542,13 +5542,13 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>370</v>
+        <v>241</v>
       </c>
       <c r="F247" s="2"/>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B248" t="s">
         <v>8</v>
@@ -5558,13 +5558,13 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>200</v>
+        <v>153</v>
       </c>
       <c r="F248" s="2"/>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B249" t="s">
         <v>8</v>
@@ -5574,13 +5574,13 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>378</v>
+        <v>62</v>
       </c>
       <c r="F249" s="2"/>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B250" t="s">
         <v>8</v>
@@ -5590,13 +5590,13 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="F250" s="2"/>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B251" t="s">
         <v>8</v>
@@ -5606,13 +5606,13 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>15</v>
+        <v>177</v>
       </c>
       <c r="F251" s="2"/>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B252" t="s">
         <v>8</v>
@@ -5622,13 +5622,13 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>220</v>
+        <v>103</v>
       </c>
       <c r="F252" s="2"/>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B253" t="s">
         <v>8</v>
@@ -5638,13 +5638,13 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="F253" s="2"/>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B254" t="s">
         <v>8</v>
@@ -5654,13 +5654,13 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="F254" s="2"/>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B255" t="s">
         <v>8</v>
@@ -5670,13 +5670,13 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="F255" s="2"/>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B256" t="s">
         <v>8</v>
@@ -5686,13 +5686,13 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>230</v>
+        <v>369</v>
       </c>
       <c r="F256" s="2"/>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B257" t="s">
         <v>8</v>
@@ -5702,13 +5702,13 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>136</v>
+        <v>200</v>
       </c>
       <c r="F257" s="2"/>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B258" t="s">
         <v>8</v>
@@ -5718,13 +5718,13 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>42</v>
+        <v>377</v>
       </c>
       <c r="F258" s="2"/>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B259" t="s">
         <v>8</v>
@@ -5734,13 +5734,13 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="F259" s="2"/>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B260" t="s">
         <v>8</v>
@@ -5750,13 +5750,13 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>336</v>
+        <v>15</v>
       </c>
       <c r="F260" s="2"/>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B261" t="s">
         <v>8</v>
@@ -5766,13 +5766,13 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
       <c r="F261" s="2"/>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B262" t="s">
         <v>8</v>
@@ -5782,13 +5782,13 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="F262" s="2"/>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B263" t="s">
         <v>8</v>
@@ -5798,7 +5798,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5814,13 +5814,13 @@
         <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>180</v>
+        <v>30</v>
       </c>
       <c r="F264" s="2"/>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B265" t="s">
         <v>8</v>
@@ -5830,13 +5830,13 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>111</v>
+        <v>230</v>
       </c>
       <c r="F265" s="2"/>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B266" t="s">
         <v>8</v>
@@ -5846,13 +5846,13 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>191</v>
+        <v>136</v>
       </c>
       <c r="F266" s="2"/>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B267" t="s">
         <v>7</v>
@@ -5862,7 +5862,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>381</v>
+        <v>42</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5878,7 +5878,7 @@
         <v>Missing</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>383</v>
+        <v>44</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5894,13 +5894,13 @@
         <v>Missing</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>32</v>
+        <v>244</v>
       </c>
       <c r="F269" s="2"/>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B270" t="s">
         <v>7</v>
@@ -5910,13 +5910,13 @@
         <v>Missing</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>137</v>
+        <v>335</v>
       </c>
       <c r="F270" s="2"/>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B271" t="s">
         <v>7</v>
@@ -5926,13 +5926,13 @@
         <v>Missing</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>151</v>
+        <v>63</v>
       </c>
       <c r="F271" s="2"/>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B272" t="s">
         <v>7</v>
@@ -5942,13 +5942,13 @@
         <v>Missing</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>246</v>
+        <v>162</v>
       </c>
       <c r="F272" s="2"/>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B273" t="s">
         <v>7</v>
@@ -5958,13 +5958,13 @@
         <v>Missing</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>198</v>
+        <v>77</v>
       </c>
       <c r="F273" s="2"/>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B274" t="s">
         <v>7</v>
@@ -5974,13 +5974,13 @@
         <v>Missing</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>396</v>
+        <v>180</v>
       </c>
       <c r="F274" s="2"/>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B275" t="s">
         <v>7</v>
@@ -5990,13 +5990,13 @@
         <v>Missing</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F275" s="2"/>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B276" t="s">
         <v>7</v>
@@ -6006,13 +6006,13 @@
         <v>Missing</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>44</v>
+        <v>191</v>
       </c>
       <c r="F276" s="2"/>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B277" t="s">
         <v>7</v>
@@ -6022,13 +6022,13 @@
         <v>Missing</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>63</v>
+        <v>380</v>
       </c>
       <c r="F277" s="2"/>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B278" t="s">
         <v>7</v>
@@ -6038,13 +6038,13 @@
         <v>Missing</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>122</v>
+        <v>382</v>
       </c>
       <c r="F278" s="2"/>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B279" t="s">
         <v>7</v>
@@ -6054,13 +6054,13 @@
         <v>Missing</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>228</v>
+        <v>32</v>
       </c>
       <c r="F279" s="2"/>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B280" t="s">
         <v>7</v>
@@ -6070,13 +6070,13 @@
         <v>Missing</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="F280" s="2"/>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B281" t="s">
         <v>7</v>
@@ -6086,13 +6086,13 @@
         <v>Missing</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="F281" s="2"/>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B282" t="s">
         <v>7</v>
@@ -6102,13 +6102,13 @@
         <v>Missing</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>150</v>
+        <v>245</v>
       </c>
       <c r="F282" s="2"/>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B283" t="s">
         <v>7</v>
@@ -6118,13 +6118,13 @@
         <v>Missing</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
       <c r="F283" s="2"/>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B284" t="s">
         <v>7</v>
@@ -6134,13 +6134,13 @@
         <v>Missing</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>203</v>
+        <v>395</v>
       </c>
       <c r="F284" s="2"/>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B285" t="s">
         <v>7</v>
@@ -6150,13 +6150,13 @@
         <v>Missing</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="F285" s="2"/>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B286" t="s">
         <v>7</v>
@@ -6166,13 +6166,13 @@
         <v>Missing</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="F286" s="2"/>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B287" t="s">
         <v>7</v>
@@ -6182,13 +6182,13 @@
         <v>Missing</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
       <c r="F287" s="2"/>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B288" t="s">
         <v>7</v>
@@ -6198,13 +6198,13 @@
         <v>Missing</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F288" s="2"/>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B289" t="s">
         <v>7</v>
@@ -6214,13 +6214,13 @@
         <v>Missing</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>92</v>
+        <v>228</v>
       </c>
       <c r="F289" s="2"/>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B290" t="s">
         <v>7</v>
@@ -6229,11 +6229,14 @@
         <f>IF(COUNTIF(D:D,$A290)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D290" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="F290" s="2"/>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B291" t="s">
         <v>7</v>
@@ -6242,11 +6245,14 @@
         <f>IF(COUNTIF(D:D,$A291)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D291" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="F291" s="2"/>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B292" t="s">
         <v>7</v>
@@ -6256,13 +6262,13 @@
         <v>Missing</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>101</v>
+        <v>150</v>
       </c>
       <c r="F292" s="2"/>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B293" t="s">
         <v>7</v>
@@ -6272,13 +6278,13 @@
         <v>Missing</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F293" s="2"/>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B294" t="s">
         <v>7</v>
@@ -6288,13 +6294,13 @@
         <v>Missing</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="F294" s="2"/>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B295" t="s">
         <v>7</v>
@@ -6304,13 +6310,13 @@
         <v>Missing</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="F295" s="2"/>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B296" t="s">
         <v>7</v>
@@ -6319,11 +6325,14 @@
         <f>IF(COUNTIF(D:D,$A296)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D296" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="F296" s="2"/>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B297" t="s">
         <v>7</v>
@@ -6332,11 +6341,14 @@
         <f>IF(COUNTIF(D:D,$A297)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D297" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="F297" s="2"/>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B298" t="s">
         <v>7</v>
@@ -6345,11 +6357,14 @@
         <f>IF(COUNTIF(D:D,$A298)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D298" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="F298" s="2"/>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B299" t="s">
         <v>7</v>
@@ -6358,11 +6373,14 @@
         <f>IF(COUNTIF(D:D,$A299)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D299" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="F299" s="2"/>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B300" t="s">
         <v>7</v>
@@ -6375,7 +6393,7 @@
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B301" t="s">
         <v>7</v>
@@ -6388,7 +6406,7 @@
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B302" t="s">
         <v>7</v>
@@ -6396,6 +6414,9 @@
       <c r="C302" t="str">
         <f>IF(COUNTIF(D:D,$A302)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
+      </c>
+      <c r="D302" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="F302" s="2"/>
     </row>
@@ -6410,6 +6431,9 @@
         <f>IF(COUNTIF(D:D,$A303)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D303" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="F303" s="2"/>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.25">
@@ -6423,6 +6447,9 @@
         <f>IF(COUNTIF(D:D,$A304)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D304" s="2" t="s">
+        <v>234</v>
+      </c>
       <c r="F304" s="2"/>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
@@ -6436,6 +6463,9 @@
         <f>IF(COUNTIF(D:D,$A305)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D305" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="F305" s="2"/>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.25">
@@ -6570,7 +6600,7 @@
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B316" t="s">
         <v>5</v>
@@ -6583,7 +6613,7 @@
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B317" t="s">
         <v>5</v>
@@ -6596,7 +6626,7 @@
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B318" t="s">
         <v>5</v>
@@ -6609,7 +6639,7 @@
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B319" t="s">
         <v>5</v>
@@ -6622,7 +6652,7 @@
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B320" t="s">
         <v>5</v>
@@ -6635,7 +6665,7 @@
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B321" t="s">
         <v>5</v>
@@ -6732,9 +6762,6 @@
         <f>IF(COUNTIF(D:D,$A328)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D328" s="2" t="s">
-        <v>231</v>
-      </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
@@ -6747,9 +6774,6 @@
         <f>IF(COUNTIF(D:D,$A329)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D329" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
@@ -6762,9 +6786,6 @@
         <f>IF(COUNTIF(D:D,$A330)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D330" s="2" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
@@ -6777,9 +6798,6 @@
         <f>IF(COUNTIF(D:D,$A331)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D331" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
@@ -6792,9 +6810,6 @@
         <f>IF(COUNTIF(D:D,$A332)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D332" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
@@ -6807,9 +6822,6 @@
         <f>IF(COUNTIF(D:D,$A333)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-      <c r="D333" s="2" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
@@ -6822,9 +6834,6 @@
         <f>IF(COUNTIF(D:D,$A334)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D334" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
@@ -6837,9 +6846,6 @@
         <f>IF(COUNTIF(D:D,$A335)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D335" s="2" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
@@ -6850,10 +6856,7 @@
       </c>
       <c r="C336" t="str">
         <f>IF(COUNTIF(D:D,$A336)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
-      </c>
-      <c r="D336" s="2" t="s">
-        <v>37</v>
+        <v>Implemented</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -6865,60 +6868,57 @@
       </c>
       <c r="C337" t="str">
         <f>IF(COUNTIF(D:D,$A337)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
-      </c>
-      <c r="D337" s="2" t="s">
-        <v>144</v>
+        <v>Implemented</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>240</v>
+        <v>400</v>
       </c>
       <c r="B338" t="s">
         <v>5</v>
       </c>
       <c r="C338" t="str">
         <f>IF(COUNTIF(D:D,$A338)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D338" s="2" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B339" t="s">
         <v>5</v>
       </c>
       <c r="C339" t="str">
         <f>IF(COUNTIF(D:D,$A339)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D339" s="2" t="s">
-        <v>156</v>
+        <v>31</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B340" t="s">
         <v>5</v>
       </c>
       <c r="C340" t="str">
         <f>IF(COUNTIF(D:D,$A340)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>215</v>
+        <v>65</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B341" t="s">
         <v>5</v>
@@ -6928,87 +6928,87 @@
         <v>Implemented</v>
       </c>
       <c r="D341" s="2" t="s">
-        <v>254</v>
+        <v>66</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B342" t="s">
         <v>5</v>
       </c>
       <c r="C342" t="str">
         <f>IF(COUNTIF(D:D,$A342)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D342" s="2" t="s">
-        <v>132</v>
+        <v>42</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B343" t="s">
         <v>5</v>
       </c>
       <c r="C343" t="str">
         <f>IF(COUNTIF(D:D,$A343)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>167</v>
+        <v>54</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B344" t="s">
         <v>5</v>
       </c>
       <c r="C344" t="str">
         <f>IF(COUNTIF(D:D,$A344)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D344" s="2" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B345" t="s">
         <v>5</v>
       </c>
       <c r="C345" t="str">
         <f>IF(COUNTIF(D:D,$A345)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D345" s="2" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B346" t="s">
         <v>5</v>
       </c>
       <c r="C346" t="str">
         <f>IF(COUNTIF(D:D,$A346)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D346" s="2" t="s">
-        <v>227</v>
+        <v>37</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B347" t="s">
         <v>5</v>
@@ -7018,12 +7018,12 @@
         <v>Missing</v>
       </c>
       <c r="D347" s="2" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B348" t="s">
         <v>5</v>
@@ -7033,12 +7033,12 @@
         <v>Missing</v>
       </c>
       <c r="D348" s="2" t="s">
-        <v>123</v>
+        <v>383</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B349" t="s">
         <v>5</v>
@@ -7048,12 +7048,12 @@
         <v>Implemented</v>
       </c>
       <c r="D349" s="2" t="s">
-        <v>238</v>
+        <v>156</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B350" t="s">
         <v>5</v>
@@ -7063,12 +7063,12 @@
         <v>Missing</v>
       </c>
       <c r="D350" s="2" t="s">
-        <v>368</v>
+        <v>215</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B351" t="s">
         <v>5</v>
@@ -7078,12 +7078,12 @@
         <v>Missing</v>
       </c>
       <c r="D351" s="2" t="s">
-        <v>104</v>
+        <v>253</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B352" t="s">
         <v>5</v>
@@ -7092,10 +7092,13 @@
         <f>IF(COUNTIF(D:D,$A352)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D352" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B353" t="s">
         <v>5</v>
@@ -7104,10 +7107,13 @@
         <f>IF(COUNTIF(D:D,$A353)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D353" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B354" t="s">
         <v>5</v>
@@ -7116,10 +7122,13 @@
         <f>IF(COUNTIF(D:D,$A354)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D354" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B355" t="s">
         <v>5</v>
@@ -7128,10 +7137,13 @@
         <f>IF(COUNTIF(D:D,$A355)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D355" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B356" t="s">
         <v>5</v>
@@ -7140,10 +7152,13 @@
         <f>IF(COUNTIF(D:D,$A356)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D356" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B357" t="s">
         <v>5</v>
@@ -7152,10 +7167,13 @@
         <f>IF(COUNTIF(D:D,$A357)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D357" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B358" t="s">
         <v>5</v>
@@ -7164,10 +7182,13 @@
         <f>IF(COUNTIF(D:D,$A358)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D358" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B359" t="s">
         <v>5</v>
@@ -7176,10 +7197,13 @@
         <f>IF(COUNTIF(D:D,$A359)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D359" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B360" t="s">
         <v>5</v>
@@ -7188,10 +7212,13 @@
         <f>IF(COUNTIF(D:D,$A360)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D360" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B361" t="s">
         <v>5</v>
@@ -7200,10 +7227,13 @@
         <f>IF(COUNTIF(D:D,$A361)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-    </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D361" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B362" t="s">
         <v>5</v>
@@ -7213,9 +7243,9 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B363" t="s">
         <v>5</v>
@@ -7225,9 +7255,9 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B364" t="s">
         <v>5</v>
@@ -7237,9 +7267,9 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B365" t="s">
         <v>5</v>
@@ -7249,9 +7279,9 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B366" t="s">
         <v>5</v>
@@ -7261,9 +7291,9 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B367" t="s">
         <v>5</v>
@@ -7273,9 +7303,9 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B368" t="s">
         <v>5</v>
@@ -7287,7 +7317,7 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B369" t="s">
         <v>5</v>
@@ -7299,7 +7329,7 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B370" t="s">
         <v>5</v>
@@ -7311,7 +7341,7 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B371" t="s">
         <v>5</v>
@@ -7323,7 +7353,7 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B372" t="s">
         <v>5</v>
@@ -7335,7 +7365,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B373" t="s">
         <v>5</v>
@@ -7347,7 +7377,7 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B374" t="s">
         <v>5</v>
@@ -7359,7 +7389,7 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B375" t="s">
         <v>5</v>
@@ -7371,7 +7401,7 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B376" t="s">
         <v>5</v>
@@ -7383,7 +7413,7 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B377" t="s">
         <v>5</v>
@@ -7395,7 +7425,7 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B378" t="s">
         <v>5</v>
@@ -7407,7 +7437,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B379" t="s">
         <v>5</v>
@@ -7419,7 +7449,7 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B380" t="s">
         <v>5</v>
@@ -7431,7 +7461,7 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B381" t="s">
         <v>5</v>
@@ -7443,7 +7473,7 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B382" t="s">
         <v>5</v>
@@ -7455,7 +7485,7 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B383" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
- implemented the following rare cards: Pint-Sized Summoner, Twilight Drake,
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$296</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$307</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="402">
   <si>
     <t>Cardname</t>
   </si>
@@ -1235,6 +1235,9 @@
   </si>
   <si>
     <t>Lightning Storm</t>
+  </si>
+  <si>
+    <t>Secret Keeper</t>
   </si>
 </sst>
 </file>
@@ -1605,7 +1608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K383"/>
+  <dimension ref="A1:K390"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A351" sqref="A351"/>
@@ -1793,7 +1796,7 @@
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>295</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1816,7 +1819,7 @@
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1927,7 +1930,7 @@
         <v>Implemented</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>194</v>
+        <v>272</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -1943,7 +1946,7 @@
         <v>Implemented</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>363</v>
+        <v>194</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1959,7 +1962,7 @@
         <v>Implemented</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>369</v>
+        <v>279</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -1975,7 +1978,7 @@
         <v>Implemented</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1991,7 +1994,7 @@
         <v>Implemented</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>211</v>
+        <v>369</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -2007,7 +2010,7 @@
         <v>Implemented</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>10</v>
+        <v>382</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -2023,7 +2026,7 @@
         <v>Implemented</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -2039,7 +2042,7 @@
         <v>Implemented</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -2055,7 +2058,7 @@
         <v>Implemented</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>237</v>
+        <v>14</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -2071,7 +2074,7 @@
         <v>Implemented</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>240</v>
+        <v>139</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -2087,7 +2090,7 @@
         <v>Implemented</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="F26" s="2"/>
     </row>
@@ -2103,7 +2106,7 @@
         <v>Implemented</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -2119,7 +2122,7 @@
         <v>Implemented</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -2135,7 +2138,7 @@
         <v>Implemented</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>68</v>
+        <v>243</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -2151,7 +2154,7 @@
         <v>Implemented</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="F30" s="2"/>
     </row>
@@ -2167,7 +2170,7 @@
         <v>Implemented</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -2183,7 +2186,7 @@
         <v>Implemented</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>264</v>
+        <v>70</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -2199,7 +2202,7 @@
         <v>Implemented</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -2215,7 +2218,7 @@
         <v>Implemented</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>184</v>
+        <v>264</v>
       </c>
       <c r="F34" s="2"/>
     </row>
@@ -2231,7 +2234,7 @@
         <v>Implemented</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>321</v>
+        <v>88</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -2247,7 +2250,7 @@
         <v>Implemented</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>192</v>
+        <v>273</v>
       </c>
       <c r="F36" s="2"/>
     </row>
@@ -2263,7 +2266,7 @@
         <v>Implemented</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>364</v>
+        <v>184</v>
       </c>
       <c r="F37" s="2"/>
     </row>
@@ -2279,7 +2282,7 @@
         <v>Implemented</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>370</v>
+        <v>321</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -2295,7 +2298,7 @@
         <v>Implemented</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>372</v>
+        <v>192</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -2311,7 +2314,7 @@
         <v>Implemented</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -2327,7 +2330,7 @@
         <v>Implemented</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>206</v>
+        <v>370</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -2343,7 +2346,7 @@
         <v>Implemented</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>11</v>
+        <v>372</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -2359,7 +2362,7 @@
         <v>Implemented</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>12</v>
+        <v>374</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -2375,7 +2378,7 @@
         <v>Implemented</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>13</v>
+        <v>206</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -2391,7 +2394,7 @@
         <v>Implemented</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>226</v>
+        <v>11</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -2407,7 +2410,7 @@
         <v>Implemented</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -2423,7 +2426,7 @@
         <v>Implemented</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>231</v>
+        <v>13</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -2439,7 +2442,7 @@
         <v>Implemented</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>399</v>
+        <v>226</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -2455,7 +2458,7 @@
         <v>Implemented</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -2471,7 +2474,7 @@
         <v>Implemented</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -2487,7 +2490,7 @@
         <v>Implemented</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>51</v>
+        <v>399</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -2503,7 +2506,7 @@
         <v>Implemented</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -2519,7 +2522,7 @@
         <v>Implemented</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -2535,7 +2538,7 @@
         <v>Implemented</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>160</v>
+        <v>51</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -2551,7 +2554,7 @@
         <v>Implemented</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>252</v>
+        <v>49</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -2567,7 +2570,7 @@
         <v>Implemented</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F56" s="2"/>
     </row>
@@ -2583,7 +2586,7 @@
         <v>Implemented</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F57" s="2"/>
     </row>
@@ -2599,7 +2602,7 @@
         <v>Implemented</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>85</v>
+        <v>252</v>
       </c>
       <c r="F58" s="2"/>
     </row>
@@ -2615,7 +2618,7 @@
         <v>Implemented</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>96</v>
+        <v>170</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -2631,7 +2634,7 @@
         <v>Implemented</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>317</v>
+        <v>172</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -2647,7 +2650,7 @@
         <v>Implemented</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>193</v>
+        <v>85</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -2663,7 +2666,7 @@
         <v>Implemented</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>323</v>
+        <v>96</v>
       </c>
       <c r="F62" s="2"/>
     </row>
@@ -2679,7 +2682,7 @@
         <v>Implemented</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>284</v>
+        <v>317</v>
       </c>
       <c r="F63" s="2"/>
     </row>
@@ -2695,7 +2698,7 @@
         <v>Implemented</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>380</v>
+        <v>193</v>
       </c>
       <c r="F64" s="2"/>
     </row>
@@ -2711,7 +2714,7 @@
         <v>Implemented</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>115</v>
+        <v>323</v>
       </c>
       <c r="F65" s="2"/>
     </row>
@@ -2727,7 +2730,7 @@
         <v>Implemented</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>121</v>
+        <v>284</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -2743,7 +2746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>3</v>
+        <v>380</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -2759,7 +2762,7 @@
         <v>Implemented</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F68" s="2"/>
     </row>
@@ -2775,7 +2778,7 @@
         <v>Implemented</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>398</v>
+        <v>121</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -2791,7 +2794,7 @@
         <v>Implemented</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="F70" s="2"/>
     </row>
@@ -2807,7 +2810,7 @@
         <v>Implemented</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F71" s="2"/>
     </row>
@@ -2823,7 +2826,7 @@
         <v>Implemented</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>215</v>
+        <v>398</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -2839,7 +2842,7 @@
         <v>Implemented</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>216</v>
+        <v>120</v>
       </c>
       <c r="F73" s="2"/>
     </row>
@@ -2855,7 +2858,7 @@
         <v>Implemented</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>217</v>
+        <v>123</v>
       </c>
       <c r="F74" s="2"/>
     </row>
@@ -2871,7 +2874,7 @@
         <v>Implemented</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -2887,7 +2890,7 @@
         <v>Implemented</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>16</v>
+        <v>216</v>
       </c>
       <c r="F76" s="2"/>
     </row>
@@ -2903,7 +2906,7 @@
         <v>Implemented</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F77" s="2"/>
     </row>
@@ -2919,7 +2922,7 @@
         <v>Implemented</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>126</v>
+        <v>218</v>
       </c>
       <c r="F78" s="2"/>
     </row>
@@ -2935,7 +2938,7 @@
         <v>Implemented</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>222</v>
+        <v>16</v>
       </c>
       <c r="F79" s="2"/>
     </row>
@@ -2951,7 +2954,7 @@
         <v>Implemented</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>22</v>
+        <v>219</v>
       </c>
       <c r="F80" s="2"/>
     </row>
@@ -2967,7 +2970,7 @@
         <v>Implemented</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>227</v>
+        <v>126</v>
       </c>
       <c r="F81" s="2"/>
     </row>
@@ -2983,7 +2986,7 @@
         <v>Implemented</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>131</v>
+        <v>222</v>
       </c>
       <c r="F82" s="2"/>
     </row>
@@ -2999,7 +3002,7 @@
         <v>Implemented</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F83" s="2"/>
     </row>
@@ -3015,7 +3018,7 @@
         <v>Implemented</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>25</v>
+        <v>227</v>
       </c>
       <c r="F84" s="2"/>
     </row>
@@ -3031,7 +3034,7 @@
         <v>Implemented</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="F85" s="2"/>
     </row>
@@ -3047,7 +3050,7 @@
         <v>Implemented</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F86" s="2"/>
     </row>
@@ -3063,7 +3066,7 @@
         <v>Implemented</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>228</v>
+        <v>25</v>
       </c>
       <c r="F87" s="2"/>
     </row>
@@ -3079,7 +3082,7 @@
         <v>Implemented</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>229</v>
+        <v>26</v>
       </c>
       <c r="F88" s="2"/>
     </row>
@@ -3095,7 +3098,7 @@
         <v>Implemented</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F89" s="2"/>
     </row>
@@ -3111,7 +3114,7 @@
         <v>Implemented</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F90" s="2"/>
     </row>
@@ -3127,7 +3130,7 @@
         <v>Implemented</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="F91" s="2"/>
     </row>
@@ -3143,7 +3146,7 @@
         <v>Implemented</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F92" s="2"/>
     </row>
@@ -3159,7 +3162,7 @@
         <v>Implemented</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>138</v>
+        <v>232</v>
       </c>
       <c r="F93" s="2"/>
     </row>
@@ -3175,7 +3178,7 @@
         <v>Implemented</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="F94" s="2"/>
     </row>
@@ -3191,7 +3194,7 @@
         <v>Implemented</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>233</v>
+        <v>34</v>
       </c>
       <c r="F95" s="2"/>
     </row>
@@ -3207,7 +3210,7 @@
         <v>Implemented</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>234</v>
+        <v>138</v>
       </c>
       <c r="F96" s="2"/>
     </row>
@@ -3223,7 +3226,7 @@
         <v>Implemented</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>142</v>
+        <v>35</v>
       </c>
       <c r="F97" s="2"/>
     </row>
@@ -3239,7 +3242,7 @@
         <v>Missing</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>38</v>
+        <v>233</v>
       </c>
       <c r="F98" s="2"/>
     </row>
@@ -3255,7 +3258,7 @@
         <v>Missing</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>143</v>
+        <v>234</v>
       </c>
       <c r="F99" s="2"/>
     </row>
@@ -3271,7 +3274,7 @@
         <v>Missing</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F100" s="2"/>
     </row>
@@ -3287,7 +3290,7 @@
         <v>Missing</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F101" s="2"/>
     </row>
@@ -3303,7 +3306,7 @@
         <v>Missing</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>238</v>
+        <v>143</v>
       </c>
       <c r="F102" s="2"/>
     </row>
@@ -3319,7 +3322,7 @@
         <v>Missing</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F103" s="2"/>
     </row>
@@ -3335,7 +3338,7 @@
         <v>Missing</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>152</v>
+        <v>41</v>
       </c>
       <c r="F104" s="2"/>
     </row>
@@ -3351,7 +3354,7 @@
         <v>Missing</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="F105" s="2"/>
     </row>
@@ -3367,7 +3370,7 @@
         <v>Missing</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F106" s="2"/>
     </row>
@@ -3383,7 +3386,7 @@
         <v>Missing</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="F107" s="2"/>
     </row>
@@ -3399,7 +3402,7 @@
         <v>Missing</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="F108" s="2"/>
     </row>
@@ -3415,7 +3418,7 @@
         <v>Missing</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>245</v>
+        <v>157</v>
       </c>
       <c r="F109" s="2"/>
     </row>
@@ -3431,7 +3434,7 @@
         <v>Missing</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F110" s="2"/>
     </row>
@@ -3447,7 +3450,7 @@
         <v>Missing</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F111" s="2"/>
     </row>
@@ -3463,7 +3466,7 @@
         <v>Missing</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>56</v>
+        <v>245</v>
       </c>
       <c r="F112" s="2"/>
     </row>
@@ -3479,7 +3482,7 @@
         <v>Missing</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F113" s="2"/>
     </row>
@@ -3495,7 +3498,7 @@
         <v>Missing</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>158</v>
+        <v>55</v>
       </c>
       <c r="F114" s="2"/>
     </row>
@@ -3511,7 +3514,7 @@
         <v>Missing</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>249</v>
+        <v>56</v>
       </c>
       <c r="F115" s="2"/>
     </row>
@@ -3527,7 +3530,7 @@
         <v>Missing</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>250</v>
+        <v>58</v>
       </c>
       <c r="F116" s="2"/>
     </row>
@@ -3543,7 +3546,7 @@
         <v>Missing</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F117" s="2"/>
     </row>
@@ -3559,7 +3562,7 @@
         <v>Missing</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>73</v>
+        <v>249</v>
       </c>
       <c r="F118" s="2"/>
     </row>
@@ -3575,7 +3578,7 @@
         <v>Missing</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>74</v>
+        <v>250</v>
       </c>
       <c r="F119" s="2"/>
     </row>
@@ -3591,7 +3594,7 @@
         <v>Missing</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F120" s="2"/>
     </row>
@@ -3607,7 +3610,7 @@
         <v>Missing</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>253</v>
+        <v>73</v>
       </c>
       <c r="F121" s="2"/>
     </row>
@@ -3623,7 +3626,7 @@
         <v>Missing</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F122" s="2"/>
     </row>
@@ -3639,7 +3642,7 @@
         <v>Missing</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F123" s="2"/>
     </row>
@@ -3655,7 +3658,7 @@
         <v>Missing</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F124" s="2"/>
     </row>
@@ -3671,7 +3674,7 @@
         <v>Missing</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>168</v>
+        <v>76</v>
       </c>
       <c r="F125" s="2"/>
     </row>
@@ -3687,7 +3690,7 @@
         <v>Missing</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>79</v>
+        <v>165</v>
       </c>
       <c r="F126" s="2"/>
     </row>
@@ -3703,7 +3706,7 @@
         <v>Missing</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>169</v>
+        <v>255</v>
       </c>
       <c r="F127" s="2"/>
     </row>
@@ -3719,7 +3722,7 @@
         <v>Missing</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>80</v>
+        <v>168</v>
       </c>
       <c r="F128" s="2"/>
     </row>
@@ -3735,7 +3738,7 @@
         <v>Missing</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>257</v>
+        <v>79</v>
       </c>
       <c r="F129" s="2"/>
     </row>
@@ -3751,7 +3754,7 @@
         <v>Missing</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>259</v>
+        <v>169</v>
       </c>
       <c r="F130" s="2"/>
     </row>
@@ -3767,7 +3770,7 @@
         <v>Implemented</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>262</v>
+        <v>80</v>
       </c>
       <c r="F131" s="2"/>
     </row>
@@ -3783,7 +3786,7 @@
         <v>Missing</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="F132" s="2"/>
     </row>
@@ -3799,7 +3802,7 @@
         <v>Missing</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>173</v>
+        <v>259</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -3815,7 +3818,7 @@
         <v>Implemented</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>89</v>
+        <v>262</v>
       </c>
       <c r="F134" s="2"/>
     </row>
@@ -3831,7 +3834,7 @@
         <v>Implemented</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F135" s="2"/>
     </row>
@@ -3847,7 +3850,7 @@
         <v>Implemented</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>90</v>
+        <v>173</v>
       </c>
       <c r="F136" s="2"/>
     </row>
@@ -3863,7 +3866,7 @@
         <v>Implemented</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -3879,7 +3882,7 @@
         <v>Implemented</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>93</v>
+        <v>266</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -3895,7 +3898,7 @@
         <v>Implemented</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -3911,7 +3914,7 @@
         <v>Implemented</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -3927,7 +3930,7 @@
         <v>Implemented</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>178</v>
+        <v>93</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -3943,7 +3946,7 @@
         <v>Implemented</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>270</v>
+        <v>94</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -3959,7 +3962,7 @@
         <v>Implemented</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>179</v>
+        <v>95</v>
       </c>
       <c r="F143" s="2"/>
     </row>
@@ -3975,7 +3978,7 @@
         <v>Implemented</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>98</v>
+        <v>178</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -3991,7 +3994,7 @@
         <v>Implemented</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F145" s="2"/>
     </row>
@@ -4007,7 +4010,7 @@
         <v>Implemented</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="F146" s="2"/>
     </row>
@@ -4023,7 +4026,7 @@
         <v>Implemented</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4039,7 +4042,7 @@
         <v>Implemented</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>101</v>
+        <v>271</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4055,7 +4058,7 @@
         <v>Implemented</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>183</v>
+        <v>99</v>
       </c>
       <c r="F149" s="2"/>
     </row>
@@ -4071,7 +4074,7 @@
         <v>Implemented</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4086,7 +4089,7 @@
         <v>Implemented</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4101,7 +4104,7 @@
         <v>Implemented</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4116,7 +4119,7 @@
         <v>Implemented</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4131,7 +4134,7 @@
         <v>Implemented</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>189</v>
+        <v>106</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4146,7 +4149,7 @@
         <v>Implemented</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>190</v>
+        <v>110</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,7 +4164,7 @@
         <v>Implemented</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4176,7 +4179,7 @@
         <v>Implemented</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>196</v>
+        <v>392</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4191,7 +4194,7 @@
         <v>Implemented</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4206,7 +4209,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>365</v>
+        <v>190</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,7 +4224,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>366</v>
+        <v>195</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4236,7 +4239,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>367</v>
+        <v>196</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4254,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>393</v>
+        <v>197</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,7 +4269,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>199</v>
+        <v>278</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,7 +4284,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>201</v>
+        <v>365</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,7 +4299,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>204</v>
+        <v>366</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,7 +4314,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>207</v>
+        <v>367</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,7 +4329,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>377</v>
+        <v>393</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,7 +4344,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>378</v>
+        <v>199</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4356,7 +4359,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>208</v>
+        <v>280</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,7 +4374,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>209</v>
+        <v>281</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,7 +4389,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>385</v>
+        <v>201</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4404,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4419,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,7 +4434,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>288</v>
+        <v>377</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4446,7 +4449,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>213</v>
+        <v>378</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,7 +4464,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>118</v>
+        <v>208</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,7 +4479,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>125</v>
+        <v>209</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4494,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>225</v>
+        <v>385</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4509,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>20</v>
+        <v>210</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4521,7 +4524,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>21</v>
+        <v>212</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4536,7 +4539,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>129</v>
+        <v>288</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,7 +4554,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>31</v>
+        <v>213</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,7 +4569,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>235</v>
+        <v>118</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4581,7 +4584,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>239</v>
+        <v>125</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,7 +4599,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>150</v>
+        <v>225</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +4614,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4629,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +4644,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,7 +4659,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,7 +4674,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4689,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>69</v>
+        <v>239</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +4704,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>78</v>
+        <v>150</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4716,7 +4719,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4731,7 +4734,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4746,7 +4749,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4761,7 +4764,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>373</v>
+        <v>65</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4776,7 +4779,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,7 +4794,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,7 +4809,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,7 +4824,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>247</v>
+        <v>175</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4839,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>66</v>
+        <v>181</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4851,7 +4854,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>67</v>
+        <v>182</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4866,7 +4869,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>161</v>
+        <v>373</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,7 +4884,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>167</v>
+        <v>221</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4896,7 +4899,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4911,7 +4914,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>260</v>
+        <v>37</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,7 +4929,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>82</v>
+        <v>247</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4941,7 +4944,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4956,7 +4959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4971,7 +4974,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>92</v>
+        <v>161</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,7 +4989,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>97</v>
+        <v>167</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,7 +5004,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>108</v>
+        <v>256</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5016,7 +5019,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>109</v>
+        <v>260</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5031,7 +5034,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>188</v>
+        <v>82</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,7 +5049,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>202</v>
+        <v>83</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5061,7 +5064,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>203</v>
+        <v>84</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,7 +5079,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,7 +5094,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5106,7 +5109,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>19</v>
+        <v>275</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,7 +5124,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,7 +5139,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>224</v>
+        <v>109</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5151,7 +5154,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>133</v>
+        <v>188</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5166,7 +5169,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,7 +5184,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>36</v>
+        <v>203</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5196,7 +5199,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>140</v>
+        <v>18</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5211,7 +5214,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>148</v>
+        <v>17</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5226,7 +5229,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5241,7 +5244,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>246</v>
+        <v>128</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,7 +5259,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5271,7 +5274,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>268</v>
+        <v>133</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5289,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5302,7 +5305,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5318,7 +5321,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5334,7 +5337,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5350,7 +5353,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>362</v>
+        <v>43</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5366,7 +5369,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>375</v>
+        <v>246</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5382,7 +5385,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>9</v>
+        <v>261</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5398,7 +5401,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>214</v>
+        <v>268</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5414,7 +5417,7 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5430,7 +5433,7 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5446,7 +5449,7 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5462,7 +5465,7 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>242</v>
+        <v>277</v>
       </c>
       <c r="F242" s="2"/>
     </row>
@@ -5478,7 +5481,7 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="F243" s="2"/>
     </row>
@@ -5494,7 +5497,7 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>48</v>
+        <v>362</v>
       </c>
       <c r="F244" s="2"/>
     </row>
@@ -5510,7 +5513,7 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>155</v>
+        <v>375</v>
       </c>
       <c r="F245" s="2"/>
     </row>
@@ -5526,7 +5529,7 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F246" s="2"/>
     </row>
@@ -5542,7 +5545,7 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="F247" s="2"/>
     </row>
@@ -5558,7 +5561,7 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>254</v>
+        <v>23</v>
       </c>
       <c r="F248" s="2"/>
     </row>
@@ -5574,7 +5577,7 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="F249" s="2"/>
     </row>
@@ -5590,7 +5593,7 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>400</v>
+        <v>146</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5606,7 +5609,7 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5622,7 +5625,7 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5638,7 +5641,7 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>198</v>
+        <v>48</v>
       </c>
       <c r="F253" s="2"/>
     </row>
@@ -5654,7 +5657,7 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>371</v>
+        <v>155</v>
       </c>
       <c r="F254" s="2"/>
     </row>
@@ -5670,7 +5673,7 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>205</v>
+        <v>50</v>
       </c>
       <c r="F255" s="2"/>
     </row>
@@ -5686,7 +5689,7 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>383</v>
+        <v>64</v>
       </c>
       <c r="F256" s="2"/>
     </row>
@@ -5702,7 +5705,7 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>384</v>
+        <v>254</v>
       </c>
       <c r="F257" s="2"/>
     </row>
@@ -5718,7 +5721,7 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="F258" s="2"/>
     </row>
@@ -5734,7 +5737,7 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>33</v>
+        <v>400</v>
       </c>
       <c r="F259" s="2"/>
     </row>
@@ -5750,7 +5753,7 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>141</v>
+        <v>258</v>
       </c>
       <c r="F260" s="2"/>
     </row>
@@ -5766,7 +5769,7 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>236</v>
+        <v>102</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -5782,7 +5785,7 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>39</v>
+        <v>198</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -5798,7 +5801,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>40</v>
+        <v>371</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5814,7 +5817,7 @@
         <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>241</v>
+        <v>205</v>
       </c>
       <c r="F264" s="2"/>
     </row>
@@ -5830,7 +5833,7 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>153</v>
+        <v>383</v>
       </c>
       <c r="F265" s="2"/>
     </row>
@@ -5846,7 +5849,7 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>62</v>
+        <v>384</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -5862,7 +5865,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5878,7 +5881,7 @@
         <v>Missing</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>177</v>
+        <v>33</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5894,7 +5897,7 @@
         <v>Missing</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -5910,7 +5913,7 @@
         <v>Missing</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>185</v>
+        <v>236</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -5926,7 +5929,7 @@
         <v>Missing</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -5942,7 +5945,7 @@
         <v>Missing</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -5958,7 +5961,7 @@
         <v>Missing</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>368</v>
+        <v>241</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -5974,7 +5977,7 @@
         <v>Missing</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>200</v>
+        <v>153</v>
       </c>
       <c r="F274" s="2"/>
     </row>
@@ -5990,7 +5993,7 @@
         <v>Missing</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>376</v>
+        <v>62</v>
       </c>
       <c r="F275" s="2"/>
     </row>
@@ -6006,7 +6009,7 @@
         <v>Missing</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="F276" s="2"/>
     </row>
@@ -6022,7 +6025,7 @@
         <v>Missing</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>15</v>
+        <v>177</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -6038,7 +6041,7 @@
         <v>Missing</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>220</v>
+        <v>103</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -6054,7 +6057,7 @@
         <v>Missing</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="F279" s="2"/>
     </row>
@@ -6070,7 +6073,7 @@
         <v>Missing</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="F280" s="2"/>
     </row>
@@ -6086,7 +6089,7 @@
         <v>Missing</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>30</v>
+        <v>276</v>
       </c>
       <c r="F281" s="2"/>
     </row>
@@ -6102,7 +6105,7 @@
         <v>Missing</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>230</v>
+        <v>397</v>
       </c>
       <c r="F282" s="2"/>
     </row>
@@ -6118,7 +6121,7 @@
         <v>Missing</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="F283" s="2"/>
     </row>
@@ -6134,7 +6137,7 @@
         <v>Missing</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>42</v>
+        <v>368</v>
       </c>
       <c r="F284" s="2"/>
     </row>
@@ -6150,7 +6153,7 @@
         <v>Missing</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>44</v>
+        <v>200</v>
       </c>
       <c r="F285" s="2"/>
     </row>
@@ -6166,7 +6169,7 @@
         <v>Missing</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>244</v>
+        <v>376</v>
       </c>
       <c r="F286" s="2"/>
     </row>
@@ -6182,7 +6185,7 @@
         <v>Missing</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>334</v>
+        <v>124</v>
       </c>
       <c r="F287" s="2"/>
     </row>
@@ -6198,7 +6201,7 @@
         <v>Missing</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="F288" s="2"/>
     </row>
@@ -6214,7 +6217,7 @@
         <v>Missing</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="F289" s="2"/>
     </row>
@@ -6230,7 +6233,7 @@
         <v>Missing</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="F290" s="2"/>
     </row>
@@ -6246,7 +6249,7 @@
         <v>Missing</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>265</v>
+        <v>27</v>
       </c>
       <c r="F291" s="2"/>
     </row>
@@ -6262,7 +6265,7 @@
         <v>Missing</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>180</v>
+        <v>30</v>
       </c>
       <c r="F292" s="2"/>
     </row>
@@ -6278,7 +6281,7 @@
         <v>Missing</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>111</v>
+        <v>230</v>
       </c>
       <c r="F293" s="2"/>
     </row>
@@ -6294,7 +6297,7 @@
         <v>Missing</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>191</v>
+        <v>136</v>
       </c>
       <c r="F294" s="2"/>
     </row>
@@ -6310,7 +6313,7 @@
         <v>Missing</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>379</v>
+        <v>42</v>
       </c>
       <c r="F295" s="2"/>
     </row>
@@ -6326,7 +6329,7 @@
         <v>Missing</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>381</v>
+        <v>44</v>
       </c>
       <c r="F296" s="2"/>
     </row>
@@ -6342,7 +6345,7 @@
         <v>Missing</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>32</v>
+        <v>244</v>
       </c>
       <c r="F297" s="2"/>
     </row>
@@ -6358,7 +6361,7 @@
         <v>Missing</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>137</v>
+        <v>334</v>
       </c>
       <c r="F298" s="2"/>
     </row>
@@ -6374,7 +6377,7 @@
         <v>Missing</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>151</v>
+        <v>63</v>
       </c>
       <c r="F299" s="2"/>
     </row>
@@ -6390,7 +6393,7 @@
         <v>Missing</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>245</v>
+        <v>162</v>
       </c>
       <c r="F300" s="2"/>
     </row>
@@ -6406,7 +6409,7 @@
         <v>Missing</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>198</v>
+        <v>77</v>
       </c>
       <c r="F301" s="2"/>
     </row>
@@ -6422,7 +6425,7 @@
         <v>Missing</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>394</v>
+        <v>265</v>
       </c>
       <c r="F302" s="2"/>
     </row>
@@ -6438,7 +6441,7 @@
         <v>Implemented</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
       <c r="F303" s="2"/>
     </row>
@@ -6454,7 +6457,7 @@
         <v>Implemented</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="F304" s="2"/>
     </row>
@@ -6470,7 +6473,7 @@
         <v>Implemented</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>63</v>
+        <v>191</v>
       </c>
       <c r="F305" s="2"/>
     </row>
@@ -6486,7 +6489,7 @@
         <v>Implemented</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>122</v>
+        <v>379</v>
       </c>
       <c r="F306" s="2"/>
     </row>
@@ -6502,7 +6505,7 @@
         <v>Implemented</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>228</v>
+        <v>381</v>
       </c>
       <c r="F307" s="2"/>
     </row>
@@ -6518,7 +6521,7 @@
         <v>Implemented</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>154</v>
+        <v>32</v>
       </c>
       <c r="F308" s="2"/>
     </row>
@@ -6534,7 +6537,7 @@
         <v>Implemented</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="F309" s="2"/>
     </row>
@@ -6550,7 +6553,7 @@
         <v>Implemented</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F310" s="2"/>
     </row>
@@ -6566,7 +6569,7 @@
         <v>Implemented</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>161</v>
+        <v>245</v>
       </c>
       <c r="F311" s="2"/>
     </row>
@@ -6582,7 +6585,7 @@
         <v>Implemented</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F312" s="2"/>
     </row>
@@ -6598,7 +6601,7 @@
         <v>Implemented</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>133</v>
+        <v>394</v>
       </c>
       <c r="F313" s="2"/>
     </row>
@@ -6614,7 +6617,7 @@
         <v>Implemented</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="F314" s="2"/>
     </row>
@@ -6630,7 +6633,7 @@
         <v>Implemented</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="F315" s="2"/>
     </row>
@@ -6646,7 +6649,7 @@
         <v>Implemented</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="F316" s="2"/>
     </row>
@@ -6662,7 +6665,7 @@
         <v>Implemented</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="F317" s="2"/>
     </row>
@@ -6677,6 +6680,9 @@
         <f>IF(COUNTIF(D:D,$A318)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D318" s="2" t="s">
+        <v>228</v>
+      </c>
       <c r="F318" s="2"/>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
@@ -6690,6 +6696,9 @@
         <f>IF(COUNTIF(D:D,$A319)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D319" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="F319" s="2"/>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
@@ -6704,7 +6713,7 @@
         <v>Implemented</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>101</v>
+        <v>173</v>
       </c>
       <c r="F320" s="2"/>
     </row>
@@ -6720,7 +6729,7 @@
         <v>Implemented</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -6736,7 +6745,7 @@
         <v>Implemented</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>234</v>
+        <v>161</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6752,7 +6761,7 @@
         <v>Implemented</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6767,6 +6776,9 @@
         <f>IF(COUNTIF(D:D,$A324)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D324" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F324" s="2"/>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
@@ -6780,6 +6792,9 @@
         <f>IF(COUNTIF(D:D,$A325)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D325" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
@@ -6792,6 +6807,9 @@
         <f>IF(COUNTIF(D:D,$A326)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D326" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
@@ -6804,6 +6822,9 @@
         <f>IF(COUNTIF(D:D,$A327)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D327" s="2" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
@@ -6816,6 +6837,9 @@
         <f>IF(COUNTIF(D:D,$A328)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D328" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
@@ -6852,6 +6876,9 @@
         <f>IF(COUNTIF(D:D,$A331)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D331" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
@@ -6864,6 +6891,9 @@
         <f>IF(COUNTIF(D:D,$A332)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D332" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
@@ -6876,6 +6906,9 @@
         <f>IF(COUNTIF(D:D,$A333)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D333" s="2" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
@@ -6888,6 +6921,9 @@
         <f>IF(COUNTIF(D:D,$A334)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D334" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
@@ -7152,9 +7188,6 @@
         <f>IF(COUNTIF(D:D,$A356)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D356" s="2" t="s">
-        <v>231</v>
-      </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
@@ -7167,9 +7200,6 @@
         <f>IF(COUNTIF(D:D,$A357)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D357" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
@@ -7182,9 +7212,6 @@
         <f>IF(COUNTIF(D:D,$A358)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D358" s="2" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
@@ -7197,9 +7224,6 @@
         <f>IF(COUNTIF(D:D,$A359)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D359" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
@@ -7212,9 +7236,6 @@
         <f>IF(COUNTIF(D:D,$A360)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D360" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
@@ -7227,9 +7248,6 @@
         <f>IF(COUNTIF(D:D,$A361)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D361" s="2" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
@@ -7242,9 +7260,6 @@
         <f>IF(COUNTIF(D:D,$A362)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D362" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
@@ -7257,9 +7272,6 @@
         <f>IF(COUNTIF(D:D,$A363)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D363" s="2" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
@@ -7272,9 +7284,6 @@
         <f>IF(COUNTIF(D:D,$A364)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
-      <c r="D364" s="2" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
@@ -7287,9 +7296,6 @@
         <f>IF(COUNTIF(D:D,$A365)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D365" s="2" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
@@ -7302,9 +7308,6 @@
         <f>IF(COUNTIF(D:D,$A366)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D366" s="2" t="s">
-        <v>382</v>
-      </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
@@ -7315,10 +7318,10 @@
       </c>
       <c r="C367" t="str">
         <f>IF(COUNTIF(D:D,$A367)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D367" s="2" t="s">
-        <v>156</v>
+        <v>231</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -7330,10 +7333,10 @@
       </c>
       <c r="C368" t="str">
         <f>IF(COUNTIF(D:D,$A368)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D368" s="2" t="s">
-        <v>215</v>
+        <v>31</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -7348,7 +7351,7 @@
         <v>Missing</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>253</v>
+        <v>65</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7360,10 +7363,10 @@
       </c>
       <c r="C370" t="str">
         <f>IF(COUNTIF(D:D,$A370)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>132</v>
+        <v>66</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
@@ -7375,10 +7378,10 @@
       </c>
       <c r="C371" t="str">
         <f>IF(COUNTIF(D:D,$A371)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>167</v>
+        <v>42</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
@@ -7390,10 +7393,10 @@
       </c>
       <c r="C372" t="str">
         <f>IF(COUNTIF(D:D,$A372)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
@@ -7405,10 +7408,10 @@
       </c>
       <c r="C373" t="str">
         <f>IF(COUNTIF(D:D,$A373)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D373" s="2" t="s">
-        <v>155</v>
+        <v>57</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
@@ -7420,10 +7423,10 @@
       </c>
       <c r="C374" t="str">
         <f>IF(COUNTIF(D:D,$A374)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D374" s="2" t="s">
-        <v>227</v>
+        <v>115</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -7435,10 +7438,10 @@
       </c>
       <c r="C375" t="str">
         <f>IF(COUNTIF(D:D,$A375)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D375" s="2" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -7450,10 +7453,10 @@
       </c>
       <c r="C376" t="str">
         <f>IF(COUNTIF(D:D,$A376)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
@@ -7465,10 +7468,10 @@
       </c>
       <c r="C377" t="str">
         <f>IF(COUNTIF(D:D,$A377)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>238</v>
+        <v>382</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
@@ -7483,7 +7486,7 @@
         <v>Missing</v>
       </c>
       <c r="D378" s="2" t="s">
-        <v>366</v>
+        <v>156</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
@@ -7498,7 +7501,7 @@
         <v>Missing</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>104</v>
+        <v>215</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
@@ -7512,6 +7515,9 @@
         <f>IF(COUNTIF(D:D,$A380)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D380" s="2" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
@@ -7524,6 +7530,9 @@
         <f>IF(COUNTIF(D:D,$A381)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D381" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
@@ -7536,6 +7545,9 @@
         <f>IF(COUNTIF(D:D,$A382)&gt;0,"Implemented","Missing")</f>
         <v>Missing</v>
       </c>
+      <c r="D382" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
@@ -7547,6 +7559,44 @@
       <c r="C383" t="str">
         <f>IF(COUNTIF(D:D,$A383)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
+      </c>
+      <c r="D383" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D384" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="385" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D385" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="386" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D386" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="387" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D387" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="388" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D388" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="389" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D389" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="390" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D390" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- implemented the following rare cards: Violet Teacher, Wild Pyromancer, Void Terror, Upgrade!
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$307</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$312</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="401">
   <si>
     <t>Cardname</t>
   </si>
@@ -1235,9 +1235,6 @@
   </si>
   <si>
     <t>Lightning Storm</t>
-  </si>
-  <si>
-    <t>Secret Keeper</t>
   </si>
 </sst>
 </file>
@@ -1608,11 +1605,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K390"/>
+  <dimension ref="A1:K395"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A351" sqref="A351"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1796,7 +1791,7 @@
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1819,7 +1814,7 @@
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3978,7 +3973,7 @@
         <v>Implemented</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>178</v>
+        <v>269</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -3994,7 +3989,7 @@
         <v>Implemented</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>270</v>
+        <v>178</v>
       </c>
       <c r="F145" s="2"/>
     </row>
@@ -4010,7 +4005,7 @@
         <v>Implemented</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>179</v>
+        <v>270</v>
       </c>
       <c r="F146" s="2"/>
     </row>
@@ -4026,7 +4021,7 @@
         <v>Implemented</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>98</v>
+        <v>179</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4042,7 +4037,7 @@
         <v>Implemented</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>271</v>
+        <v>98</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4058,7 +4053,7 @@
         <v>Implemented</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>99</v>
+        <v>271</v>
       </c>
       <c r="F149" s="2"/>
     </row>
@@ -4074,7 +4069,7 @@
         <v>Implemented</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4089,7 +4084,7 @@
         <v>Implemented</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4104,7 +4099,7 @@
         <v>Implemented</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>183</v>
+        <v>101</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4119,7 +4114,7 @@
         <v>Implemented</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>401</v>
+        <v>183</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4134,7 +4129,7 @@
         <v>Implemented</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>106</v>
+        <v>274</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4149,7 +4144,7 @@
         <v>Implemented</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4164,7 +4159,7 @@
         <v>Implemented</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>187</v>
+        <v>110</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4179,7 +4174,7 @@
         <v>Implemented</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>392</v>
+        <v>187</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4194,7 +4189,7 @@
         <v>Implemented</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>189</v>
+        <v>392</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4209,7 +4204,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4224,7 +4219,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4239,7 +4234,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4254,7 +4249,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4269,7 +4264,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>278</v>
+        <v>197</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4284,7 +4279,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4299,7 +4294,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4314,7 +4309,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4329,7 +4324,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>393</v>
+        <v>367</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4344,7 +4339,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>199</v>
+        <v>393</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4359,7 +4354,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>280</v>
+        <v>199</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4374,7 +4369,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4389,7 +4384,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>201</v>
+        <v>281</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4404,7 +4399,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4419,7 +4414,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4434,7 +4429,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>377</v>
+        <v>282</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4449,7 +4444,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>378</v>
+        <v>207</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4464,7 +4459,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>208</v>
+        <v>285</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4479,7 +4474,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>209</v>
+        <v>377</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4494,7 +4489,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4509,7 +4504,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>210</v>
+        <v>287</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4524,7 +4519,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4539,7 +4534,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>288</v>
+        <v>209</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4554,7 +4549,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>213</v>
+        <v>385</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4569,7 +4564,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4584,7 +4579,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4599,7 +4594,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>225</v>
+        <v>288</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4614,7 +4609,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>20</v>
+        <v>213</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4629,7 +4624,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4644,7 +4639,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4659,7 +4654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>31</v>
+        <v>225</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4674,7 +4669,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>235</v>
+        <v>20</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4689,7 +4684,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>239</v>
+        <v>21</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4704,7 +4699,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4719,7 +4714,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4734,7 +4729,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>59</v>
+        <v>235</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4749,7 +4744,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>60</v>
+        <v>239</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4764,7 +4759,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4779,7 +4774,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>248</v>
+        <v>57</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4794,7 +4789,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4809,7 +4804,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4824,7 +4819,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>175</v>
+        <v>65</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4839,7 +4834,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4854,7 +4849,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>182</v>
+        <v>69</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4869,7 +4864,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>373</v>
+        <v>78</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4884,7 +4879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>221</v>
+        <v>175</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4899,7 +4894,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4914,7 +4909,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>37</v>
+        <v>182</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4929,7 +4924,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>247</v>
+        <v>373</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4944,7 +4939,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>66</v>
+        <v>221</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4959,7 +4954,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4974,7 +4969,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>161</v>
+        <v>37</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4989,7 +4984,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>167</v>
+        <v>247</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5004,7 +4999,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>256</v>
+        <v>66</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5019,7 +5014,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>260</v>
+        <v>67</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5034,7 +5029,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>82</v>
+        <v>161</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5049,7 +5044,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>83</v>
+        <v>167</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5064,7 +5059,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>84</v>
+        <v>256</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5079,7 +5074,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>92</v>
+        <v>260</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5094,7 +5089,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5109,7 +5104,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>275</v>
+        <v>83</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5124,7 +5119,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5139,7 +5134,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5154,7 +5149,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>188</v>
+        <v>97</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5169,7 +5164,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>202</v>
+        <v>275</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5184,7 +5179,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>203</v>
+        <v>108</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5199,7 +5194,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5214,7 +5209,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5229,7 +5224,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>19</v>
+        <v>202</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5244,7 +5239,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>128</v>
+        <v>203</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5259,7 +5254,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>224</v>
+        <v>18</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5274,7 +5269,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5289,7 +5284,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>134</v>
+        <v>19</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5305,7 +5300,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5321,7 +5316,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>140</v>
+        <v>224</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5337,7 +5332,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5353,7 +5348,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>43</v>
+        <v>134</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5369,7 +5364,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>246</v>
+        <v>36</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5385,7 +5380,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>261</v>
+        <v>140</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5401,7 +5396,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>268</v>
+        <v>148</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5417,7 +5412,7 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5433,7 +5428,7 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>186</v>
+        <v>246</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5449,7 +5444,7 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>112</v>
+        <v>261</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5465,7 +5460,7 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="F242" s="2"/>
     </row>
@@ -5481,7 +5476,7 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F243" s="2"/>
     </row>
@@ -5497,7 +5492,7 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>362</v>
+        <v>186</v>
       </c>
       <c r="F244" s="2"/>
     </row>
@@ -5513,7 +5508,7 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>375</v>
+        <v>112</v>
       </c>
       <c r="F245" s="2"/>
     </row>
@@ -5529,7 +5524,7 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>9</v>
+        <v>277</v>
       </c>
       <c r="F246" s="2"/>
     </row>
@@ -5545,7 +5540,7 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>214</v>
+        <v>113</v>
       </c>
       <c r="F247" s="2"/>
     </row>
@@ -5561,7 +5556,7 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>23</v>
+        <v>362</v>
       </c>
       <c r="F248" s="2"/>
     </row>
@@ -5577,7 +5572,7 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>145</v>
+        <v>375</v>
       </c>
       <c r="F249" s="2"/>
     </row>
@@ -5593,7 +5588,7 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>146</v>
+        <v>9</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5609,7 +5604,7 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5625,7 +5620,7 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5641,7 +5636,7 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>48</v>
+        <v>145</v>
       </c>
       <c r="F253" s="2"/>
     </row>
@@ -5657,7 +5652,7 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F254" s="2"/>
     </row>
@@ -5673,7 +5668,7 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>50</v>
+        <v>242</v>
       </c>
       <c r="F255" s="2"/>
     </row>
@@ -5689,7 +5684,7 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="F256" s="2"/>
     </row>
@@ -5705,7 +5700,7 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>254</v>
+        <v>48</v>
       </c>
       <c r="F257" s="2"/>
     </row>
@@ -5721,7 +5716,7 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="F258" s="2"/>
     </row>
@@ -5737,7 +5732,7 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="F259" s="2"/>
     </row>
@@ -5753,7 +5748,7 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>258</v>
+        <v>64</v>
       </c>
       <c r="F260" s="2"/>
     </row>
@@ -5769,7 +5764,7 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -5785,7 +5780,7 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -5801,7 +5796,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>371</v>
+        <v>400</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5817,7 +5812,7 @@
         <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
       <c r="F264" s="2"/>
     </row>
@@ -5833,7 +5828,7 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>383</v>
+        <v>102</v>
       </c>
       <c r="F265" s="2"/>
     </row>
@@ -5849,7 +5844,7 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>384</v>
+        <v>198</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -5865,7 +5860,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>130</v>
+        <v>371</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5881,7 +5876,7 @@
         <v>Missing</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>33</v>
+        <v>205</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5897,7 +5892,7 @@
         <v>Missing</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>141</v>
+        <v>383</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -5913,7 +5908,7 @@
         <v>Missing</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>236</v>
+        <v>384</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -5929,7 +5924,7 @@
         <v>Missing</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -5945,7 +5940,7 @@
         <v>Missing</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -5961,7 +5956,7 @@
         <v>Missing</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>241</v>
+        <v>141</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -5977,7 +5972,7 @@
         <v>Missing</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>153</v>
+        <v>236</v>
       </c>
       <c r="F274" s="2"/>
     </row>
@@ -5993,7 +5988,7 @@
         <v>Missing</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="F275" s="2"/>
     </row>
@@ -6009,7 +6004,7 @@
         <v>Missing</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="F276" s="2"/>
     </row>
@@ -6025,7 +6020,7 @@
         <v>Missing</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -6041,7 +6036,7 @@
         <v>Missing</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -6057,7 +6052,7 @@
         <v>Missing</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>185</v>
+        <v>62</v>
       </c>
       <c r="F279" s="2"/>
     </row>
@@ -6073,7 +6068,7 @@
         <v>Missing</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="F280" s="2"/>
     </row>
@@ -6089,7 +6084,7 @@
         <v>Missing</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>276</v>
+        <v>177</v>
       </c>
       <c r="F281" s="2"/>
     </row>
@@ -6105,7 +6100,7 @@
         <v>Missing</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>397</v>
+        <v>103</v>
       </c>
       <c r="F282" s="2"/>
     </row>
@@ -6121,7 +6116,7 @@
         <v>Missing</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>114</v>
+        <v>185</v>
       </c>
       <c r="F283" s="2"/>
     </row>
@@ -6137,7 +6132,7 @@
         <v>Missing</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>368</v>
+        <v>107</v>
       </c>
       <c r="F284" s="2"/>
     </row>
@@ -6153,7 +6148,7 @@
         <v>Missing</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>200</v>
+        <v>276</v>
       </c>
       <c r="F285" s="2"/>
     </row>
@@ -6169,7 +6164,7 @@
         <v>Missing</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="F286" s="2"/>
     </row>
@@ -6185,7 +6180,7 @@
         <v>Missing</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F287" s="2"/>
     </row>
@@ -6201,7 +6196,7 @@
         <v>Missing</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>15</v>
+        <v>368</v>
       </c>
       <c r="F288" s="2"/>
     </row>
@@ -6217,7 +6212,7 @@
         <v>Missing</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="F289" s="2"/>
     </row>
@@ -6233,7 +6228,7 @@
         <v>Missing</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>127</v>
+        <v>376</v>
       </c>
       <c r="F290" s="2"/>
     </row>
@@ -6249,7 +6244,7 @@
         <v>Missing</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="F291" s="2"/>
     </row>
@@ -6265,7 +6260,7 @@
         <v>Missing</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F292" s="2"/>
     </row>
@@ -6281,7 +6276,7 @@
         <v>Missing</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="F293" s="2"/>
     </row>
@@ -6297,7 +6292,7 @@
         <v>Missing</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F294" s="2"/>
     </row>
@@ -6313,7 +6308,7 @@
         <v>Missing</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="F295" s="2"/>
     </row>
@@ -6329,7 +6324,7 @@
         <v>Missing</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F296" s="2"/>
     </row>
@@ -6345,7 +6340,7 @@
         <v>Missing</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="F297" s="2"/>
     </row>
@@ -6361,7 +6356,7 @@
         <v>Missing</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>334</v>
+        <v>136</v>
       </c>
       <c r="F298" s="2"/>
     </row>
@@ -6377,7 +6372,7 @@
         <v>Missing</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="F299" s="2"/>
     </row>
@@ -6393,7 +6388,7 @@
         <v>Missing</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>162</v>
+        <v>44</v>
       </c>
       <c r="F300" s="2"/>
     </row>
@@ -6409,7 +6404,7 @@
         <v>Missing</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>77</v>
+        <v>244</v>
       </c>
       <c r="F301" s="2"/>
     </row>
@@ -6425,7 +6420,7 @@
         <v>Missing</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>265</v>
+        <v>334</v>
       </c>
       <c r="F302" s="2"/>
     </row>
@@ -6441,7 +6436,7 @@
         <v>Implemented</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>180</v>
+        <v>63</v>
       </c>
       <c r="F303" s="2"/>
     </row>
@@ -6457,7 +6452,7 @@
         <v>Implemented</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>111</v>
+        <v>162</v>
       </c>
       <c r="F304" s="2"/>
     </row>
@@ -6473,7 +6468,7 @@
         <v>Implemented</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>191</v>
+        <v>77</v>
       </c>
       <c r="F305" s="2"/>
     </row>
@@ -6489,7 +6484,7 @@
         <v>Implemented</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>379</v>
+        <v>265</v>
       </c>
       <c r="F306" s="2"/>
     </row>
@@ -6505,7 +6500,7 @@
         <v>Implemented</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>381</v>
+        <v>180</v>
       </c>
       <c r="F307" s="2"/>
     </row>
@@ -6521,7 +6516,7 @@
         <v>Implemented</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="F308" s="2"/>
     </row>
@@ -6537,7 +6532,7 @@
         <v>Implemented</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>137</v>
+        <v>191</v>
       </c>
       <c r="F309" s="2"/>
     </row>
@@ -6553,7 +6548,7 @@
         <v>Implemented</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>151</v>
+        <v>283</v>
       </c>
       <c r="F310" s="2"/>
     </row>
@@ -6569,7 +6564,7 @@
         <v>Implemented</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>245</v>
+        <v>379</v>
       </c>
       <c r="F311" s="2"/>
     </row>
@@ -6585,7 +6580,7 @@
         <v>Implemented</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>198</v>
+        <v>381</v>
       </c>
       <c r="F312" s="2"/>
     </row>
@@ -6601,7 +6596,7 @@
         <v>Implemented</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>394</v>
+        <v>32</v>
       </c>
       <c r="F313" s="2"/>
     </row>
@@ -6617,7 +6612,7 @@
         <v>Implemented</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="F314" s="2"/>
     </row>
@@ -6633,7 +6628,7 @@
         <v>Implemented</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="F315" s="2"/>
     </row>
@@ -6649,7 +6644,7 @@
         <v>Implemented</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>63</v>
+        <v>245</v>
       </c>
       <c r="F316" s="2"/>
     </row>
@@ -6665,7 +6660,7 @@
         <v>Implemented</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>122</v>
+        <v>198</v>
       </c>
       <c r="F317" s="2"/>
     </row>
@@ -6681,7 +6676,7 @@
         <v>Implemented</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>228</v>
+        <v>394</v>
       </c>
       <c r="F318" s="2"/>
     </row>
@@ -6697,7 +6692,7 @@
         <v>Implemented</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="F319" s="2"/>
     </row>
@@ -6713,7 +6708,7 @@
         <v>Implemented</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>173</v>
+        <v>44</v>
       </c>
       <c r="F320" s="2"/>
     </row>
@@ -6729,7 +6724,7 @@
         <v>Implemented</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -6745,7 +6740,7 @@
         <v>Implemented</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6761,7 +6756,7 @@
         <v>Implemented</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6777,7 +6772,7 @@
         <v>Implemented</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="F324" s="2"/>
     </row>
@@ -6793,7 +6788,7 @@
         <v>Implemented</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
@@ -6808,7 +6803,7 @@
         <v>Implemented</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
@@ -6823,7 +6818,7 @@
         <v>Implemented</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -6838,7 +6833,7 @@
         <v>Implemented</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>92</v>
+        <v>203</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
@@ -6852,6 +6847,9 @@
         <f>IF(COUNTIF(D:D,$A329)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D329" s="2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
@@ -6864,6 +6862,9 @@
         <f>IF(COUNTIF(D:D,$A330)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D330" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
@@ -6877,7 +6878,7 @@
         <v>Implemented</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -6892,7 +6893,7 @@
         <v>Implemented</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
@@ -6907,7 +6908,7 @@
         <v>Implemented</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>234</v>
+        <v>92</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
@@ -6921,9 +6922,6 @@
         <f>IF(COUNTIF(D:D,$A334)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D334" s="2" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
@@ -6948,8 +6946,11 @@
         <f>IF(COUNTIF(D:D,$A336)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D336" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>239</v>
       </c>
@@ -6960,8 +6961,11 @@
         <f>IF(COUNTIF(D:D,$A337)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D337" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>399</v>
       </c>
@@ -6972,8 +6976,11 @@
         <f>IF(COUNTIF(D:D,$A338)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D338" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>240</v>
       </c>
@@ -6984,8 +6991,11 @@
         <f>IF(COUNTIF(D:D,$A339)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D339" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>241</v>
       </c>
@@ -6997,7 +7007,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>242</v>
       </c>
@@ -7009,7 +7019,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>243</v>
       </c>
@@ -7021,7 +7031,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>244</v>
       </c>
@@ -7033,7 +7043,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>246</v>
       </c>
@@ -7045,7 +7055,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>247</v>
       </c>
@@ -7057,7 +7067,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>248</v>
       </c>
@@ -7069,7 +7079,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>251</v>
       </c>
@@ -7081,7 +7091,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>252</v>
       </c>
@@ -7093,7 +7103,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>254</v>
       </c>
@@ -7105,7 +7115,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>400</v>
       </c>
@@ -7117,7 +7127,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>256</v>
       </c>
@@ -7129,7 +7139,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>257</v>
       </c>
@@ -7141,7 +7151,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>258</v>
       </c>
@@ -7153,7 +7163,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>259</v>
       </c>
@@ -7165,7 +7175,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>260</v>
       </c>
@@ -7177,7 +7187,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>261</v>
       </c>
@@ -7189,7 +7199,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>262</v>
       </c>
@@ -7201,7 +7211,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>263</v>
       </c>
@@ -7213,7 +7223,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>264</v>
       </c>
@@ -7225,7 +7235,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>265</v>
       </c>
@@ -7237,7 +7247,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>266</v>
       </c>
@@ -7249,7 +7259,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>267</v>
       </c>
@@ -7261,7 +7271,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>268</v>
       </c>
@@ -7273,7 +7283,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>269</v>
       </c>
@@ -7282,10 +7292,10 @@
       </c>
       <c r="C364" t="str">
         <f>IF(COUNTIF(D:D,$A364)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
-      </c>
-    </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+        <v>Implemented</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>270</v>
       </c>
@@ -7297,7 +7307,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>271</v>
       </c>
@@ -7309,7 +7319,7 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>272</v>
       </c>
@@ -7320,11 +7330,8 @@
         <f>IF(COUNTIF(D:D,$A367)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D367" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>273</v>
       </c>
@@ -7334,9 +7341,6 @@
       <c r="C368" t="str">
         <f>IF(COUNTIF(D:D,$A368)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
-      </c>
-      <c r="D368" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -7348,10 +7352,7 @@
       </c>
       <c r="C369" t="str">
         <f>IF(COUNTIF(D:D,$A369)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
-      </c>
-      <c r="D369" s="2" t="s">
-        <v>65</v>
+        <v>Implemented</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7365,9 +7366,6 @@
         <f>IF(COUNTIF(D:D,$A370)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D370" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
@@ -7380,9 +7378,6 @@
         <f>IF(COUNTIF(D:D,$A371)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D371" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
@@ -7396,7 +7391,7 @@
         <v>Implemented</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>54</v>
+        <v>231</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
@@ -7411,7 +7406,7 @@
         <v>Implemented</v>
       </c>
       <c r="D373" s="2" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
@@ -7426,7 +7421,7 @@
         <v>Implemented</v>
       </c>
       <c r="D374" s="2" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -7441,7 +7436,7 @@
         <v>Implemented</v>
       </c>
       <c r="D375" s="2" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -7456,7 +7451,7 @@
         <v>Implemented</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
@@ -7471,7 +7466,7 @@
         <v>Implemented</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>382</v>
+        <v>54</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
@@ -7483,10 +7478,10 @@
       </c>
       <c r="C378" t="str">
         <f>IF(COUNTIF(D:D,$A378)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D378" s="2" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
@@ -7498,10 +7493,10 @@
       </c>
       <c r="C379" t="str">
         <f>IF(COUNTIF(D:D,$A379)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
@@ -7513,10 +7508,10 @@
       </c>
       <c r="C380" t="str">
         <f>IF(COUNTIF(D:D,$A380)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D380" s="2" t="s">
-        <v>253</v>
+        <v>37</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
@@ -7531,7 +7526,7 @@
         <v>Missing</v>
       </c>
       <c r="D381" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
@@ -7543,10 +7538,10 @@
       </c>
       <c r="C382" t="str">
         <f>IF(COUNTIF(D:D,$A382)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D382" s="2" t="s">
-        <v>167</v>
+        <v>382</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
@@ -7561,41 +7556,66 @@
         <v>Implemented</v>
       </c>
       <c r="D383" s="2" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D384" s="2" t="s">
-        <v>155</v>
+        <v>215</v>
       </c>
     </row>
     <row r="385" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D385" s="2" t="s">
-        <v>227</v>
+        <v>253</v>
       </c>
     </row>
     <row r="386" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D386" s="2" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
     </row>
     <row r="387" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D387" s="2" t="s">
-        <v>123</v>
+        <v>167</v>
       </c>
     </row>
     <row r="388" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D388" s="2" t="s">
-        <v>238</v>
+        <v>43</v>
       </c>
     </row>
     <row r="389" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D389" s="2" t="s">
-        <v>366</v>
+        <v>155</v>
       </c>
     </row>
     <row r="390" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D390" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="391" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D391" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="392" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D392" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="393" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D393" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="394" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D394" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="395" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D395" s="2" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- refactored ChooseOne Mechanic of Druid to be exactly consistent with in-game behaviour (there are now either two separate cards or a separate Battlecry) - implemented the following epic cards: Ancient of Lore, Ancient of War, Avenging Wrath and Bane of Doom
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$312</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$317</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="401">
   <si>
     <t>Cardname</t>
   </si>
@@ -1605,9 +1605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K395"/>
+  <dimension ref="A1:K400"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A370" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1652,7 +1654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>223</v>
+        <v>289</v>
       </c>
       <c r="F2" s="2"/>
       <c r="J2" t="s">
@@ -1675,7 +1677,7 @@
         <v>Implemented</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>290</v>
       </c>
       <c r="F3" s="2"/>
       <c r="J3" t="s">
@@ -1698,7 +1700,7 @@
         <v>Implemented</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>144</v>
+        <v>223</v>
       </c>
       <c r="F4" s="2"/>
       <c r="J4" t="s">
@@ -1721,7 +1723,7 @@
         <v>Implemented</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2"/>
       <c r="J5" t="s">
@@ -1744,7 +1746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="F6" s="2"/>
       <c r="J6" s="1" t="s">
@@ -1767,7 +1769,7 @@
         <v>Implemented</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1783,7 +1785,7 @@
         <v>Implemented</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>251</v>
+        <v>71</v>
       </c>
       <c r="F8" s="2"/>
       <c r="J8" t="s">
@@ -1791,7 +1793,7 @@
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1806,7 +1808,7 @@
         <v>Implemented</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>171</v>
+        <v>72</v>
       </c>
       <c r="F9" s="2"/>
       <c r="J9" t="s">
@@ -1814,7 +1816,7 @@
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1829,7 +1831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>81</v>
+        <v>251</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1845,7 +1847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1861,7 +1863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>174</v>
+        <v>81</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -1877,7 +1879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>267</v>
+        <v>86</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -1893,7 +1895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1909,7 +1911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>105</v>
+        <v>267</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1925,7 +1927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>272</v>
+        <v>176</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -1941,7 +1943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>194</v>
+        <v>105</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1957,7 +1959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -1973,7 +1975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>363</v>
+        <v>194</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1989,7 +1991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>369</v>
+        <v>279</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -2005,7 +2007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -2021,7 +2023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>211</v>
+        <v>369</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -2037,7 +2039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>10</v>
+        <v>382</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -2053,7 +2055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -2069,7 +2071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -2085,7 +2087,7 @@
         <v>Implemented</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>237</v>
+        <v>14</v>
       </c>
       <c r="F26" s="2"/>
     </row>
@@ -2101,7 +2103,7 @@
         <v>Implemented</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>240</v>
+        <v>139</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -2117,7 +2119,7 @@
         <v>Implemented</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -2133,7 +2135,7 @@
         <v>Implemented</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -2149,7 +2151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F30" s="2"/>
     </row>
@@ -2165,7 +2167,7 @@
         <v>Implemented</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>68</v>
+        <v>243</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -2181,7 +2183,7 @@
         <v>Implemented</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -2197,7 +2199,7 @@
         <v>Implemented</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -2213,7 +2215,7 @@
         <v>Implemented</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>264</v>
+        <v>70</v>
       </c>
       <c r="F34" s="2"/>
     </row>
@@ -2229,7 +2231,7 @@
         <v>Implemented</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -2245,7 +2247,7 @@
         <v>Implemented</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="F36" s="2"/>
     </row>
@@ -2261,7 +2263,7 @@
         <v>Implemented</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>184</v>
+        <v>88</v>
       </c>
       <c r="F37" s="2"/>
     </row>
@@ -2277,7 +2279,7 @@
         <v>Implemented</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>321</v>
+        <v>273</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -2293,7 +2295,7 @@
         <v>Implemented</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -2309,7 +2311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>364</v>
+        <v>321</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -2325,7 +2327,7 @@
         <v>Implemented</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>370</v>
+        <v>192</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -2341,7 +2343,7 @@
         <v>Implemented</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -2357,7 +2359,7 @@
         <v>Implemented</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -2373,7 +2375,7 @@
         <v>Implemented</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>206</v>
+        <v>372</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -2389,7 +2391,7 @@
         <v>Implemented</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>11</v>
+        <v>374</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -2405,7 +2407,7 @@
         <v>Implemented</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>12</v>
+        <v>206</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -2421,7 +2423,7 @@
         <v>Implemented</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -2437,7 +2439,7 @@
         <v>Implemented</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>226</v>
+        <v>12</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -2453,7 +2455,7 @@
         <v>Implemented</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>135</v>
+        <v>13</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -2469,7 +2471,7 @@
         <v>Implemented</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -2485,7 +2487,7 @@
         <v>Implemented</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>399</v>
+        <v>135</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -2501,7 +2503,7 @@
         <v>Implemented</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>46</v>
+        <v>231</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -2517,7 +2519,7 @@
         <v>Implemented</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>47</v>
+        <v>399</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -2533,7 +2535,7 @@
         <v>Implemented</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -2549,7 +2551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -2565,7 +2567,7 @@
         <v>Implemented</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="F56" s="2"/>
     </row>
@@ -2581,7 +2583,7 @@
         <v>Implemented</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>160</v>
+        <v>49</v>
       </c>
       <c r="F57" s="2"/>
     </row>
@@ -2597,7 +2599,7 @@
         <v>Implemented</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>252</v>
+        <v>159</v>
       </c>
       <c r="F58" s="2"/>
     </row>
@@ -2613,7 +2615,7 @@
         <v>Implemented</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -2629,7 +2631,7 @@
         <v>Implemented</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>172</v>
+        <v>252</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -2645,7 +2647,7 @@
         <v>Implemented</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -2661,7 +2663,7 @@
         <v>Implemented</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="F62" s="2"/>
     </row>
@@ -2677,7 +2679,7 @@
         <v>Implemented</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>317</v>
+        <v>85</v>
       </c>
       <c r="F63" s="2"/>
     </row>
@@ -2693,7 +2695,7 @@
         <v>Implemented</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>193</v>
+        <v>96</v>
       </c>
       <c r="F64" s="2"/>
     </row>
@@ -2709,7 +2711,7 @@
         <v>Implemented</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="F65" s="2"/>
     </row>
@@ -2725,7 +2727,7 @@
         <v>Implemented</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>284</v>
+        <v>193</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -2741,7 +2743,7 @@
         <v>Implemented</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>380</v>
+        <v>323</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -2757,7 +2759,7 @@
         <v>Implemented</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>115</v>
+        <v>284</v>
       </c>
       <c r="F68" s="2"/>
     </row>
@@ -2773,7 +2775,7 @@
         <v>Implemented</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>121</v>
+        <v>380</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -2789,7 +2791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="F70" s="2"/>
     </row>
@@ -2805,7 +2807,7 @@
         <v>Implemented</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F71" s="2"/>
     </row>
@@ -2821,7 +2823,7 @@
         <v>Implemented</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>398</v>
+        <v>3</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -2837,7 +2839,7 @@
         <v>Implemented</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F73" s="2"/>
     </row>
@@ -2853,7 +2855,7 @@
         <v>Implemented</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>123</v>
+        <v>398</v>
       </c>
       <c r="F74" s="2"/>
     </row>
@@ -2869,7 +2871,7 @@
         <v>Implemented</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>215</v>
+        <v>120</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -2885,7 +2887,7 @@
         <v>Implemented</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>216</v>
+        <v>123</v>
       </c>
       <c r="F76" s="2"/>
     </row>
@@ -2901,7 +2903,7 @@
         <v>Implemented</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F77" s="2"/>
     </row>
@@ -2917,7 +2919,7 @@
         <v>Implemented</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F78" s="2"/>
     </row>
@@ -2933,7 +2935,7 @@
         <v>Implemented</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="F79" s="2"/>
     </row>
@@ -2949,7 +2951,7 @@
         <v>Implemented</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F80" s="2"/>
     </row>
@@ -2965,7 +2967,7 @@
         <v>Implemented</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="F81" s="2"/>
     </row>
@@ -2981,7 +2983,7 @@
         <v>Implemented</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F82" s="2"/>
     </row>
@@ -2997,7 +2999,7 @@
         <v>Implemented</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="F83" s="2"/>
     </row>
@@ -3013,7 +3015,7 @@
         <v>Implemented</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F84" s="2"/>
     </row>
@@ -3029,7 +3031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="F85" s="2"/>
     </row>
@@ -3045,7 +3047,7 @@
         <v>Implemented</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>24</v>
+        <v>227</v>
       </c>
       <c r="F86" s="2"/>
     </row>
@@ -3061,7 +3063,7 @@
         <v>Implemented</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>25</v>
+        <v>131</v>
       </c>
       <c r="F87" s="2"/>
     </row>
@@ -3077,7 +3079,7 @@
         <v>Implemented</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F88" s="2"/>
     </row>
@@ -3093,7 +3095,7 @@
         <v>Implemented</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F89" s="2"/>
     </row>
@@ -3109,7 +3111,7 @@
         <v>Implemented</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>228</v>
+        <v>26</v>
       </c>
       <c r="F90" s="2"/>
     </row>
@@ -3125,7 +3127,7 @@
         <v>Implemented</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>229</v>
+        <v>28</v>
       </c>
       <c r="F91" s="2"/>
     </row>
@@ -3141,7 +3143,7 @@
         <v>Implemented</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
       <c r="F92" s="2"/>
     </row>
@@ -3157,7 +3159,7 @@
         <v>Implemented</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F93" s="2"/>
     </row>
@@ -3173,7 +3175,7 @@
         <v>Implemented</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="F94" s="2"/>
     </row>
@@ -3189,7 +3191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>34</v>
+        <v>232</v>
       </c>
       <c r="F95" s="2"/>
     </row>
@@ -3205,7 +3207,7 @@
         <v>Implemented</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F96" s="2"/>
     </row>
@@ -3221,7 +3223,7 @@
         <v>Implemented</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F97" s="2"/>
     </row>
@@ -3234,10 +3236,10 @@
       </c>
       <c r="C98" t="str">
         <f>IF(COUNTIF(D:D,$A98)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>233</v>
+        <v>138</v>
       </c>
       <c r="F98" s="2"/>
     </row>
@@ -3250,10 +3252,10 @@
       </c>
       <c r="C99" t="str">
         <f>IF(COUNTIF(D:D,$A99)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>234</v>
+        <v>35</v>
       </c>
       <c r="F99" s="2"/>
     </row>
@@ -3266,10 +3268,10 @@
       </c>
       <c r="C100" t="str">
         <f>IF(COUNTIF(D:D,$A100)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>142</v>
+        <v>233</v>
       </c>
       <c r="F100" s="2"/>
     </row>
@@ -3282,10 +3284,10 @@
       </c>
       <c r="C101" t="str">
         <f>IF(COUNTIF(D:D,$A101)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>38</v>
+        <v>234</v>
       </c>
       <c r="F101" s="2"/>
     </row>
@@ -3301,7 +3303,7 @@
         <v>Missing</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F102" s="2"/>
     </row>
@@ -3317,7 +3319,7 @@
         <v>Missing</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="F103" s="2"/>
     </row>
@@ -3333,7 +3335,7 @@
         <v>Missing</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="F104" s="2"/>
     </row>
@@ -3349,7 +3351,7 @@
         <v>Missing</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>238</v>
+        <v>147</v>
       </c>
       <c r="F105" s="2"/>
     </row>
@@ -3365,7 +3367,7 @@
         <v>Missing</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="F106" s="2"/>
     </row>
@@ -3381,7 +3383,7 @@
         <v>Missing</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="F107" s="2"/>
     </row>
@@ -3397,7 +3399,7 @@
         <v>Missing</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F108" s="2"/>
     </row>
@@ -3413,7 +3415,7 @@
         <v>Missing</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F109" s="2"/>
     </row>
@@ -3429,7 +3431,7 @@
         <v>Missing</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>52</v>
+        <v>154</v>
       </c>
       <c r="F110" s="2"/>
     </row>
@@ -3445,7 +3447,7 @@
         <v>Missing</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>53</v>
+        <v>157</v>
       </c>
       <c r="F111" s="2"/>
     </row>
@@ -3461,7 +3463,7 @@
         <v>Missing</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>245</v>
+        <v>52</v>
       </c>
       <c r="F112" s="2"/>
     </row>
@@ -3477,7 +3479,7 @@
         <v>Missing</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F113" s="2"/>
     </row>
@@ -3493,7 +3495,7 @@
         <v>Missing</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>55</v>
+        <v>245</v>
       </c>
       <c r="F114" s="2"/>
     </row>
@@ -3509,7 +3511,7 @@
         <v>Missing</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F115" s="2"/>
     </row>
@@ -3525,7 +3527,7 @@
         <v>Missing</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F116" s="2"/>
     </row>
@@ -3541,7 +3543,7 @@
         <v>Missing</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>158</v>
+        <v>56</v>
       </c>
       <c r="F117" s="2"/>
     </row>
@@ -3557,7 +3559,7 @@
         <v>Missing</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>249</v>
+        <v>58</v>
       </c>
       <c r="F118" s="2"/>
     </row>
@@ -3573,7 +3575,7 @@
         <v>Missing</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>250</v>
+        <v>158</v>
       </c>
       <c r="F119" s="2"/>
     </row>
@@ -3589,7 +3591,7 @@
         <v>Missing</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>163</v>
+        <v>249</v>
       </c>
       <c r="F120" s="2"/>
     </row>
@@ -3605,7 +3607,7 @@
         <v>Missing</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="F121" s="2"/>
     </row>
@@ -3621,7 +3623,7 @@
         <v>Missing</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="F122" s="2"/>
     </row>
@@ -3637,7 +3639,7 @@
         <v>Missing</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>164</v>
+        <v>73</v>
       </c>
       <c r="F123" s="2"/>
     </row>
@@ -3653,7 +3655,7 @@
         <v>Missing</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>253</v>
+        <v>74</v>
       </c>
       <c r="F124" s="2"/>
     </row>
@@ -3669,7 +3671,7 @@
         <v>Missing</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="F125" s="2"/>
     </row>
@@ -3685,7 +3687,7 @@
         <v>Missing</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>165</v>
+        <v>253</v>
       </c>
       <c r="F126" s="2"/>
     </row>
@@ -3701,7 +3703,7 @@
         <v>Missing</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>255</v>
+        <v>76</v>
       </c>
       <c r="F127" s="2"/>
     </row>
@@ -3717,7 +3719,7 @@
         <v>Missing</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F128" s="2"/>
     </row>
@@ -3733,7 +3735,7 @@
         <v>Missing</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>79</v>
+        <v>255</v>
       </c>
       <c r="F129" s="2"/>
     </row>
@@ -3749,7 +3751,7 @@
         <v>Missing</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F130" s="2"/>
     </row>
@@ -3765,7 +3767,7 @@
         <v>Implemented</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F131" s="2"/>
     </row>
@@ -3781,7 +3783,7 @@
         <v>Missing</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>257</v>
+        <v>169</v>
       </c>
       <c r="F132" s="2"/>
     </row>
@@ -3797,7 +3799,7 @@
         <v>Missing</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>259</v>
+        <v>80</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -3813,7 +3815,7 @@
         <v>Implemented</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F134" s="2"/>
     </row>
@@ -3829,7 +3831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F135" s="2"/>
     </row>
@@ -3845,7 +3847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>173</v>
+        <v>262</v>
       </c>
       <c r="F136" s="2"/>
     </row>
@@ -3861,7 +3863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>89</v>
+        <v>263</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -3877,7 +3879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>266</v>
+        <v>173</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -3893,7 +3895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -3909,7 +3911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>91</v>
+        <v>266</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -3925,7 +3927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -3941,7 +3943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -3957,7 +3959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F143" s="2"/>
     </row>
@@ -3973,7 +3975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>269</v>
+        <v>94</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -3989,7 +3991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>178</v>
+        <v>95</v>
       </c>
       <c r="F145" s="2"/>
     </row>
@@ -4005,7 +4007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F146" s="2"/>
     </row>
@@ -4021,7 +4023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4037,7 +4039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>98</v>
+        <v>270</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4053,7 +4055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>271</v>
+        <v>179</v>
       </c>
       <c r="F149" s="2"/>
     </row>
@@ -4069,7 +4071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4084,7 +4086,7 @@
         <v>Implemented</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>100</v>
+        <v>271</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4099,7 +4101,7 @@
         <v>Implemented</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4114,7 +4116,7 @@
         <v>Implemented</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>183</v>
+        <v>100</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4129,7 +4131,7 @@
         <v>Implemented</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>274</v>
+        <v>101</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4144,7 +4146,7 @@
         <v>Implemented</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>106</v>
+        <v>183</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4159,7 +4161,7 @@
         <v>Implemented</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>110</v>
+        <v>274</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4174,7 +4176,7 @@
         <v>Implemented</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>187</v>
+        <v>106</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4189,7 +4191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>392</v>
+        <v>110</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4204,7 +4206,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4219,7 +4221,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>190</v>
+        <v>392</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4234,7 +4236,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4249,7 +4251,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4264,7 +4266,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4279,7 +4281,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>278</v>
+        <v>196</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4294,7 +4296,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>365</v>
+        <v>197</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4309,7 +4311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>366</v>
+        <v>278</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4324,7 +4326,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4339,7 +4341,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>393</v>
+        <v>366</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4354,7 +4356,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>199</v>
+        <v>367</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4369,7 +4371,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>280</v>
+        <v>393</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4384,7 +4386,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>281</v>
+        <v>199</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4399,7 +4401,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>201</v>
+        <v>280</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4414,7 +4416,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>204</v>
+        <v>281</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4429,7 +4431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>282</v>
+        <v>201</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4444,7 +4446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4459,7 +4461,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4474,7 +4476,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>377</v>
+        <v>207</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4489,7 +4491,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>378</v>
+        <v>285</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4504,7 +4506,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>287</v>
+        <v>377</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4519,7 +4521,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>208</v>
+        <v>378</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4534,7 +4536,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>209</v>
+        <v>287</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4549,7 +4551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>385</v>
+        <v>208</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4564,7 +4566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4579,7 +4581,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>212</v>
+        <v>385</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4594,7 +4596,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>288</v>
+        <v>210</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4609,7 +4611,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4624,7 +4626,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>118</v>
+        <v>288</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4639,7 +4641,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>125</v>
+        <v>213</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4654,7 +4656,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>225</v>
+        <v>118</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4669,7 +4671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4684,7 +4686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>21</v>
+        <v>291</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4699,7 +4701,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>129</v>
+        <v>225</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4714,7 +4716,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4729,7 +4731,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>235</v>
+        <v>21</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4744,7 +4746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>239</v>
+        <v>129</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4759,7 +4761,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>150</v>
+        <v>31</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4774,7 +4776,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>57</v>
+        <v>235</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4789,7 +4791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>59</v>
+        <v>239</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4804,7 +4806,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>60</v>
+        <v>150</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4819,7 +4821,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4834,7 +4836,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>248</v>
+        <v>59</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4849,7 +4851,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4864,7 +4866,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4879,7 +4881,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>175</v>
+        <v>248</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4894,7 +4896,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>181</v>
+        <v>69</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4909,7 +4911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>182</v>
+        <v>78</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4924,7 +4926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>373</v>
+        <v>175</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4939,7 +4941,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>221</v>
+        <v>181</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4954,7 +4956,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>132</v>
+        <v>182</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4969,7 +4971,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>37</v>
+        <v>373</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4984,7 +4986,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -4999,7 +5001,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5014,7 +5016,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5029,7 +5031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>161</v>
+        <v>247</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5044,7 +5046,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>167</v>
+        <v>66</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5059,7 +5061,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>256</v>
+        <v>67</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5074,7 +5076,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>260</v>
+        <v>161</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5089,7 +5091,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>82</v>
+        <v>167</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5104,7 +5106,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>83</v>
+        <v>256</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5119,7 +5121,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>84</v>
+        <v>260</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5134,7 +5136,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5149,7 +5151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5164,7 +5166,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>275</v>
+        <v>84</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5179,7 +5181,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5194,7 +5196,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5209,7 +5211,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>188</v>
+        <v>275</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5224,7 +5226,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>202</v>
+        <v>108</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5239,7 +5241,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>203</v>
+        <v>109</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5254,7 +5256,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>18</v>
+        <v>188</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5269,7 +5271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>17</v>
+        <v>202</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5284,7 +5286,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>19</v>
+        <v>203</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5300,7 +5302,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>128</v>
+        <v>18</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5316,7 +5318,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>224</v>
+        <v>17</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5332,7 +5334,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>133</v>
+        <v>19</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5348,7 +5350,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5364,7 +5366,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>36</v>
+        <v>224</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5380,7 +5382,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5396,7 +5398,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5412,7 +5414,7 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5428,7 +5430,7 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>246</v>
+        <v>140</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5444,7 +5446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>261</v>
+        <v>148</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5460,7 +5462,7 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>268</v>
+        <v>43</v>
       </c>
       <c r="F242" s="2"/>
     </row>
@@ -5476,7 +5478,7 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>104</v>
+        <v>246</v>
       </c>
       <c r="F243" s="2"/>
     </row>
@@ -5492,7 +5494,7 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>186</v>
+        <v>261</v>
       </c>
       <c r="F244" s="2"/>
     </row>
@@ -5508,7 +5510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>112</v>
+        <v>268</v>
       </c>
       <c r="F245" s="2"/>
     </row>
@@ -5524,7 +5526,7 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>277</v>
+        <v>104</v>
       </c>
       <c r="F246" s="2"/>
     </row>
@@ -5540,7 +5542,7 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
       <c r="F247" s="2"/>
     </row>
@@ -5556,7 +5558,7 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>362</v>
+        <v>112</v>
       </c>
       <c r="F248" s="2"/>
     </row>
@@ -5572,7 +5574,7 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>375</v>
+        <v>277</v>
       </c>
       <c r="F249" s="2"/>
     </row>
@@ -5588,7 +5590,7 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5604,7 +5606,7 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>214</v>
+        <v>362</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5620,7 +5622,7 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>23</v>
+        <v>375</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5636,7 +5638,7 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>145</v>
+        <v>9</v>
       </c>
       <c r="F253" s="2"/>
     </row>
@@ -5652,7 +5654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>146</v>
+        <v>214</v>
       </c>
       <c r="F254" s="2"/>
     </row>
@@ -5668,7 +5670,7 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>242</v>
+        <v>23</v>
       </c>
       <c r="F255" s="2"/>
     </row>
@@ -5684,7 +5686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="F256" s="2"/>
     </row>
@@ -5700,7 +5702,7 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>48</v>
+        <v>146</v>
       </c>
       <c r="F257" s="2"/>
     </row>
@@ -5716,7 +5718,7 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>155</v>
+        <v>242</v>
       </c>
       <c r="F258" s="2"/>
     </row>
@@ -5732,7 +5734,7 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F259" s="2"/>
     </row>
@@ -5748,7 +5750,7 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F260" s="2"/>
     </row>
@@ -5764,7 +5766,7 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>254</v>
+        <v>155</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -5780,7 +5782,7 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>166</v>
+        <v>50</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -5796,7 +5798,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>400</v>
+        <v>64</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5812,7 +5814,7 @@
         <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F264" s="2"/>
     </row>
@@ -5828,7 +5830,7 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
       <c r="F265" s="2"/>
     </row>
@@ -5844,7 +5846,7 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>198</v>
+        <v>400</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -5860,7 +5862,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>371</v>
+        <v>258</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5876,7 +5878,7 @@
         <v>Missing</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>205</v>
+        <v>102</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5892,7 +5894,7 @@
         <v>Missing</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>383</v>
+        <v>198</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -5908,7 +5910,7 @@
         <v>Missing</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -5924,7 +5926,7 @@
         <v>Missing</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>130</v>
+        <v>205</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -5940,7 +5942,7 @@
         <v>Missing</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>33</v>
+        <v>383</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -5956,7 +5958,7 @@
         <v>Missing</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>141</v>
+        <v>384</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -5972,7 +5974,7 @@
         <v>Missing</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>236</v>
+        <v>292</v>
       </c>
       <c r="F274" s="2"/>
     </row>
@@ -5988,7 +5990,7 @@
         <v>Missing</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="F275" s="2"/>
     </row>
@@ -6004,7 +6006,7 @@
         <v>Missing</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F276" s="2"/>
     </row>
@@ -6020,7 +6022,7 @@
         <v>Missing</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>241</v>
+        <v>141</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -6036,7 +6038,7 @@
         <v>Missing</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>153</v>
+        <v>236</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -6052,7 +6054,7 @@
         <v>Missing</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="F279" s="2"/>
     </row>
@@ -6068,7 +6070,7 @@
         <v>Missing</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="F280" s="2"/>
     </row>
@@ -6084,7 +6086,7 @@
         <v>Missing</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F281" s="2"/>
     </row>
@@ -6100,7 +6102,7 @@
         <v>Missing</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="F282" s="2"/>
     </row>
@@ -6116,7 +6118,7 @@
         <v>Missing</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>185</v>
+        <v>62</v>
       </c>
       <c r="F283" s="2"/>
     </row>
@@ -6132,7 +6134,7 @@
         <v>Missing</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="F284" s="2"/>
     </row>
@@ -6148,7 +6150,7 @@
         <v>Missing</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>276</v>
+        <v>177</v>
       </c>
       <c r="F285" s="2"/>
     </row>
@@ -6164,7 +6166,7 @@
         <v>Missing</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>397</v>
+        <v>103</v>
       </c>
       <c r="F286" s="2"/>
     </row>
@@ -6180,7 +6182,7 @@
         <v>Missing</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>114</v>
+        <v>185</v>
       </c>
       <c r="F287" s="2"/>
     </row>
@@ -6196,7 +6198,7 @@
         <v>Missing</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>368</v>
+        <v>107</v>
       </c>
       <c r="F288" s="2"/>
     </row>
@@ -6212,7 +6214,7 @@
         <v>Missing</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>200</v>
+        <v>276</v>
       </c>
       <c r="F289" s="2"/>
     </row>
@@ -6228,7 +6230,7 @@
         <v>Missing</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="F290" s="2"/>
     </row>
@@ -6244,7 +6246,7 @@
         <v>Missing</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F291" s="2"/>
     </row>
@@ -6260,7 +6262,7 @@
         <v>Missing</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>15</v>
+        <v>368</v>
       </c>
       <c r="F292" s="2"/>
     </row>
@@ -6276,7 +6278,7 @@
         <v>Missing</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="F293" s="2"/>
     </row>
@@ -6292,7 +6294,7 @@
         <v>Missing</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>127</v>
+        <v>286</v>
       </c>
       <c r="F294" s="2"/>
     </row>
@@ -6308,7 +6310,7 @@
         <v>Missing</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>27</v>
+        <v>376</v>
       </c>
       <c r="F295" s="2"/>
     </row>
@@ -6324,7 +6326,7 @@
         <v>Missing</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="F296" s="2"/>
     </row>
@@ -6340,7 +6342,7 @@
         <v>Missing</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>230</v>
+        <v>15</v>
       </c>
       <c r="F297" s="2"/>
     </row>
@@ -6356,7 +6358,7 @@
         <v>Missing</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>136</v>
+        <v>220</v>
       </c>
       <c r="F298" s="2"/>
     </row>
@@ -6372,7 +6374,7 @@
         <v>Missing</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>42</v>
+        <v>127</v>
       </c>
       <c r="F299" s="2"/>
     </row>
@@ -6388,7 +6390,7 @@
         <v>Missing</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F300" s="2"/>
     </row>
@@ -6404,7 +6406,7 @@
         <v>Missing</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>244</v>
+        <v>30</v>
       </c>
       <c r="F301" s="2"/>
     </row>
@@ -6420,7 +6422,7 @@
         <v>Missing</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>334</v>
+        <v>230</v>
       </c>
       <c r="F302" s="2"/>
     </row>
@@ -6436,7 +6438,7 @@
         <v>Implemented</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="F303" s="2"/>
     </row>
@@ -6452,7 +6454,7 @@
         <v>Implemented</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
       <c r="F304" s="2"/>
     </row>
@@ -6468,7 +6470,7 @@
         <v>Implemented</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="F305" s="2"/>
     </row>
@@ -6484,7 +6486,7 @@
         <v>Implemented</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="F306" s="2"/>
     </row>
@@ -6500,7 +6502,7 @@
         <v>Implemented</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>180</v>
+        <v>334</v>
       </c>
       <c r="F307" s="2"/>
     </row>
@@ -6516,7 +6518,7 @@
         <v>Implemented</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="F308" s="2"/>
     </row>
@@ -6532,7 +6534,7 @@
         <v>Implemented</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
       <c r="F309" s="2"/>
     </row>
@@ -6548,7 +6550,7 @@
         <v>Implemented</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>283</v>
+        <v>77</v>
       </c>
       <c r="F310" s="2"/>
     </row>
@@ -6564,7 +6566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>379</v>
+        <v>265</v>
       </c>
       <c r="F311" s="2"/>
     </row>
@@ -6580,7 +6582,7 @@
         <v>Implemented</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>381</v>
+        <v>180</v>
       </c>
       <c r="F312" s="2"/>
     </row>
@@ -6596,7 +6598,7 @@
         <v>Implemented</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="F313" s="2"/>
     </row>
@@ -6612,7 +6614,7 @@
         <v>Implemented</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>137</v>
+        <v>191</v>
       </c>
       <c r="F314" s="2"/>
     </row>
@@ -6628,7 +6630,7 @@
         <v>Implemented</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>151</v>
+        <v>283</v>
       </c>
       <c r="F315" s="2"/>
     </row>
@@ -6644,7 +6646,7 @@
         <v>Implemented</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>245</v>
+        <v>379</v>
       </c>
       <c r="F316" s="2"/>
     </row>
@@ -6660,7 +6662,7 @@
         <v>Implemented</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>198</v>
+        <v>381</v>
       </c>
       <c r="F317" s="2"/>
     </row>
@@ -6676,7 +6678,7 @@
         <v>Implemented</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>394</v>
+        <v>32</v>
       </c>
       <c r="F318" s="2"/>
     </row>
@@ -6692,7 +6694,7 @@
         <v>Implemented</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="F319" s="2"/>
     </row>
@@ -6708,7 +6710,7 @@
         <v>Implemented</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="F320" s="2"/>
     </row>
@@ -6724,7 +6726,7 @@
         <v>Implemented</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>63</v>
+        <v>245</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -6740,7 +6742,7 @@
         <v>Implemented</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>122</v>
+        <v>198</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6756,7 +6758,7 @@
         <v>Implemented</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>228</v>
+        <v>394</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6772,7 +6774,7 @@
         <v>Implemented</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="F324" s="2"/>
     </row>
@@ -6788,7 +6790,7 @@
         <v>Implemented</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>173</v>
+        <v>44</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
@@ -6803,7 +6805,7 @@
         <v>Implemented</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
@@ -6818,7 +6820,7 @@
         <v>Implemented</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -6833,7 +6835,7 @@
         <v>Implemented</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
@@ -6848,7 +6850,7 @@
         <v>Implemented</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -6863,7 +6865,7 @@
         <v>Implemented</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
@@ -6878,7 +6880,7 @@
         <v>Implemented</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -6893,7 +6895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
@@ -6908,7 +6910,7 @@
         <v>Implemented</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>92</v>
+        <v>203</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
@@ -6922,6 +6924,9 @@
         <f>IF(COUNTIF(D:D,$A334)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D334" s="2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
@@ -6934,6 +6939,9 @@
         <f>IF(COUNTIF(D:D,$A335)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D335" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
@@ -6947,7 +6955,7 @@
         <v>Implemented</v>
       </c>
       <c r="D336" s="2" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -6962,7 +6970,7 @@
         <v>Implemented</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -6977,7 +6985,7 @@
         <v>Implemented</v>
       </c>
       <c r="D338" s="2" t="s">
-        <v>234</v>
+        <v>92</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -6991,9 +6999,6 @@
         <f>IF(COUNTIF(D:D,$A339)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D339" s="2" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
@@ -7018,6 +7023,9 @@
         <f>IF(COUNTIF(D:D,$A341)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D341" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
@@ -7030,6 +7038,9 @@
         <f>IF(COUNTIF(D:D,$A342)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D342" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
@@ -7042,6 +7053,9 @@
         <f>IF(COUNTIF(D:D,$A343)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D343" s="2" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
@@ -7054,6 +7068,9 @@
         <f>IF(COUNTIF(D:D,$A344)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D344" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
@@ -7390,9 +7407,6 @@
         <f>IF(COUNTIF(D:D,$A372)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D372" s="2" t="s">
-        <v>231</v>
-      </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
@@ -7405,9 +7419,6 @@
         <f>IF(COUNTIF(D:D,$A373)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D373" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
@@ -7420,9 +7431,6 @@
         <f>IF(COUNTIF(D:D,$A374)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D374" s="2" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
@@ -7435,9 +7443,6 @@
         <f>IF(COUNTIF(D:D,$A375)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D375" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
@@ -7450,9 +7455,6 @@
         <f>IF(COUNTIF(D:D,$A376)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D376" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
@@ -7466,7 +7468,7 @@
         <v>Implemented</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>54</v>
+        <v>231</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
@@ -7481,7 +7483,7 @@
         <v>Implemented</v>
       </c>
       <c r="D378" s="2" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
@@ -7496,7 +7498,7 @@
         <v>Implemented</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
@@ -7511,7 +7513,7 @@
         <v>Implemented</v>
       </c>
       <c r="D380" s="2" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
@@ -7523,10 +7525,10 @@
       </c>
       <c r="C381" t="str">
         <f>IF(COUNTIF(D:D,$A381)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D381" s="2" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
@@ -7541,7 +7543,7 @@
         <v>Implemented</v>
       </c>
       <c r="D382" s="2" t="s">
-        <v>382</v>
+        <v>54</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
@@ -7556,66 +7558,91 @@
         <v>Implemented</v>
       </c>
       <c r="D383" s="2" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D384" s="2" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
     </row>
     <row r="385" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D385" s="2" t="s">
-        <v>253</v>
+        <v>37</v>
       </c>
     </row>
     <row r="386" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D386" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="387" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D387" s="2" t="s">
-        <v>167</v>
+        <v>382</v>
       </c>
     </row>
     <row r="388" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D388" s="2" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
     </row>
     <row r="389" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D389" s="2" t="s">
-        <v>155</v>
+        <v>215</v>
       </c>
     </row>
     <row r="390" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D390" s="2" t="s">
-        <v>227</v>
+        <v>253</v>
       </c>
     </row>
     <row r="391" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D391" s="2" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
     </row>
     <row r="392" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D392" s="2" t="s">
-        <v>123</v>
+        <v>167</v>
       </c>
     </row>
     <row r="393" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D393" s="2" t="s">
-        <v>238</v>
+        <v>43</v>
       </c>
     </row>
     <row r="394" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D394" s="2" t="s">
-        <v>366</v>
+        <v>155</v>
       </c>
     </row>
     <row r="395" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D395" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="396" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D396" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="397" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D397" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="398" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D398" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="399" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D399" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="400" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D400" s="2" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- implemented the following epic cards: Ice Block, Hungry Crab, Molten Giant, Mountain Giant, Murloc Warleader, Sea Giant, Southsea Captain, Lay on Hands, Sword of Justice, Mindgames, Shadowform, Kidnapper, Patient Assassin, Preparation, Pit Lord, Twisting Nether, Shield Slam
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$317</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$348</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="401">
   <si>
     <t>Cardname</t>
   </si>
@@ -1605,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K400"/>
+  <dimension ref="A1:K431"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A370" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,7 +1769,7 @@
         <v>Implemented</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>61</v>
+        <v>303</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1785,7 +1785,7 @@
         <v>Implemented</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F8" s="2"/>
       <c r="J8" t="s">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>316</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
         <v>Implemented</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="2"/>
       <c r="J9" t="s">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>66</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1831,7 +1831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>251</v>
+        <v>72</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1847,7 +1847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>171</v>
+        <v>251</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1863,7 +1863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>81</v>
+        <v>171</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -1879,7 +1879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -1895,7 +1895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>174</v>
+        <v>86</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1911,7 +1911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>267</v>
+        <v>174</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1927,7 +1927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>176</v>
+        <v>267</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -1943,7 +1943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>105</v>
+        <v>176</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1959,7 +1959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>272</v>
+        <v>105</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -1975,7 +1975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>194</v>
+        <v>272</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1991,7 +1991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -2007,7 +2007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>363</v>
+        <v>279</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -2023,7 +2023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -2039,7 +2039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -2055,7 +2055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>211</v>
+        <v>382</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -2071,7 +2071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>10</v>
+        <v>211</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -2087,7 +2087,7 @@
         <v>Implemented</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F26" s="2"/>
     </row>
@@ -2103,7 +2103,7 @@
         <v>Implemented</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -2119,7 +2119,7 @@
         <v>Implemented</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>237</v>
+        <v>293</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -2135,7 +2135,7 @@
         <v>Implemented</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>240</v>
+        <v>139</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -2151,7 +2151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="F30" s="2"/>
     </row>
@@ -2167,7 +2167,7 @@
         <v>Implemented</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -2183,7 +2183,7 @@
         <v>Implemented</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -2199,7 +2199,7 @@
         <v>Implemented</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>68</v>
+        <v>243</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -2215,7 +2215,7 @@
         <v>Implemented</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="F34" s="2"/>
     </row>
@@ -2231,7 +2231,7 @@
         <v>Implemented</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>75</v>
+        <v>304</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -2247,7 +2247,7 @@
         <v>Implemented</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>264</v>
+        <v>68</v>
       </c>
       <c r="F36" s="2"/>
     </row>
@@ -2263,7 +2263,7 @@
         <v>Implemented</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F37" s="2"/>
     </row>
@@ -2279,7 +2279,7 @@
         <v>Implemented</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>273</v>
+        <v>75</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -2295,7 +2295,7 @@
         <v>Implemented</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>184</v>
+        <v>264</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -2311,7 +2311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>321</v>
+        <v>88</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -2327,7 +2327,7 @@
         <v>Implemented</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>192</v>
+        <v>273</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -2343,7 +2343,7 @@
         <v>Implemented</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>364</v>
+        <v>184</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -2359,7 +2359,7 @@
         <v>Implemented</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>370</v>
+        <v>321</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -2375,7 +2375,7 @@
         <v>Implemented</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>372</v>
+        <v>192</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -2391,7 +2391,7 @@
         <v>Implemented</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -2407,7 +2407,7 @@
         <v>Implemented</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>206</v>
+        <v>370</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -2423,7 +2423,7 @@
         <v>Implemented</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>11</v>
+        <v>372</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -2439,7 +2439,7 @@
         <v>Implemented</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>12</v>
+        <v>374</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -2455,7 +2455,7 @@
         <v>Implemented</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>13</v>
+        <v>206</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -2471,7 +2471,7 @@
         <v>Implemented</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>226</v>
+        <v>11</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -2487,7 +2487,7 @@
         <v>Implemented</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -2503,7 +2503,7 @@
         <v>Implemented</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>231</v>
+        <v>13</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -2519,7 +2519,7 @@
         <v>Implemented</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>399</v>
+        <v>226</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -2535,7 +2535,7 @@
         <v>Implemented</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -2551,7 +2551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -2567,7 +2567,7 @@
         <v>Implemented</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>51</v>
+        <v>399</v>
       </c>
       <c r="F56" s="2"/>
     </row>
@@ -2583,7 +2583,7 @@
         <v>Implemented</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F57" s="2"/>
     </row>
@@ -2599,7 +2599,7 @@
         <v>Implemented</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="F58" s="2"/>
     </row>
@@ -2615,7 +2615,7 @@
         <v>Implemented</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>160</v>
+        <v>51</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -2631,7 +2631,7 @@
         <v>Implemented</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>252</v>
+        <v>49</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -2647,7 +2647,7 @@
         <v>Implemented</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -2663,7 +2663,7 @@
         <v>Implemented</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>172</v>
+        <v>307</v>
       </c>
       <c r="F62" s="2"/>
     </row>
@@ -2679,7 +2679,7 @@
         <v>Implemented</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="F63" s="2"/>
     </row>
@@ -2695,7 +2695,7 @@
         <v>Implemented</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>96</v>
+        <v>252</v>
       </c>
       <c r="F64" s="2"/>
     </row>
@@ -2711,7 +2711,7 @@
         <v>Implemented</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>317</v>
+        <v>170</v>
       </c>
       <c r="F65" s="2"/>
     </row>
@@ -2727,7 +2727,7 @@
         <v>Implemented</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -2743,7 +2743,7 @@
         <v>Implemented</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>323</v>
+        <v>85</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -2759,7 +2759,7 @@
         <v>Implemented</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>284</v>
+        <v>96</v>
       </c>
       <c r="F68" s="2"/>
     </row>
@@ -2775,7 +2775,7 @@
         <v>Implemented</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>380</v>
+        <v>317</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -2791,7 +2791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>115</v>
+        <v>193</v>
       </c>
       <c r="F70" s="2"/>
     </row>
@@ -2807,7 +2807,7 @@
         <v>Implemented</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>121</v>
+        <v>323</v>
       </c>
       <c r="F71" s="2"/>
     </row>
@@ -2823,7 +2823,7 @@
         <v>Implemented</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>3</v>
+        <v>284</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -2839,7 +2839,7 @@
         <v>Implemented</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>122</v>
+        <v>380</v>
       </c>
       <c r="F73" s="2"/>
     </row>
@@ -2855,7 +2855,7 @@
         <v>Implemented</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>398</v>
+        <v>115</v>
       </c>
       <c r="F74" s="2"/>
     </row>
@@ -2871,7 +2871,7 @@
         <v>Implemented</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -2887,7 +2887,7 @@
         <v>Implemented</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="F76" s="2"/>
     </row>
@@ -2903,7 +2903,7 @@
         <v>Implemented</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>215</v>
+        <v>122</v>
       </c>
       <c r="F77" s="2"/>
     </row>
@@ -2919,7 +2919,7 @@
         <v>Implemented</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>216</v>
+        <v>398</v>
       </c>
       <c r="F78" s="2"/>
     </row>
@@ -2935,7 +2935,7 @@
         <v>Implemented</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>217</v>
+        <v>120</v>
       </c>
       <c r="F79" s="2"/>
     </row>
@@ -2951,7 +2951,7 @@
         <v>Implemented</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="F80" s="2"/>
     </row>
@@ -2967,7 +2967,7 @@
         <v>Implemented</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="F81" s="2"/>
     </row>
@@ -2983,7 +2983,7 @@
         <v>Implemented</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F82" s="2"/>
     </row>
@@ -2999,7 +2999,7 @@
         <v>Implemented</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>126</v>
+        <v>217</v>
       </c>
       <c r="F83" s="2"/>
     </row>
@@ -3015,7 +3015,7 @@
         <v>Implemented</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F84" s="2"/>
     </row>
@@ -3031,7 +3031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F85" s="2"/>
     </row>
@@ -3047,7 +3047,7 @@
         <v>Implemented</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F86" s="2"/>
     </row>
@@ -3063,7 +3063,7 @@
         <v>Implemented</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F87" s="2"/>
     </row>
@@ -3079,7 +3079,7 @@
         <v>Implemented</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>24</v>
+        <v>222</v>
       </c>
       <c r="F88" s="2"/>
     </row>
@@ -3095,7 +3095,7 @@
         <v>Implemented</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>25</v>
+        <v>294</v>
       </c>
       <c r="F89" s="2"/>
     </row>
@@ -3111,7 +3111,7 @@
         <v>Implemented</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F90" s="2"/>
     </row>
@@ -3127,7 +3127,7 @@
         <v>Implemented</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>28</v>
+        <v>295</v>
       </c>
       <c r="F91" s="2"/>
     </row>
@@ -3143,7 +3143,7 @@
         <v>Implemented</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F92" s="2"/>
     </row>
@@ -3159,7 +3159,7 @@
         <v>Implemented</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>229</v>
+        <v>131</v>
       </c>
       <c r="F93" s="2"/>
     </row>
@@ -3175,7 +3175,7 @@
         <v>Implemented</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F94" s="2"/>
     </row>
@@ -3191,7 +3191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>232</v>
+        <v>25</v>
       </c>
       <c r="F95" s="2"/>
     </row>
@@ -3207,7 +3207,7 @@
         <v>Implemented</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>137</v>
+        <v>26</v>
       </c>
       <c r="F96" s="2"/>
     </row>
@@ -3223,7 +3223,7 @@
         <v>Implemented</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>34</v>
+        <v>389</v>
       </c>
       <c r="F97" s="2"/>
     </row>
@@ -3239,7 +3239,7 @@
         <v>Implemented</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="F98" s="2"/>
     </row>
@@ -3255,7 +3255,7 @@
         <v>Implemented</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>35</v>
+        <v>228</v>
       </c>
       <c r="F99" s="2"/>
     </row>
@@ -3271,7 +3271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F100" s="2"/>
     </row>
@@ -3287,7 +3287,7 @@
         <v>Implemented</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>234</v>
+        <v>32</v>
       </c>
       <c r="F101" s="2"/>
     </row>
@@ -3300,10 +3300,10 @@
       </c>
       <c r="C102" t="str">
         <f>IF(COUNTIF(D:D,$A102)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>142</v>
+        <v>232</v>
       </c>
       <c r="F102" s="2"/>
     </row>
@@ -3316,10 +3316,10 @@
       </c>
       <c r="C103" t="str">
         <f>IF(COUNTIF(D:D,$A103)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
       <c r="F103" s="2"/>
     </row>
@@ -3332,10 +3332,10 @@
       </c>
       <c r="C104" t="str">
         <f>IF(COUNTIF(D:D,$A104)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="F104" s="2"/>
     </row>
@@ -3348,10 +3348,10 @@
       </c>
       <c r="C105" t="str">
         <f>IF(COUNTIF(D:D,$A105)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F105" s="2"/>
     </row>
@@ -3364,10 +3364,10 @@
       </c>
       <c r="C106" t="str">
         <f>IF(COUNTIF(D:D,$A106)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F106" s="2"/>
     </row>
@@ -3380,10 +3380,10 @@
       </c>
       <c r="C107" t="str">
         <f>IF(COUNTIF(D:D,$A107)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F107" s="2"/>
     </row>
@@ -3396,10 +3396,10 @@
       </c>
       <c r="C108" t="str">
         <f>IF(COUNTIF(D:D,$A108)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>151</v>
+        <v>234</v>
       </c>
       <c r="F108" s="2"/>
     </row>
@@ -3412,10 +3412,10 @@
       </c>
       <c r="C109" t="str">
         <f>IF(COUNTIF(D:D,$A109)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F109" s="2"/>
     </row>
@@ -3428,10 +3428,10 @@
       </c>
       <c r="C110" t="str">
         <f>IF(COUNTIF(D:D,$A110)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>154</v>
+        <v>299</v>
       </c>
       <c r="F110" s="2"/>
     </row>
@@ -3444,10 +3444,10 @@
       </c>
       <c r="C111" t="str">
         <f>IF(COUNTIF(D:D,$A111)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>157</v>
+        <v>38</v>
       </c>
       <c r="F111" s="2"/>
     </row>
@@ -3460,10 +3460,10 @@
       </c>
       <c r="C112" t="str">
         <f>IF(COUNTIF(D:D,$A112)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>52</v>
+        <v>143</v>
       </c>
       <c r="F112" s="2"/>
     </row>
@@ -3476,10 +3476,10 @@
       </c>
       <c r="C113" t="str">
         <f>IF(COUNTIF(D:D,$A113)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>53</v>
+        <v>147</v>
       </c>
       <c r="F113" s="2"/>
     </row>
@@ -3492,10 +3492,10 @@
       </c>
       <c r="C114" t="str">
         <f>IF(COUNTIF(D:D,$A114)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>245</v>
+        <v>41</v>
       </c>
       <c r="F114" s="2"/>
     </row>
@@ -3508,10 +3508,10 @@
       </c>
       <c r="C115" t="str">
         <f>IF(COUNTIF(D:D,$A115)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>54</v>
+        <v>238</v>
       </c>
       <c r="F115" s="2"/>
     </row>
@@ -3524,10 +3524,10 @@
       </c>
       <c r="C116" t="str">
         <f>IF(COUNTIF(D:D,$A116)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>55</v>
+        <v>301</v>
       </c>
       <c r="F116" s="2"/>
     </row>
@@ -3540,10 +3540,10 @@
       </c>
       <c r="C117" t="str">
         <f>IF(COUNTIF(D:D,$A117)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="F117" s="2"/>
     </row>
@@ -3556,10 +3556,10 @@
       </c>
       <c r="C118" t="str">
         <f>IF(COUNTIF(D:D,$A118)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="F118" s="2"/>
     </row>
@@ -3572,10 +3572,10 @@
       </c>
       <c r="C119" t="str">
         <f>IF(COUNTIF(D:D,$A119)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F119" s="2"/>
     </row>
@@ -3588,10 +3588,10 @@
       </c>
       <c r="C120" t="str">
         <f>IF(COUNTIF(D:D,$A120)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>249</v>
+        <v>157</v>
       </c>
       <c r="F120" s="2"/>
     </row>
@@ -3604,10 +3604,10 @@
       </c>
       <c r="C121" t="str">
         <f>IF(COUNTIF(D:D,$A121)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>250</v>
+        <v>52</v>
       </c>
       <c r="F121" s="2"/>
     </row>
@@ -3620,10 +3620,10 @@
       </c>
       <c r="C122" t="str">
         <f>IF(COUNTIF(D:D,$A122)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>163</v>
+        <v>53</v>
       </c>
       <c r="F122" s="2"/>
     </row>
@@ -3636,10 +3636,10 @@
       </c>
       <c r="C123" t="str">
         <f>IF(COUNTIF(D:D,$A123)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>73</v>
+        <v>245</v>
       </c>
       <c r="F123" s="2"/>
     </row>
@@ -3652,10 +3652,10 @@
       </c>
       <c r="C124" t="str">
         <f>IF(COUNTIF(D:D,$A124)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="F124" s="2"/>
     </row>
@@ -3668,10 +3668,10 @@
       </c>
       <c r="C125" t="str">
         <f>IF(COUNTIF(D:D,$A125)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>164</v>
+        <v>55</v>
       </c>
       <c r="F125" s="2"/>
     </row>
@@ -3684,10 +3684,10 @@
       </c>
       <c r="C126" t="str">
         <f>IF(COUNTIF(D:D,$A126)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>253</v>
+        <v>56</v>
       </c>
       <c r="F126" s="2"/>
     </row>
@@ -3700,10 +3700,10 @@
       </c>
       <c r="C127" t="str">
         <f>IF(COUNTIF(D:D,$A127)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="F127" s="2"/>
     </row>
@@ -3716,10 +3716,10 @@
       </c>
       <c r="C128" t="str">
         <f>IF(COUNTIF(D:D,$A128)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="F128" s="2"/>
     </row>
@@ -3732,10 +3732,10 @@
       </c>
       <c r="C129" t="str">
         <f>IF(COUNTIF(D:D,$A129)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="F129" s="2"/>
     </row>
@@ -3748,10 +3748,10 @@
       </c>
       <c r="C130" t="str">
         <f>IF(COUNTIF(D:D,$A130)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>168</v>
+        <v>249</v>
       </c>
       <c r="F130" s="2"/>
     </row>
@@ -3767,7 +3767,7 @@
         <v>Implemented</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>79</v>
+        <v>250</v>
       </c>
       <c r="F131" s="2"/>
     </row>
@@ -3780,10 +3780,10 @@
       </c>
       <c r="C132" t="str">
         <f>IF(COUNTIF(D:D,$A132)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F132" s="2"/>
     </row>
@@ -3796,10 +3796,10 @@
       </c>
       <c r="C133" t="str">
         <f>IF(COUNTIF(D:D,$A133)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -3815,7 +3815,7 @@
         <v>Implemented</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>257</v>
+        <v>74</v>
       </c>
       <c r="F134" s="2"/>
     </row>
@@ -3831,7 +3831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>259</v>
+        <v>164</v>
       </c>
       <c r="F135" s="2"/>
     </row>
@@ -3847,7 +3847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="F136" s="2"/>
     </row>
@@ -3863,7 +3863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>263</v>
+        <v>76</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -3879,7 +3879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -3895,7 +3895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>89</v>
+        <v>255</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -3911,7 +3911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>266</v>
+        <v>168</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -3927,7 +3927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -3943,7 +3943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -3959,7 +3959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="F143" s="2"/>
     </row>
@@ -3975,7 +3975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>94</v>
+        <v>257</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -3991,7 +3991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>95</v>
+        <v>259</v>
       </c>
       <c r="F145" s="2"/>
     </row>
@@ -4007,7 +4007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="F146" s="2"/>
     </row>
@@ -4023,7 +4023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>178</v>
+        <v>263</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4039,7 +4039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>270</v>
+        <v>173</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4055,7 +4055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>179</v>
+        <v>311</v>
       </c>
       <c r="F149" s="2"/>
     </row>
@@ -4071,7 +4071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>98</v>
+        <v>312</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4086,7 +4086,7 @@
         <v>Implemented</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>271</v>
+        <v>89</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>Implemented</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>99</v>
+        <v>266</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4116,7 +4116,7 @@
         <v>Implemented</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4131,7 +4131,7 @@
         <v>Implemented</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>101</v>
+        <v>313</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4146,7 +4146,7 @@
         <v>Implemented</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>183</v>
+        <v>91</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
         <v>Implemented</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>274</v>
+        <v>93</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4176,7 +4176,7 @@
         <v>Implemented</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4206,7 +4206,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>187</v>
+        <v>269</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>392</v>
+        <v>178</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>189</v>
+        <v>270</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4251,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>195</v>
+        <v>98</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>196</v>
+        <v>271</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,7 +4296,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>197</v>
+        <v>99</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>278</v>
+        <v>100</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,7 +4326,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>365</v>
+        <v>101</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>366</v>
+        <v>183</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4356,7 +4356,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>367</v>
+        <v>318</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,7 +4371,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>393</v>
+        <v>274</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,7 +4386,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>199</v>
+        <v>106</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>280</v>
+        <v>110</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>281</v>
+        <v>187</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,7 +4431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>201</v>
+        <v>392</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4446,7 +4446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>282</v>
+        <v>190</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>207</v>
+        <v>322</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4491,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>285</v>
+        <v>195</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4506,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>377</v>
+        <v>196</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4521,7 +4521,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>378</v>
+        <v>197</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4536,7 +4536,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,7 +4551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,7 +4566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>209</v>
+        <v>366</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>210</v>
+        <v>393</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +4611,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +4641,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>213</v>
+        <v>281</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,7 +4656,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>118</v>
+        <v>201</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>125</v>
+        <v>204</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +4701,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4716,7 +4716,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>20</v>
+        <v>285</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4731,7 +4731,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>21</v>
+        <v>377</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4746,7 +4746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>129</v>
+        <v>378</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4761,7 +4761,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>31</v>
+        <v>287</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4776,7 +4776,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>150</v>
+        <v>385</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,7 +4821,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>57</v>
+        <v>210</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4836,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>59</v>
+        <v>212</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4851,7 +4851,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>60</v>
+        <v>288</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4866,7 +4866,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>65</v>
+        <v>213</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,7 +4881,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>248</v>
+        <v>118</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4896,7 +4896,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4911,7 +4911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>78</v>
+        <v>291</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4941,7 +4941,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>181</v>
+        <v>20</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>182</v>
+        <v>21</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4971,7 +4971,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>373</v>
+        <v>129</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,7 +4986,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>221</v>
+        <v>31</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,7 +5001,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>132</v>
+        <v>235</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5016,7 +5016,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>37</v>
+        <v>239</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5031,7 +5031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>247</v>
+        <v>150</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5061,7 +5061,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,7 +5076,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>161</v>
+        <v>60</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,7 +5091,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>167</v>
+        <v>65</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,7 +5121,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>260</v>
+        <v>69</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,7 +5136,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>82</v>
+        <v>309</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5166,7 +5166,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>84</v>
+        <v>175</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,7 +5181,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>92</v>
+        <v>181</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5211,7 +5211,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>275</v>
+        <v>324</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5226,7 +5226,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>108</v>
+        <v>373</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>109</v>
+        <v>221</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,7 +5256,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>188</v>
+        <v>297</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5271,7 +5271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>202</v>
+        <v>132</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>203</v>
+        <v>37</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5302,7 +5302,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>18</v>
+        <v>247</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5318,7 +5318,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5334,7 +5334,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5350,7 +5350,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>128</v>
+        <v>161</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5366,7 +5366,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>224</v>
+        <v>167</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5382,7 +5382,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>133</v>
+        <v>256</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5398,7 +5398,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>134</v>
+        <v>260</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5414,7 +5414,7 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5430,7 +5430,7 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5446,7 +5446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>148</v>
+        <v>310</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5462,7 +5462,7 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="F242" s="2"/>
     </row>
@@ -5478,7 +5478,7 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>246</v>
+        <v>92</v>
       </c>
       <c r="F243" s="2"/>
     </row>
@@ -5494,7 +5494,7 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>261</v>
+        <v>97</v>
       </c>
       <c r="F244" s="2"/>
     </row>
@@ -5510,7 +5510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>268</v>
+        <v>319</v>
       </c>
       <c r="F245" s="2"/>
     </row>
@@ -5526,7 +5526,7 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>104</v>
+        <v>275</v>
       </c>
       <c r="F246" s="2"/>
     </row>
@@ -5542,7 +5542,7 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>186</v>
+        <v>108</v>
       </c>
       <c r="F247" s="2"/>
     </row>
@@ -5558,7 +5558,7 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F248" s="2"/>
     </row>
@@ -5574,7 +5574,7 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>277</v>
+        <v>188</v>
       </c>
       <c r="F249" s="2"/>
     </row>
@@ -5590,7 +5590,7 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5606,7 +5606,7 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>362</v>
+        <v>203</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5622,7 +5622,7 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>375</v>
+        <v>18</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5638,7 +5638,7 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F253" s="2"/>
     </row>
@@ -5654,7 +5654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>214</v>
+        <v>19</v>
       </c>
       <c r="F254" s="2"/>
     </row>
@@ -5670,7 +5670,7 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="F255" s="2"/>
     </row>
@@ -5686,7 +5686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>145</v>
+        <v>224</v>
       </c>
       <c r="F256" s="2"/>
     </row>
@@ -5702,7 +5702,7 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="F257" s="2"/>
     </row>
@@ -5718,7 +5718,7 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>242</v>
+        <v>134</v>
       </c>
       <c r="F258" s="2"/>
     </row>
@@ -5734,7 +5734,7 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F259" s="2"/>
     </row>
@@ -5750,7 +5750,7 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
       <c r="F260" s="2"/>
     </row>
@@ -5766,7 +5766,7 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -5782,7 +5782,7 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -5798,7 +5798,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>64</v>
+        <v>246</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5814,7 +5814,7 @@
         <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>254</v>
+        <v>308</v>
       </c>
       <c r="F264" s="2"/>
     </row>
@@ -5830,7 +5830,7 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>166</v>
+        <v>261</v>
       </c>
       <c r="F265" s="2"/>
     </row>
@@ -5846,7 +5846,7 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>400</v>
+        <v>314</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -5862,7 +5862,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5878,7 +5878,7 @@
         <v>Missing</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>102</v>
+        <v>316</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5894,7 +5894,7 @@
         <v>Missing</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>198</v>
+        <v>104</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -5910,7 +5910,7 @@
         <v>Missing</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>371</v>
+        <v>186</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -5926,7 +5926,7 @@
         <v>Missing</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>205</v>
+        <v>112</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -5942,7 +5942,7 @@
         <v>Missing</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>383</v>
+        <v>277</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -5958,7 +5958,7 @@
         <v>Missing</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>384</v>
+        <v>113</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -5974,7 +5974,7 @@
         <v>Missing</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>292</v>
+        <v>362</v>
       </c>
       <c r="F274" s="2"/>
     </row>
@@ -5990,7 +5990,7 @@
         <v>Missing</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>130</v>
+        <v>375</v>
       </c>
       <c r="F275" s="2"/>
     </row>
@@ -6006,7 +6006,7 @@
         <v>Missing</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="F276" s="2"/>
     </row>
@@ -6022,7 +6022,7 @@
         <v>Missing</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>141</v>
+        <v>214</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -6038,7 +6038,7 @@
         <v>Missing</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>236</v>
+        <v>23</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -6054,7 +6054,7 @@
         <v>Missing</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>39</v>
+        <v>298</v>
       </c>
       <c r="F279" s="2"/>
     </row>
@@ -6070,7 +6070,7 @@
         <v>Missing</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="F280" s="2"/>
     </row>
@@ -6086,7 +6086,7 @@
         <v>Missing</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>241</v>
+        <v>300</v>
       </c>
       <c r="F281" s="2"/>
     </row>
@@ -6102,7 +6102,7 @@
         <v>Missing</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F282" s="2"/>
     </row>
@@ -6118,7 +6118,7 @@
         <v>Missing</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>62</v>
+        <v>302</v>
       </c>
       <c r="F283" s="2"/>
     </row>
@@ -6134,7 +6134,7 @@
         <v>Missing</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>87</v>
+        <v>242</v>
       </c>
       <c r="F284" s="2"/>
     </row>
@@ -6150,7 +6150,7 @@
         <v>Missing</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>177</v>
+        <v>45</v>
       </c>
       <c r="F285" s="2"/>
     </row>
@@ -6166,7 +6166,7 @@
         <v>Missing</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="F286" s="2"/>
     </row>
@@ -6182,7 +6182,7 @@
         <v>Missing</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="F287" s="2"/>
     </row>
@@ -6198,7 +6198,7 @@
         <v>Missing</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="F288" s="2"/>
     </row>
@@ -6214,7 +6214,7 @@
         <v>Missing</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>276</v>
+        <v>64</v>
       </c>
       <c r="F289" s="2"/>
     </row>
@@ -6230,7 +6230,7 @@
         <v>Missing</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>397</v>
+        <v>254</v>
       </c>
       <c r="F290" s="2"/>
     </row>
@@ -6246,7 +6246,7 @@
         <v>Missing</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="F291" s="2"/>
     </row>
@@ -6262,7 +6262,7 @@
         <v>Missing</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>368</v>
+        <v>400</v>
       </c>
       <c r="F292" s="2"/>
     </row>
@@ -6278,7 +6278,7 @@
         <v>Missing</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>200</v>
+        <v>258</v>
       </c>
       <c r="F293" s="2"/>
     </row>
@@ -6294,7 +6294,7 @@
         <v>Missing</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>286</v>
+        <v>102</v>
       </c>
       <c r="F294" s="2"/>
     </row>
@@ -6310,7 +6310,7 @@
         <v>Missing</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>376</v>
+        <v>198</v>
       </c>
       <c r="F295" s="2"/>
     </row>
@@ -6326,7 +6326,7 @@
         <v>Missing</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>124</v>
+        <v>371</v>
       </c>
       <c r="F296" s="2"/>
     </row>
@@ -6342,7 +6342,7 @@
         <v>Missing</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>15</v>
+        <v>205</v>
       </c>
       <c r="F297" s="2"/>
     </row>
@@ -6358,7 +6358,7 @@
         <v>Missing</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>220</v>
+        <v>383</v>
       </c>
       <c r="F298" s="2"/>
     </row>
@@ -6374,7 +6374,7 @@
         <v>Missing</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>127</v>
+        <v>384</v>
       </c>
       <c r="F299" s="2"/>
     </row>
@@ -6390,7 +6390,7 @@
         <v>Missing</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="F300" s="2"/>
     </row>
@@ -6406,7 +6406,7 @@
         <v>Missing</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="F301" s="2"/>
     </row>
@@ -6422,7 +6422,7 @@
         <v>Missing</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>230</v>
+        <v>33</v>
       </c>
       <c r="F302" s="2"/>
     </row>
@@ -6438,7 +6438,7 @@
         <v>Implemented</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F303" s="2"/>
     </row>
@@ -6454,7 +6454,7 @@
         <v>Implemented</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>42</v>
+        <v>236</v>
       </c>
       <c r="F304" s="2"/>
     </row>
@@ -6470,7 +6470,7 @@
         <v>Implemented</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F305" s="2"/>
     </row>
@@ -6486,7 +6486,7 @@
         <v>Implemented</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="F306" s="2"/>
     </row>
@@ -6502,7 +6502,7 @@
         <v>Implemented</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>334</v>
+        <v>241</v>
       </c>
       <c r="F307" s="2"/>
     </row>
@@ -6518,7 +6518,7 @@
         <v>Implemented</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>63</v>
+        <v>153</v>
       </c>
       <c r="F308" s="2"/>
     </row>
@@ -6534,7 +6534,7 @@
         <v>Implemented</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="F309" s="2"/>
     </row>
@@ -6550,7 +6550,7 @@
         <v>Implemented</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F310" s="2"/>
     </row>
@@ -6566,7 +6566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>265</v>
+        <v>315</v>
       </c>
       <c r="F311" s="2"/>
     </row>
@@ -6582,7 +6582,7 @@
         <v>Implemented</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F312" s="2"/>
     </row>
@@ -6598,7 +6598,7 @@
         <v>Implemented</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F313" s="2"/>
     </row>
@@ -6614,7 +6614,7 @@
         <v>Implemented</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F314" s="2"/>
     </row>
@@ -6630,7 +6630,7 @@
         <v>Implemented</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>283</v>
+        <v>107</v>
       </c>
       <c r="F315" s="2"/>
     </row>
@@ -6646,7 +6646,7 @@
         <v>Implemented</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>379</v>
+        <v>276</v>
       </c>
       <c r="F316" s="2"/>
     </row>
@@ -6662,7 +6662,7 @@
         <v>Implemented</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>381</v>
+        <v>397</v>
       </c>
       <c r="F317" s="2"/>
     </row>
@@ -6678,7 +6678,7 @@
         <v>Implemented</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="F318" s="2"/>
     </row>
@@ -6694,7 +6694,7 @@
         <v>Implemented</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>137</v>
+        <v>368</v>
       </c>
       <c r="F319" s="2"/>
     </row>
@@ -6710,7 +6710,7 @@
         <v>Implemented</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>151</v>
+        <v>200</v>
       </c>
       <c r="F320" s="2"/>
     </row>
@@ -6726,7 +6726,7 @@
         <v>Implemented</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>245</v>
+        <v>325</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -6742,7 +6742,7 @@
         <v>Implemented</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>198</v>
+        <v>286</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6758,7 +6758,7 @@
         <v>Implemented</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6774,7 +6774,7 @@
         <v>Implemented</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="F324" s="2"/>
     </row>
@@ -6790,7 +6790,7 @@
         <v>Implemented</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
@@ -6805,7 +6805,7 @@
         <v>Implemented</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
@@ -6820,7 +6820,7 @@
         <v>Implemented</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -6835,7 +6835,7 @@
         <v>Implemented</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>228</v>
+        <v>296</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
@@ -6850,7 +6850,7 @@
         <v>Implemented</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>154</v>
+        <v>27</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -6865,7 +6865,7 @@
         <v>Implemented</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>173</v>
+        <v>30</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
@@ -6880,7 +6880,7 @@
         <v>Implemented</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>150</v>
+        <v>230</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -6895,7 +6895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
@@ -6910,7 +6910,7 @@
         <v>Implemented</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>203</v>
+        <v>42</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
@@ -6925,7 +6925,7 @@
         <v>Implemented</v>
       </c>
       <c r="D334" s="2" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
@@ -6940,7 +6940,7 @@
         <v>Implemented</v>
       </c>
       <c r="D335" s="2" t="s">
-        <v>134</v>
+        <v>244</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
@@ -6955,7 +6955,7 @@
         <v>Implemented</v>
       </c>
       <c r="D336" s="2" t="s">
-        <v>130</v>
+        <v>305</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -6970,7 +6970,7 @@
         <v>Implemented</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>124</v>
+        <v>334</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -6985,7 +6985,7 @@
         <v>Implemented</v>
       </c>
       <c r="D338" s="2" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -6999,6 +6999,9 @@
         <f>IF(COUNTIF(D:D,$A339)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D339" s="2" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
@@ -7011,6 +7014,9 @@
         <f>IF(COUNTIF(D:D,$A340)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D340" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
@@ -7024,7 +7030,7 @@
         <v>Implemented</v>
       </c>
       <c r="D341" s="2" t="s">
-        <v>101</v>
+        <v>265</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -7039,7 +7045,7 @@
         <v>Implemented</v>
       </c>
       <c r="D342" s="2" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -7054,7 +7060,7 @@
         <v>Implemented</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>234</v>
+        <v>111</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -7069,7 +7075,7 @@
         <v>Implemented</v>
       </c>
       <c r="D344" s="2" t="s">
-        <v>106</v>
+        <v>320</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -7083,6 +7089,9 @@
         <f>IF(COUNTIF(D:D,$A345)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D345" s="2" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
@@ -7095,6 +7104,9 @@
         <f>IF(COUNTIF(D:D,$A346)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D346" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
@@ -7107,6 +7119,9 @@
         <f>IF(COUNTIF(D:D,$A347)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D347" s="2" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
@@ -7119,6 +7134,9 @@
         <f>IF(COUNTIF(D:D,$A348)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D348" s="2" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
@@ -7131,6 +7149,9 @@
         <f>IF(COUNTIF(D:D,$A349)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D349" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
@@ -7143,6 +7164,9 @@
         <f>IF(COUNTIF(D:D,$A350)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D350" s="2" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
@@ -7155,6 +7179,9 @@
         <f>IF(COUNTIF(D:D,$A351)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D351" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
@@ -7167,8 +7194,11 @@
         <f>IF(COUNTIF(D:D,$A352)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D352" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>258</v>
       </c>
@@ -7179,8 +7209,11 @@
         <f>IF(COUNTIF(D:D,$A353)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D353" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>259</v>
       </c>
@@ -7191,8 +7224,11 @@
         <f>IF(COUNTIF(D:D,$A354)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D354" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>260</v>
       </c>
@@ -7203,8 +7239,11 @@
         <f>IF(COUNTIF(D:D,$A355)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D355" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>261</v>
       </c>
@@ -7215,8 +7254,11 @@
         <f>IF(COUNTIF(D:D,$A356)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D356" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>262</v>
       </c>
@@ -7227,8 +7269,11 @@
         <f>IF(COUNTIF(D:D,$A357)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D357" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>263</v>
       </c>
@@ -7239,8 +7284,11 @@
         <f>IF(COUNTIF(D:D,$A358)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D358" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>264</v>
       </c>
@@ -7251,8 +7299,11 @@
         <f>IF(COUNTIF(D:D,$A359)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D359" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>265</v>
       </c>
@@ -7263,8 +7314,11 @@
         <f>IF(COUNTIF(D:D,$A360)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D360" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>266</v>
       </c>
@@ -7275,8 +7329,11 @@
         <f>IF(COUNTIF(D:D,$A361)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D361" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>267</v>
       </c>
@@ -7287,8 +7344,11 @@
         <f>IF(COUNTIF(D:D,$A362)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D362" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>268</v>
       </c>
@@ -7299,8 +7359,11 @@
         <f>IF(COUNTIF(D:D,$A363)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D363" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>269</v>
       </c>
@@ -7311,8 +7374,11 @@
         <f>IF(COUNTIF(D:D,$A364)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D364" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>270</v>
       </c>
@@ -7323,8 +7389,11 @@
         <f>IF(COUNTIF(D:D,$A365)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D365" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>271</v>
       </c>
@@ -7335,8 +7404,11 @@
         <f>IF(COUNTIF(D:D,$A366)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D366" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>272</v>
       </c>
@@ -7347,8 +7419,11 @@
         <f>IF(COUNTIF(D:D,$A367)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-    </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D367" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>273</v>
       </c>
@@ -7358,6 +7433,9 @@
       <c r="C368" t="str">
         <f>IF(COUNTIF(D:D,$A368)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -7371,6 +7449,9 @@
         <f>IF(COUNTIF(D:D,$A369)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D369" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
@@ -7407,6 +7488,9 @@
         <f>IF(COUNTIF(D:D,$A372)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D372" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
@@ -7419,6 +7503,9 @@
         <f>IF(COUNTIF(D:D,$A373)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D373" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
@@ -7431,6 +7518,9 @@
         <f>IF(COUNTIF(D:D,$A374)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D374" s="2" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
@@ -7443,6 +7533,9 @@
         <f>IF(COUNTIF(D:D,$A375)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D375" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
@@ -7467,9 +7560,6 @@
         <f>IF(COUNTIF(D:D,$A377)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D377" s="2" t="s">
-        <v>231</v>
-      </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
@@ -7482,9 +7572,6 @@
         <f>IF(COUNTIF(D:D,$A378)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D378" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
@@ -7497,9 +7584,6 @@
         <f>IF(COUNTIF(D:D,$A379)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D379" s="2" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
@@ -7512,9 +7596,6 @@
         <f>IF(COUNTIF(D:D,$A380)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D380" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
@@ -7527,9 +7608,6 @@
         <f>IF(COUNTIF(D:D,$A381)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D381" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
@@ -7542,9 +7620,6 @@
         <f>IF(COUNTIF(D:D,$A382)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D382" s="2" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
@@ -7557,92 +7632,124 @@
         <f>IF(COUNTIF(D:D,$A383)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
-      <c r="D383" s="2" t="s">
+    </row>
+    <row r="408" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D408" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="409" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D409" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="410" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D410" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="411" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D411" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="412" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D412" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="413" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D413" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="414" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D414" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D384" s="2" t="s">
+    <row r="415" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D415" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="385" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D385" s="2" t="s">
+    <row r="416" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D416" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="386" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D386" s="2" t="s">
+    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D417" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="387" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D387" s="2" t="s">
+    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D418" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="388" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D388" s="2" t="s">
+    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D419" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="389" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D389" s="2" t="s">
+    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D420" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="390" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D390" s="2" t="s">
+    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D421" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="391" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D391" s="2" t="s">
+    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D422" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="392" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D392" s="2" t="s">
+    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D423" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="393" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D393" s="2" t="s">
+    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D424" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="394" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D394" s="2" t="s">
+    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D425" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="395" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D395" s="2" t="s">
+    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D426" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="396" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D396" s="2" t="s">
+    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D427" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="397" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D397" s="2" t="s">
+    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D428" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="398" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D398" s="2" t="s">
+    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D429" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="399" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D399" s="2" t="s">
+    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D430" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="400" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D400" s="2" t="s">
+    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D431" s="2" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- removed ununsed (because: slow) cloning lib - removed Swing UI lib - implemented Al'Akir the Windlord
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -1607,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K431"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="A268" sqref="A268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- implemented the following Legendary cards: Cenarius, Archmage Antonidas, Alexstrasza, Baron Geddon, Bloodmage Thalnos, Cairne Bloodhoof, Captain Greenskin, Deathwing, Elite Tauren Chieftain, Gelbin Mekkatorque, Edwin VanCleef - GameLogic thread is now flagged as daemon and therefor automatically terminated when UI is closed
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$348</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$360</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="401">
   <si>
     <t>Cardname</t>
   </si>
@@ -1605,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K431"/>
+  <dimension ref="A1:K443"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268"/>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="A279" sqref="A279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,7 +1723,7 @@
         <v>Implemented</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>331</v>
       </c>
       <c r="F5" s="2"/>
       <c r="J5" t="s">
@@ -1746,7 +1746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2"/>
       <c r="J6" s="1" t="s">
@@ -1769,7 +1769,7 @@
         <v>Implemented</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>303</v>
+        <v>144</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1785,7 +1785,7 @@
         <v>Implemented</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>61</v>
+        <v>303</v>
       </c>
       <c r="F8" s="2"/>
       <c r="J8" t="s">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>347</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
         <v>Implemented</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F9" s="2"/>
       <c r="J9" t="s">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1831,7 +1831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1847,7 +1847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>251</v>
+        <v>72</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1863,7 +1863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>171</v>
+        <v>251</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -1879,7 +1879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>81</v>
+        <v>171</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -1895,7 +1895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1911,7 +1911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>174</v>
+        <v>86</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1927,7 +1927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>267</v>
+        <v>174</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -1943,7 +1943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>176</v>
+        <v>267</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1959,7 +1959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>105</v>
+        <v>176</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -1975,7 +1975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>272</v>
+        <v>105</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1991,7 +1991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>194</v>
+        <v>272</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -2007,7 +2007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -2023,7 +2023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>363</v>
+        <v>279</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -2039,7 +2039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -2055,7 +2055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -2071,7 +2071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>211</v>
+        <v>382</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -2087,7 +2087,7 @@
         <v>Implemented</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>10</v>
+        <v>211</v>
       </c>
       <c r="F26" s="2"/>
     </row>
@@ -2103,7 +2103,7 @@
         <v>Implemented</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -2119,7 +2119,7 @@
         <v>Implemented</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>293</v>
+        <v>14</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -2135,7 +2135,7 @@
         <v>Implemented</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>139</v>
+        <v>293</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -2151,7 +2151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>237</v>
+        <v>139</v>
       </c>
       <c r="F30" s="2"/>
     </row>
@@ -2167,7 +2167,7 @@
         <v>Implemented</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -2183,7 +2183,7 @@
         <v>Implemented</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>149</v>
+        <v>240</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -2199,7 +2199,7 @@
         <v>Implemented</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>243</v>
+        <v>149</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -2215,7 +2215,7 @@
         <v>Implemented</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>156</v>
+        <v>243</v>
       </c>
       <c r="F34" s="2"/>
     </row>
@@ -2231,7 +2231,7 @@
         <v>Implemented</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>304</v>
+        <v>156</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -2247,7 +2247,7 @@
         <v>Implemented</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>68</v>
+        <v>304</v>
       </c>
       <c r="F36" s="2"/>
     </row>
@@ -2263,7 +2263,7 @@
         <v>Implemented</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F37" s="2"/>
     </row>
@@ -2279,7 +2279,7 @@
         <v>Implemented</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -2295,7 +2295,7 @@
         <v>Implemented</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>264</v>
+        <v>75</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -2311,7 +2311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>88</v>
+        <v>264</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -2327,7 +2327,7 @@
         <v>Implemented</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>273</v>
+        <v>88</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -2343,7 +2343,7 @@
         <v>Implemented</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>184</v>
+        <v>273</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -2359,7 +2359,7 @@
         <v>Implemented</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>321</v>
+        <v>184</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -2375,7 +2375,7 @@
         <v>Implemented</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>192</v>
+        <v>321</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -2391,7 +2391,7 @@
         <v>Implemented</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>364</v>
+        <v>192</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -2407,7 +2407,7 @@
         <v>Implemented</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -2423,7 +2423,7 @@
         <v>Implemented</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -2439,7 +2439,7 @@
         <v>Implemented</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -2455,7 +2455,7 @@
         <v>Implemented</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>206</v>
+        <v>374</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -2471,7 +2471,7 @@
         <v>Implemented</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>11</v>
+        <v>206</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -2487,7 +2487,7 @@
         <v>Implemented</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -2503,7 +2503,7 @@
         <v>Implemented</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -2519,7 +2519,7 @@
         <v>Implemented</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>226</v>
+        <v>13</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -2535,7 +2535,7 @@
         <v>Implemented</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>135</v>
+        <v>326</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -2551,7 +2551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -2567,7 +2567,7 @@
         <v>Implemented</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>399</v>
+        <v>135</v>
       </c>
       <c r="F56" s="2"/>
     </row>
@@ -2583,7 +2583,7 @@
         <v>Implemented</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>46</v>
+        <v>231</v>
       </c>
       <c r="F57" s="2"/>
     </row>
@@ -2599,7 +2599,7 @@
         <v>Implemented</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>47</v>
+        <v>399</v>
       </c>
       <c r="F58" s="2"/>
     </row>
@@ -2615,7 +2615,7 @@
         <v>Implemented</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -2631,7 +2631,7 @@
         <v>Implemented</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -2647,7 +2647,7 @@
         <v>Implemented</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -2663,7 +2663,7 @@
         <v>Implemented</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>307</v>
+        <v>49</v>
       </c>
       <c r="F62" s="2"/>
     </row>
@@ -2679,7 +2679,7 @@
         <v>Implemented</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F63" s="2"/>
     </row>
@@ -2695,7 +2695,7 @@
         <v>Implemented</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>252</v>
+        <v>307</v>
       </c>
       <c r="F64" s="2"/>
     </row>
@@ -2711,7 +2711,7 @@
         <v>Implemented</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F65" s="2"/>
     </row>
@@ -2727,7 +2727,7 @@
         <v>Implemented</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>172</v>
+        <v>252</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -2743,7 +2743,7 @@
         <v>Implemented</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -2759,7 +2759,7 @@
         <v>Implemented</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="F68" s="2"/>
     </row>
@@ -2775,7 +2775,7 @@
         <v>Implemented</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>317</v>
+        <v>85</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -2791,7 +2791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>193</v>
+        <v>96</v>
       </c>
       <c r="F70" s="2"/>
     </row>
@@ -2807,7 +2807,7 @@
         <v>Implemented</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="F71" s="2"/>
     </row>
@@ -2823,7 +2823,7 @@
         <v>Implemented</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>284</v>
+        <v>193</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -2839,7 +2839,7 @@
         <v>Implemented</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>380</v>
+        <v>323</v>
       </c>
       <c r="F73" s="2"/>
     </row>
@@ -2855,7 +2855,7 @@
         <v>Implemented</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>115</v>
+        <v>284</v>
       </c>
       <c r="F74" s="2"/>
     </row>
@@ -2871,7 +2871,7 @@
         <v>Implemented</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>121</v>
+        <v>380</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -2887,7 +2887,7 @@
         <v>Implemented</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="F76" s="2"/>
     </row>
@@ -2903,7 +2903,7 @@
         <v>Implemented</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F77" s="2"/>
     </row>
@@ -2919,7 +2919,7 @@
         <v>Implemented</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>398</v>
+        <v>3</v>
       </c>
       <c r="F78" s="2"/>
     </row>
@@ -2935,7 +2935,7 @@
         <v>Implemented</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F79" s="2"/>
     </row>
@@ -2951,7 +2951,7 @@
         <v>Implemented</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>123</v>
+        <v>398</v>
       </c>
       <c r="F80" s="2"/>
     </row>
@@ -2967,7 +2967,7 @@
         <v>Implemented</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>215</v>
+        <v>119</v>
       </c>
       <c r="F81" s="2"/>
     </row>
@@ -2983,7 +2983,7 @@
         <v>Implemented</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>216</v>
+        <v>120</v>
       </c>
       <c r="F82" s="2"/>
     </row>
@@ -2999,7 +2999,7 @@
         <v>Implemented</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>217</v>
+        <v>123</v>
       </c>
       <c r="F83" s="2"/>
     </row>
@@ -3015,7 +3015,7 @@
         <v>Implemented</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F84" s="2"/>
     </row>
@@ -3031,7 +3031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>16</v>
+        <v>216</v>
       </c>
       <c r="F85" s="2"/>
     </row>
@@ -3047,7 +3047,7 @@
         <v>Implemented</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F86" s="2"/>
     </row>
@@ -3063,7 +3063,7 @@
         <v>Implemented</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>126</v>
+        <v>218</v>
       </c>
       <c r="F87" s="2"/>
     </row>
@@ -3079,7 +3079,7 @@
         <v>Implemented</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>222</v>
+        <v>16</v>
       </c>
       <c r="F88" s="2"/>
     </row>
@@ -3095,7 +3095,7 @@
         <v>Implemented</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>294</v>
+        <v>219</v>
       </c>
       <c r="F89" s="2"/>
     </row>
@@ -3111,7 +3111,7 @@
         <v>Implemented</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="F90" s="2"/>
     </row>
@@ -3127,7 +3127,7 @@
         <v>Implemented</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>295</v>
+        <v>222</v>
       </c>
       <c r="F91" s="2"/>
     </row>
@@ -3143,7 +3143,7 @@
         <v>Implemented</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>227</v>
+        <v>327</v>
       </c>
       <c r="F92" s="2"/>
     </row>
@@ -3159,7 +3159,7 @@
         <v>Implemented</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>131</v>
+        <v>294</v>
       </c>
       <c r="F93" s="2"/>
     </row>
@@ -3175,7 +3175,7 @@
         <v>Implemented</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F94" s="2"/>
     </row>
@@ -3191,7 +3191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>25</v>
+        <v>295</v>
       </c>
       <c r="F95" s="2"/>
     </row>
@@ -3207,7 +3207,7 @@
         <v>Implemented</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>26</v>
+        <v>328</v>
       </c>
       <c r="F96" s="2"/>
     </row>
@@ -3223,7 +3223,7 @@
         <v>Implemented</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>389</v>
+        <v>227</v>
       </c>
       <c r="F97" s="2"/>
     </row>
@@ -3239,7 +3239,7 @@
         <v>Implemented</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
       <c r="F98" s="2"/>
     </row>
@@ -3255,7 +3255,7 @@
         <v>Implemented</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>228</v>
+        <v>24</v>
       </c>
       <c r="F99" s="2"/>
     </row>
@@ -3271,7 +3271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>229</v>
+        <v>25</v>
       </c>
       <c r="F100" s="2"/>
     </row>
@@ -3287,7 +3287,7 @@
         <v>Implemented</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F101" s="2"/>
     </row>
@@ -3303,7 +3303,7 @@
         <v>Implemented</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>232</v>
+        <v>329</v>
       </c>
       <c r="F102" s="2"/>
     </row>
@@ -3319,7 +3319,7 @@
         <v>Implemented</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>137</v>
+        <v>330</v>
       </c>
       <c r="F103" s="2"/>
     </row>
@@ -3335,7 +3335,7 @@
         <v>Implemented</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>34</v>
+        <v>389</v>
       </c>
       <c r="F104" s="2"/>
     </row>
@@ -3351,7 +3351,7 @@
         <v>Implemented</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="F105" s="2"/>
     </row>
@@ -3367,7 +3367,7 @@
         <v>Implemented</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>35</v>
+        <v>228</v>
       </c>
       <c r="F106" s="2"/>
     </row>
@@ -3383,7 +3383,7 @@
         <v>Implemented</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F107" s="2"/>
     </row>
@@ -3399,7 +3399,7 @@
         <v>Implemented</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>234</v>
+        <v>32</v>
       </c>
       <c r="F108" s="2"/>
     </row>
@@ -3415,7 +3415,7 @@
         <v>Implemented</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>142</v>
+        <v>232</v>
       </c>
       <c r="F109" s="2"/>
     </row>
@@ -3431,7 +3431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>299</v>
+        <v>137</v>
       </c>
       <c r="F110" s="2"/>
     </row>
@@ -3447,7 +3447,7 @@
         <v>Implemented</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F111" s="2"/>
     </row>
@@ -3463,7 +3463,7 @@
         <v>Implemented</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F112" s="2"/>
     </row>
@@ -3479,7 +3479,7 @@
         <v>Implemented</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>147</v>
+        <v>35</v>
       </c>
       <c r="F113" s="2"/>
     </row>
@@ -3495,7 +3495,7 @@
         <v>Implemented</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>41</v>
+        <v>332</v>
       </c>
       <c r="F114" s="2"/>
     </row>
@@ -3511,7 +3511,7 @@
         <v>Implemented</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F115" s="2"/>
     </row>
@@ -3527,7 +3527,7 @@
         <v>Implemented</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>301</v>
+        <v>234</v>
       </c>
       <c r="F116" s="2"/>
     </row>
@@ -3543,7 +3543,7 @@
         <v>Implemented</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F117" s="2"/>
     </row>
@@ -3559,7 +3559,7 @@
         <v>Implemented</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>152</v>
+        <v>299</v>
       </c>
       <c r="F118" s="2"/>
     </row>
@@ -3575,7 +3575,7 @@
         <v>Implemented</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="F119" s="2"/>
     </row>
@@ -3591,7 +3591,7 @@
         <v>Implemented</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="F120" s="2"/>
     </row>
@@ -3607,7 +3607,7 @@
         <v>Implemented</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="F121" s="2"/>
     </row>
@@ -3623,7 +3623,7 @@
         <v>Implemented</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>53</v>
+        <v>387</v>
       </c>
       <c r="F122" s="2"/>
     </row>
@@ -3639,7 +3639,7 @@
         <v>Implemented</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>245</v>
+        <v>41</v>
       </c>
       <c r="F123" s="2"/>
     </row>
@@ -3655,7 +3655,7 @@
         <v>Implemented</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>54</v>
+        <v>238</v>
       </c>
       <c r="F124" s="2"/>
     </row>
@@ -3671,7 +3671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>55</v>
+        <v>301</v>
       </c>
       <c r="F125" s="2"/>
     </row>
@@ -3687,7 +3687,7 @@
         <v>Implemented</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="F126" s="2"/>
     </row>
@@ -3703,7 +3703,7 @@
         <v>Implemented</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="F127" s="2"/>
     </row>
@@ -3719,7 +3719,7 @@
         <v>Implemented</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F128" s="2"/>
     </row>
@@ -3735,7 +3735,7 @@
         <v>Implemented</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>306</v>
+        <v>157</v>
       </c>
       <c r="F129" s="2"/>
     </row>
@@ -3751,7 +3751,7 @@
         <v>Implemented</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>249</v>
+        <v>52</v>
       </c>
       <c r="F130" s="2"/>
     </row>
@@ -3767,7 +3767,7 @@
         <v>Implemented</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>250</v>
+        <v>53</v>
       </c>
       <c r="F131" s="2"/>
     </row>
@@ -3783,7 +3783,7 @@
         <v>Implemented</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>163</v>
+        <v>245</v>
       </c>
       <c r="F132" s="2"/>
     </row>
@@ -3799,7 +3799,7 @@
         <v>Implemented</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>73</v>
+        <v>388</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -3815,7 +3815,7 @@
         <v>Implemented</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="F134" s="2"/>
     </row>
@@ -3831,7 +3831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>164</v>
+        <v>55</v>
       </c>
       <c r="F135" s="2"/>
     </row>
@@ -3847,7 +3847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>253</v>
+        <v>56</v>
       </c>
       <c r="F136" s="2"/>
     </row>
@@ -3863,7 +3863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -3879,7 +3879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -3895,7 +3895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -3911,7 +3911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>168</v>
+        <v>249</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -3927,7 +3927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>79</v>
+        <v>250</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -3943,7 +3943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -3959,7 +3959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F143" s="2"/>
     </row>
@@ -3975,7 +3975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>257</v>
+        <v>74</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -3991,7 +3991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>259</v>
+        <v>164</v>
       </c>
       <c r="F145" s="2"/>
     </row>
@@ -4007,7 +4007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="F146" s="2"/>
     </row>
@@ -4023,7 +4023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>263</v>
+        <v>76</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4039,7 +4039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4055,7 +4055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>311</v>
+        <v>255</v>
       </c>
       <c r="F149" s="2"/>
     </row>
@@ -4071,7 +4071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>312</v>
+        <v>168</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4086,7 +4086,7 @@
         <v>Implemented</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>Implemented</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>266</v>
+        <v>169</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4116,7 +4116,7 @@
         <v>Implemented</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4131,7 +4131,7 @@
         <v>Implemented</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>313</v>
+        <v>257</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4146,7 +4146,7 @@
         <v>Implemented</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>91</v>
+        <v>259</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
         <v>Implemented</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>93</v>
+        <v>262</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4176,7 +4176,7 @@
         <v>Implemented</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>94</v>
+        <v>263</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>95</v>
+        <v>173</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4206,7 +4206,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>269</v>
+        <v>311</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>178</v>
+        <v>312</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>270</v>
+        <v>89</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4251,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>179</v>
+        <v>266</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,7 +4296,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,7 +4326,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4356,7 +4356,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>318</v>
+        <v>269</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,7 +4371,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>274</v>
+        <v>178</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,7 +4386,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>106</v>
+        <v>270</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>110</v>
+        <v>179</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>187</v>
+        <v>98</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,7 +4431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>392</v>
+        <v>271</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4446,7 +4446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>190</v>
+        <v>100</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>322</v>
+        <v>101</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4491,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4506,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>196</v>
+        <v>318</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4521,7 +4521,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>197</v>
+        <v>274</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4536,7 +4536,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>278</v>
+        <v>106</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,7 +4551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>365</v>
+        <v>110</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,7 +4566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>366</v>
+        <v>187</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>367</v>
+        <v>392</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>393</v>
+        <v>189</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +4611,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>280</v>
+        <v>322</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +4641,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>281</v>
+        <v>195</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,7 +4656,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +4701,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>207</v>
+        <v>365</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4716,7 +4716,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>285</v>
+        <v>366</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4731,7 +4731,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4746,7 +4746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>378</v>
+        <v>393</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4761,7 +4761,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>287</v>
+        <v>199</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4776,7 +4776,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>208</v>
+        <v>280</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>209</v>
+        <v>281</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>385</v>
+        <v>201</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,7 +4821,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4836,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>212</v>
+        <v>282</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4851,7 +4851,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>288</v>
+        <v>207</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4866,7 +4866,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>213</v>
+        <v>285</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,7 +4881,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>118</v>
+        <v>377</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4896,7 +4896,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>125</v>
+        <v>378</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4911,7 +4911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4941,7 +4941,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>20</v>
+        <v>209</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4971,7 +4971,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>129</v>
+        <v>210</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,7 +4986,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>31</v>
+        <v>212</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,7 +5001,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>235</v>
+        <v>288</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5016,7 +5016,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5031,7 +5031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5061,7 +5061,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>59</v>
+        <v>291</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,7 +5076,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,7 +5091,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>248</v>
+        <v>21</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,7 +5121,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,7 +5136,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>309</v>
+        <v>31</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>78</v>
+        <v>235</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5166,7 +5166,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>175</v>
+        <v>239</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,7 +5181,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>182</v>
+        <v>57</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5211,7 +5211,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>324</v>
+        <v>59</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5226,7 +5226,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>373</v>
+        <v>60</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>221</v>
+        <v>65</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,7 +5256,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>297</v>
+        <v>248</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5271,7 +5271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>37</v>
+        <v>309</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5302,7 +5302,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>247</v>
+        <v>78</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5318,7 +5318,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>66</v>
+        <v>175</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5334,7 +5334,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>67</v>
+        <v>181</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5350,7 +5350,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5366,7 +5366,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>167</v>
+        <v>324</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5382,7 +5382,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>256</v>
+        <v>373</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5398,7 +5398,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>260</v>
+        <v>221</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5414,7 +5414,7 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>82</v>
+        <v>297</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5430,7 +5430,7 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5446,7 +5446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>310</v>
+        <v>37</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5462,7 +5462,7 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>84</v>
+        <v>247</v>
       </c>
       <c r="F242" s="2"/>
     </row>
@@ -5478,7 +5478,7 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="F243" s="2"/>
     </row>
@@ -5494,7 +5494,7 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="F244" s="2"/>
     </row>
@@ -5510,7 +5510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>319</v>
+        <v>161</v>
       </c>
       <c r="F245" s="2"/>
     </row>
@@ -5526,7 +5526,7 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>275</v>
+        <v>167</v>
       </c>
       <c r="F246" s="2"/>
     </row>
@@ -5542,7 +5542,7 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>108</v>
+        <v>256</v>
       </c>
       <c r="F247" s="2"/>
     </row>
@@ -5558,7 +5558,7 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>109</v>
+        <v>260</v>
       </c>
       <c r="F248" s="2"/>
     </row>
@@ -5574,7 +5574,7 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>188</v>
+        <v>82</v>
       </c>
       <c r="F249" s="2"/>
     </row>
@@ -5590,7 +5590,7 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>202</v>
+        <v>83</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5606,7 +5606,7 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>203</v>
+        <v>310</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5622,7 +5622,7 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5638,7 +5638,7 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="F253" s="2"/>
     </row>
@@ -5654,7 +5654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="F254" s="2"/>
     </row>
@@ -5670,7 +5670,7 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>128</v>
+        <v>319</v>
       </c>
       <c r="F255" s="2"/>
     </row>
@@ -5686,7 +5686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>224</v>
+        <v>275</v>
       </c>
       <c r="F256" s="2"/>
     </row>
@@ -5702,7 +5702,7 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F257" s="2"/>
     </row>
@@ -5718,7 +5718,7 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="F258" s="2"/>
     </row>
@@ -5734,7 +5734,7 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>36</v>
+        <v>188</v>
       </c>
       <c r="F259" s="2"/>
     </row>
@@ -5750,7 +5750,7 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>140</v>
+        <v>202</v>
       </c>
       <c r="F260" s="2"/>
     </row>
@@ -5766,7 +5766,7 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>148</v>
+        <v>203</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -5782,7 +5782,7 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -5798,7 +5798,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>246</v>
+        <v>17</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5814,7 +5814,7 @@
         <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>308</v>
+        <v>19</v>
       </c>
       <c r="F264" s="2"/>
     </row>
@@ -5830,7 +5830,7 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>261</v>
+        <v>128</v>
       </c>
       <c r="F265" s="2"/>
     </row>
@@ -5846,7 +5846,7 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>314</v>
+        <v>224</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -5862,7 +5862,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>268</v>
+        <v>133</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5875,10 +5875,10 @@
       </c>
       <c r="C268" t="str">
         <f>IF(COUNTIF(D:D,$A268)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>316</v>
+        <v>134</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5891,10 +5891,10 @@
       </c>
       <c r="C269" t="str">
         <f>IF(COUNTIF(D:D,$A269)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>104</v>
+        <v>36</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -5907,10 +5907,10 @@
       </c>
       <c r="C270" t="str">
         <f>IF(COUNTIF(D:D,$A270)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>186</v>
+        <v>140</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -5923,10 +5923,10 @@
       </c>
       <c r="C271" t="str">
         <f>IF(COUNTIF(D:D,$A271)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>112</v>
+        <v>333</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -5939,10 +5939,10 @@
       </c>
       <c r="C272" t="str">
         <f>IF(COUNTIF(D:D,$A272)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>277</v>
+        <v>148</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -5955,10 +5955,10 @@
       </c>
       <c r="C273" t="str">
         <f>IF(COUNTIF(D:D,$A273)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -5971,10 +5971,10 @@
       </c>
       <c r="C274" t="str">
         <f>IF(COUNTIF(D:D,$A274)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>362</v>
+        <v>246</v>
       </c>
       <c r="F274" s="2"/>
     </row>
@@ -5987,10 +5987,10 @@
       </c>
       <c r="C275" t="str">
         <f>IF(COUNTIF(D:D,$A275)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>375</v>
+        <v>308</v>
       </c>
       <c r="F275" s="2"/>
     </row>
@@ -6003,10 +6003,10 @@
       </c>
       <c r="C276" t="str">
         <f>IF(COUNTIF(D:D,$A276)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>9</v>
+        <v>261</v>
       </c>
       <c r="F276" s="2"/>
     </row>
@@ -6019,10 +6019,10 @@
       </c>
       <c r="C277" t="str">
         <f>IF(COUNTIF(D:D,$A277)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>214</v>
+        <v>314</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -6035,10 +6035,10 @@
       </c>
       <c r="C278" t="str">
         <f>IF(COUNTIF(D:D,$A278)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>23</v>
+        <v>268</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -6051,10 +6051,10 @@
       </c>
       <c r="C279" t="str">
         <f>IF(COUNTIF(D:D,$A279)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="F279" s="2"/>
     </row>
@@ -6070,7 +6070,7 @@
         <v>Missing</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>145</v>
+        <v>104</v>
       </c>
       <c r="F280" s="2"/>
     </row>
@@ -6086,7 +6086,7 @@
         <v>Missing</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>300</v>
+        <v>186</v>
       </c>
       <c r="F281" s="2"/>
     </row>
@@ -6102,7 +6102,7 @@
         <v>Missing</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="F282" s="2"/>
     </row>
@@ -6118,7 +6118,7 @@
         <v>Missing</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
       <c r="F283" s="2"/>
     </row>
@@ -6134,7 +6134,7 @@
         <v>Missing</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>242</v>
+        <v>113</v>
       </c>
       <c r="F284" s="2"/>
     </row>
@@ -6150,7 +6150,7 @@
         <v>Missing</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="F285" s="2"/>
     </row>
@@ -6166,7 +6166,7 @@
         <v>Missing</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>48</v>
+        <v>375</v>
       </c>
       <c r="F286" s="2"/>
     </row>
@@ -6182,7 +6182,7 @@
         <v>Missing</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="F287" s="2"/>
     </row>
@@ -6198,7 +6198,7 @@
         <v>Missing</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F288" s="2"/>
     </row>
@@ -6214,7 +6214,7 @@
         <v>Missing</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="F289" s="2"/>
     </row>
@@ -6230,7 +6230,7 @@
         <v>Missing</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>254</v>
+        <v>23</v>
       </c>
       <c r="F290" s="2"/>
     </row>
@@ -6246,7 +6246,7 @@
         <v>Missing</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>166</v>
+        <v>298</v>
       </c>
       <c r="F291" s="2"/>
     </row>
@@ -6262,7 +6262,7 @@
         <v>Missing</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>400</v>
+        <v>145</v>
       </c>
       <c r="F292" s="2"/>
     </row>
@@ -6278,7 +6278,7 @@
         <v>Missing</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>258</v>
+        <v>300</v>
       </c>
       <c r="F293" s="2"/>
     </row>
@@ -6294,7 +6294,7 @@
         <v>Missing</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="F294" s="2"/>
     </row>
@@ -6310,7 +6310,7 @@
         <v>Missing</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>198</v>
+        <v>302</v>
       </c>
       <c r="F295" s="2"/>
     </row>
@@ -6326,7 +6326,7 @@
         <v>Missing</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>371</v>
+        <v>242</v>
       </c>
       <c r="F296" s="2"/>
     </row>
@@ -6342,7 +6342,7 @@
         <v>Missing</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>205</v>
+        <v>45</v>
       </c>
       <c r="F297" s="2"/>
     </row>
@@ -6358,7 +6358,7 @@
         <v>Missing</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>383</v>
+        <v>48</v>
       </c>
       <c r="F298" s="2"/>
     </row>
@@ -6374,7 +6374,7 @@
         <v>Missing</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>384</v>
+        <v>155</v>
       </c>
       <c r="F299" s="2"/>
     </row>
@@ -6390,7 +6390,7 @@
         <v>Missing</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>292</v>
+        <v>50</v>
       </c>
       <c r="F300" s="2"/>
     </row>
@@ -6406,7 +6406,7 @@
         <v>Missing</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>130</v>
+        <v>64</v>
       </c>
       <c r="F301" s="2"/>
     </row>
@@ -6422,7 +6422,7 @@
         <v>Missing</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>33</v>
+        <v>254</v>
       </c>
       <c r="F302" s="2"/>
     </row>
@@ -6438,7 +6438,7 @@
         <v>Implemented</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="F303" s="2"/>
     </row>
@@ -6454,7 +6454,7 @@
         <v>Implemented</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>236</v>
+        <v>400</v>
       </c>
       <c r="F304" s="2"/>
     </row>
@@ -6470,7 +6470,7 @@
         <v>Implemented</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>39</v>
+        <v>258</v>
       </c>
       <c r="F305" s="2"/>
     </row>
@@ -6486,7 +6486,7 @@
         <v>Implemented</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="F306" s="2"/>
     </row>
@@ -6502,7 +6502,7 @@
         <v>Implemented</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="F307" s="2"/>
     </row>
@@ -6518,7 +6518,7 @@
         <v>Implemented</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>153</v>
+        <v>371</v>
       </c>
       <c r="F308" s="2"/>
     </row>
@@ -6534,7 +6534,7 @@
         <v>Implemented</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>62</v>
+        <v>205</v>
       </c>
       <c r="F309" s="2"/>
     </row>
@@ -6550,7 +6550,7 @@
         <v>Implemented</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>87</v>
+        <v>383</v>
       </c>
       <c r="F310" s="2"/>
     </row>
@@ -6566,7 +6566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>315</v>
+        <v>384</v>
       </c>
       <c r="F311" s="2"/>
     </row>
@@ -6582,7 +6582,7 @@
         <v>Implemented</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>177</v>
+        <v>292</v>
       </c>
       <c r="F312" s="2"/>
     </row>
@@ -6598,7 +6598,7 @@
         <v>Implemented</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="F313" s="2"/>
     </row>
@@ -6614,7 +6614,7 @@
         <v>Implemented</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>185</v>
+        <v>33</v>
       </c>
       <c r="F314" s="2"/>
     </row>
@@ -6630,7 +6630,7 @@
         <v>Implemented</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="F315" s="2"/>
     </row>
@@ -6646,7 +6646,7 @@
         <v>Implemented</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>276</v>
+        <v>236</v>
       </c>
       <c r="F316" s="2"/>
     </row>
@@ -6662,7 +6662,7 @@
         <v>Implemented</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>397</v>
+        <v>39</v>
       </c>
       <c r="F317" s="2"/>
     </row>
@@ -6678,7 +6678,7 @@
         <v>Implemented</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="F318" s="2"/>
     </row>
@@ -6694,7 +6694,7 @@
         <v>Implemented</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>368</v>
+        <v>241</v>
       </c>
       <c r="F319" s="2"/>
     </row>
@@ -6710,7 +6710,7 @@
         <v>Implemented</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>200</v>
+        <v>153</v>
       </c>
       <c r="F320" s="2"/>
     </row>
@@ -6726,7 +6726,7 @@
         <v>Implemented</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>325</v>
+        <v>62</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -6742,7 +6742,7 @@
         <v>Implemented</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>286</v>
+        <v>87</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6758,7 +6758,7 @@
         <v>Implemented</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>376</v>
+        <v>315</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6774,7 +6774,7 @@
         <v>Implemented</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>124</v>
+        <v>177</v>
       </c>
       <c r="F324" s="2"/>
     </row>
@@ -6790,7 +6790,7 @@
         <v>Implemented</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
@@ -6805,7 +6805,7 @@
         <v>Implemented</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>220</v>
+        <v>185</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
@@ -6820,7 +6820,7 @@
         <v>Implemented</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -6835,7 +6835,7 @@
         <v>Implemented</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
@@ -6850,7 +6850,7 @@
         <v>Implemented</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>27</v>
+        <v>397</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -6865,7 +6865,7 @@
         <v>Implemented</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
@@ -6880,7 +6880,7 @@
         <v>Implemented</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>230</v>
+        <v>368</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -6895,7 +6895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>136</v>
+        <v>200</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
@@ -6910,7 +6910,7 @@
         <v>Implemented</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>42</v>
+        <v>325</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
@@ -6925,7 +6925,7 @@
         <v>Implemented</v>
       </c>
       <c r="D334" s="2" t="s">
-        <v>44</v>
+        <v>286</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
@@ -6940,7 +6940,7 @@
         <v>Implemented</v>
       </c>
       <c r="D335" s="2" t="s">
-        <v>244</v>
+        <v>376</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
@@ -6955,7 +6955,7 @@
         <v>Implemented</v>
       </c>
       <c r="D336" s="2" t="s">
-        <v>305</v>
+        <v>124</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -6970,7 +6970,7 @@
         <v>Implemented</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>334</v>
+        <v>15</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -6985,7 +6985,7 @@
         <v>Implemented</v>
       </c>
       <c r="D338" s="2" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -7000,7 +7000,7 @@
         <v>Implemented</v>
       </c>
       <c r="D339" s="2" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -7015,7 +7015,7 @@
         <v>Implemented</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>77</v>
+        <v>296</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -7030,7 +7030,7 @@
         <v>Implemented</v>
       </c>
       <c r="D341" s="2" t="s">
-        <v>265</v>
+        <v>27</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -7045,7 +7045,7 @@
         <v>Implemented</v>
       </c>
       <c r="D342" s="2" t="s">
-        <v>180</v>
+        <v>30</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -7060,7 +7060,7 @@
         <v>Implemented</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>111</v>
+        <v>230</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -7075,7 +7075,7 @@
         <v>Implemented</v>
       </c>
       <c r="D344" s="2" t="s">
-        <v>320</v>
+        <v>136</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -7090,7 +7090,7 @@
         <v>Implemented</v>
       </c>
       <c r="D345" s="2" t="s">
-        <v>191</v>
+        <v>42</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
@@ -7105,7 +7105,7 @@
         <v>Implemented</v>
       </c>
       <c r="D346" s="2" t="s">
-        <v>283</v>
+        <v>44</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
@@ -7120,7 +7120,7 @@
         <v>Implemented</v>
       </c>
       <c r="D347" s="2" t="s">
-        <v>379</v>
+        <v>244</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
@@ -7135,7 +7135,7 @@
         <v>Implemented</v>
       </c>
       <c r="D348" s="2" t="s">
-        <v>381</v>
+        <v>305</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -7150,7 +7150,7 @@
         <v>Implemented</v>
       </c>
       <c r="D349" s="2" t="s">
-        <v>32</v>
+        <v>334</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
@@ -7165,7 +7165,7 @@
         <v>Implemented</v>
       </c>
       <c r="D350" s="2" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
@@ -7180,7 +7180,7 @@
         <v>Implemented</v>
       </c>
       <c r="D351" s="2" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -7195,7 +7195,7 @@
         <v>Implemented</v>
       </c>
       <c r="D352" s="2" t="s">
-        <v>245</v>
+        <v>77</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
@@ -7210,7 +7210,7 @@
         <v>Implemented</v>
       </c>
       <c r="D353" s="2" t="s">
-        <v>198</v>
+        <v>265</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
@@ -7225,7 +7225,7 @@
         <v>Implemented</v>
       </c>
       <c r="D354" s="2" t="s">
-        <v>394</v>
+        <v>180</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
@@ -7240,7 +7240,7 @@
         <v>Implemented</v>
       </c>
       <c r="D355" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
@@ -7255,7 +7255,7 @@
         <v>Implemented</v>
       </c>
       <c r="D356" s="2" t="s">
-        <v>44</v>
+        <v>320</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
@@ -7270,7 +7270,7 @@
         <v>Implemented</v>
       </c>
       <c r="D357" s="2" t="s">
-        <v>63</v>
+        <v>191</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
@@ -7285,7 +7285,7 @@
         <v>Implemented</v>
       </c>
       <c r="D358" s="2" t="s">
-        <v>122</v>
+        <v>283</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -7300,7 +7300,7 @@
         <v>Implemented</v>
       </c>
       <c r="D359" s="2" t="s">
-        <v>228</v>
+        <v>379</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -7315,7 +7315,7 @@
         <v>Implemented</v>
       </c>
       <c r="D360" s="2" t="s">
-        <v>154</v>
+        <v>381</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
@@ -7330,7 +7330,7 @@
         <v>Implemented</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>173</v>
+        <v>32</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
@@ -7345,7 +7345,7 @@
         <v>Implemented</v>
       </c>
       <c r="D362" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
@@ -7360,7 +7360,7 @@
         <v>Implemented</v>
       </c>
       <c r="D363" s="2" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
@@ -7375,7 +7375,7 @@
         <v>Implemented</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
@@ -7390,7 +7390,7 @@
         <v>Implemented</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>133</v>
+        <v>198</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
@@ -7405,7 +7405,7 @@
         <v>Implemented</v>
       </c>
       <c r="D366" s="2" t="s">
-        <v>134</v>
+        <v>394</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
@@ -7420,7 +7420,7 @@
         <v>Implemented</v>
       </c>
       <c r="D367" s="2" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -7435,7 +7435,7 @@
         <v>Implemented</v>
       </c>
       <c r="D368" s="2" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -7450,7 +7450,7 @@
         <v>Implemented</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7464,6 +7464,9 @@
         <f>IF(COUNTIF(D:D,$A370)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D370" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
@@ -7476,6 +7479,9 @@
         <f>IF(COUNTIF(D:D,$A371)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D371" s="2" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
@@ -7489,7 +7495,7 @@
         <v>Implemented</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
@@ -7504,7 +7510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D373" s="2" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
@@ -7519,7 +7525,7 @@
         <v>Implemented</v>
       </c>
       <c r="D374" s="2" t="s">
-        <v>234</v>
+        <v>150</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -7534,7 +7540,7 @@
         <v>Implemented</v>
       </c>
       <c r="D375" s="2" t="s">
-        <v>106</v>
+        <v>161</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -7548,6 +7554,9 @@
         <f>IF(COUNTIF(D:D,$A376)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D376" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
@@ -7560,6 +7569,9 @@
         <f>IF(COUNTIF(D:D,$A377)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D377" s="2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
@@ -7572,6 +7584,9 @@
         <f>IF(COUNTIF(D:D,$A378)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D378" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
@@ -7584,6 +7599,9 @@
         <f>IF(COUNTIF(D:D,$A379)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D379" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
@@ -7596,6 +7614,9 @@
         <f>IF(COUNTIF(D:D,$A380)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D380" s="2" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
@@ -7608,6 +7629,9 @@
         <f>IF(COUNTIF(D:D,$A381)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D381" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
@@ -7633,123 +7657,143 @@
         <v>Implemented</v>
       </c>
     </row>
-    <row r="408" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D408" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="409" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D409" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="410" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D410" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="411" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D411" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="412" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D412" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="413" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D413" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="414" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D414" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="415" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D415" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="416" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D416" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D417" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D418" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D419" s="2" t="s">
-        <v>156</v>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D384" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="385" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D385" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="386" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D386" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="387" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D387" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="420" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D420" s="2" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="421" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D421" s="2" t="s">
-        <v>253</v>
+        <v>31</v>
       </c>
     </row>
     <row r="422" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D422" s="2" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
     </row>
     <row r="423" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D423" s="2" t="s">
-        <v>167</v>
+        <v>66</v>
       </c>
     </row>
     <row r="424" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D424" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="425" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D425" s="2" t="s">
-        <v>155</v>
+        <v>54</v>
       </c>
     </row>
     <row r="426" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D426" s="2" t="s">
-        <v>227</v>
+        <v>57</v>
       </c>
     </row>
     <row r="427" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D427" s="2" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
     </row>
     <row r="428" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D428" s="2" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
     </row>
     <row r="429" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D429" s="2" t="s">
-        <v>238</v>
+        <v>144</v>
       </c>
     </row>
     <row r="430" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D430" s="2" t="s">
-        <v>366</v>
+        <v>382</v>
       </c>
     </row>
     <row r="431" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D431" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D432" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D433" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D434" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D435" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D436" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D437" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D438" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D439" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D440" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D441" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D442" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D443" s="2" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- refactored how SpellPower is applied and calculated - fixed some bugs with untested cards like Blizzard, Blade Flurry and Defias Ringleader - Minions with instant kill mechanic no longer work on heroes - implemented the following legendary cards: Lorewalker Cho, Malygos, Millhouse Manastorm, Nat Pagle, Nozdormu, Old Murk-Eye, Onyxia, Prophet Velen and Lord Jaraxxus
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$360</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$367</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="401">
   <si>
     <t>Cardname</t>
   </si>
@@ -1605,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K443"/>
+  <dimension ref="A1:K450"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="A279" sqref="A279"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C284" sqref="C284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2311,7 +2311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>264</v>
+        <v>339</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -2327,7 +2327,7 @@
         <v>Implemented</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>88</v>
+        <v>264</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -2343,7 +2343,7 @@
         <v>Implemented</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>273</v>
+        <v>88</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -2359,7 +2359,7 @@
         <v>Implemented</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>184</v>
+        <v>273</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -2375,7 +2375,7 @@
         <v>Implemented</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>321</v>
+        <v>184</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -2391,7 +2391,7 @@
         <v>Implemented</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>192</v>
+        <v>321</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -2407,7 +2407,7 @@
         <v>Implemented</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>364</v>
+        <v>192</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -2423,7 +2423,7 @@
         <v>Implemented</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -2439,7 +2439,7 @@
         <v>Implemented</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -2455,7 +2455,7 @@
         <v>Implemented</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -2471,7 +2471,7 @@
         <v>Implemented</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>206</v>
+        <v>374</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -2487,7 +2487,7 @@
         <v>Implemented</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>11</v>
+        <v>206</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -2503,7 +2503,7 @@
         <v>Implemented</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -2519,7 +2519,7 @@
         <v>Implemented</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -2535,7 +2535,7 @@
         <v>Implemented</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>326</v>
+        <v>13</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -2551,7 +2551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>226</v>
+        <v>326</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -2567,7 +2567,7 @@
         <v>Implemented</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>135</v>
+        <v>226</v>
       </c>
       <c r="F56" s="2"/>
     </row>
@@ -2583,7 +2583,7 @@
         <v>Implemented</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>231</v>
+        <v>135</v>
       </c>
       <c r="F57" s="2"/>
     </row>
@@ -2599,7 +2599,7 @@
         <v>Implemented</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>399</v>
+        <v>231</v>
       </c>
       <c r="F58" s="2"/>
     </row>
@@ -2615,7 +2615,7 @@
         <v>Implemented</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>46</v>
+        <v>399</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -2631,7 +2631,7 @@
         <v>Implemented</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -2647,7 +2647,7 @@
         <v>Implemented</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -2663,7 +2663,7 @@
         <v>Implemented</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F62" s="2"/>
     </row>
@@ -2679,7 +2679,7 @@
         <v>Implemented</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>159</v>
+        <v>49</v>
       </c>
       <c r="F63" s="2"/>
     </row>
@@ -2695,7 +2695,7 @@
         <v>Implemented</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>307</v>
+        <v>159</v>
       </c>
       <c r="F64" s="2"/>
     </row>
@@ -2711,7 +2711,7 @@
         <v>Implemented</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>160</v>
+        <v>307</v>
       </c>
       <c r="F65" s="2"/>
     </row>
@@ -2727,7 +2727,7 @@
         <v>Implemented</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>252</v>
+        <v>160</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -2743,7 +2743,7 @@
         <v>Implemented</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>170</v>
+        <v>252</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -2759,7 +2759,7 @@
         <v>Implemented</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F68" s="2"/>
     </row>
@@ -2775,7 +2775,7 @@
         <v>Implemented</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>85</v>
+        <v>172</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -2791,7 +2791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F70" s="2"/>
     </row>
@@ -2807,7 +2807,7 @@
         <v>Implemented</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>317</v>
+        <v>96</v>
       </c>
       <c r="F71" s="2"/>
     </row>
@@ -2823,7 +2823,7 @@
         <v>Implemented</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>193</v>
+        <v>317</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -2839,7 +2839,7 @@
         <v>Implemented</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>323</v>
+        <v>193</v>
       </c>
       <c r="F73" s="2"/>
     </row>
@@ -2855,7 +2855,7 @@
         <v>Implemented</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>284</v>
+        <v>323</v>
       </c>
       <c r="F74" s="2"/>
     </row>
@@ -2871,7 +2871,7 @@
         <v>Implemented</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>380</v>
+        <v>284</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -2887,7 +2887,7 @@
         <v>Implemented</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>115</v>
+        <v>380</v>
       </c>
       <c r="F76" s="2"/>
     </row>
@@ -2903,7 +2903,7 @@
         <v>Implemented</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F77" s="2"/>
     </row>
@@ -2919,7 +2919,7 @@
         <v>Implemented</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>3</v>
+        <v>121</v>
       </c>
       <c r="F78" s="2"/>
     </row>
@@ -2935,7 +2935,7 @@
         <v>Implemented</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>122</v>
+        <v>3</v>
       </c>
       <c r="F79" s="2"/>
     </row>
@@ -2951,7 +2951,7 @@
         <v>Implemented</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>398</v>
+        <v>122</v>
       </c>
       <c r="F80" s="2"/>
     </row>
@@ -2967,7 +2967,7 @@
         <v>Implemented</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>119</v>
+        <v>398</v>
       </c>
       <c r="F81" s="2"/>
     </row>
@@ -2983,7 +2983,7 @@
         <v>Implemented</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F82" s="2"/>
     </row>
@@ -2999,7 +2999,7 @@
         <v>Implemented</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F83" s="2"/>
     </row>
@@ -3015,7 +3015,7 @@
         <v>Implemented</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>215</v>
+        <v>123</v>
       </c>
       <c r="F84" s="2"/>
     </row>
@@ -3031,7 +3031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F85" s="2"/>
     </row>
@@ -3047,7 +3047,7 @@
         <v>Implemented</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F86" s="2"/>
     </row>
@@ -3063,7 +3063,7 @@
         <v>Implemented</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F87" s="2"/>
     </row>
@@ -3079,7 +3079,7 @@
         <v>Implemented</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>16</v>
+        <v>218</v>
       </c>
       <c r="F88" s="2"/>
     </row>
@@ -3095,7 +3095,7 @@
         <v>Implemented</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>219</v>
+        <v>16</v>
       </c>
       <c r="F89" s="2"/>
     </row>
@@ -3111,7 +3111,7 @@
         <v>Implemented</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>126</v>
+        <v>219</v>
       </c>
       <c r="F90" s="2"/>
     </row>
@@ -3127,7 +3127,7 @@
         <v>Implemented</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>222</v>
+        <v>126</v>
       </c>
       <c r="F91" s="2"/>
     </row>
@@ -3143,7 +3143,7 @@
         <v>Implemented</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>327</v>
+        <v>222</v>
       </c>
       <c r="F92" s="2"/>
     </row>
@@ -3159,7 +3159,7 @@
         <v>Implemented</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>294</v>
+        <v>327</v>
       </c>
       <c r="F93" s="2"/>
     </row>
@@ -3175,7 +3175,7 @@
         <v>Implemented</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>22</v>
+        <v>294</v>
       </c>
       <c r="F94" s="2"/>
     </row>
@@ -3191,7 +3191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>295</v>
+        <v>22</v>
       </c>
       <c r="F95" s="2"/>
     </row>
@@ -3207,7 +3207,7 @@
         <v>Implemented</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>328</v>
+        <v>295</v>
       </c>
       <c r="F96" s="2"/>
     </row>
@@ -3223,7 +3223,7 @@
         <v>Implemented</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>227</v>
+        <v>328</v>
       </c>
       <c r="F97" s="2"/>
     </row>
@@ -3239,7 +3239,7 @@
         <v>Implemented</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>131</v>
+        <v>227</v>
       </c>
       <c r="F98" s="2"/>
     </row>
@@ -3255,7 +3255,7 @@
         <v>Implemented</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="F99" s="2"/>
     </row>
@@ -3271,7 +3271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F100" s="2"/>
     </row>
@@ -3287,7 +3287,7 @@
         <v>Implemented</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F101" s="2"/>
     </row>
@@ -3303,7 +3303,7 @@
         <v>Implemented</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>329</v>
+        <v>26</v>
       </c>
       <c r="F102" s="2"/>
     </row>
@@ -3319,7 +3319,7 @@
         <v>Implemented</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F103" s="2"/>
     </row>
@@ -3335,7 +3335,7 @@
         <v>Implemented</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>389</v>
+        <v>330</v>
       </c>
       <c r="F104" s="2"/>
     </row>
@@ -3351,7 +3351,7 @@
         <v>Implemented</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>28</v>
+        <v>389</v>
       </c>
       <c r="F105" s="2"/>
     </row>
@@ -3367,7 +3367,7 @@
         <v>Implemented</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>228</v>
+        <v>28</v>
       </c>
       <c r="F106" s="2"/>
     </row>
@@ -3383,7 +3383,7 @@
         <v>Implemented</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F107" s="2"/>
     </row>
@@ -3399,7 +3399,7 @@
         <v>Implemented</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>32</v>
+        <v>229</v>
       </c>
       <c r="F108" s="2"/>
     </row>
@@ -3415,7 +3415,7 @@
         <v>Implemented</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>232</v>
+        <v>32</v>
       </c>
       <c r="F109" s="2"/>
     </row>
@@ -3431,7 +3431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>137</v>
+        <v>232</v>
       </c>
       <c r="F110" s="2"/>
     </row>
@@ -3447,7 +3447,7 @@
         <v>Implemented</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
       <c r="F111" s="2"/>
     </row>
@@ -3463,7 +3463,7 @@
         <v>Implemented</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="F112" s="2"/>
     </row>
@@ -3479,7 +3479,7 @@
         <v>Implemented</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>35</v>
+        <v>138</v>
       </c>
       <c r="F113" s="2"/>
     </row>
@@ -3495,7 +3495,7 @@
         <v>Implemented</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>332</v>
+        <v>35</v>
       </c>
       <c r="F114" s="2"/>
     </row>
@@ -3511,7 +3511,7 @@
         <v>Implemented</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>233</v>
+        <v>332</v>
       </c>
       <c r="F115" s="2"/>
     </row>
@@ -3527,7 +3527,7 @@
         <v>Implemented</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F116" s="2"/>
     </row>
@@ -3543,7 +3543,7 @@
         <v>Implemented</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>142</v>
+        <v>234</v>
       </c>
       <c r="F117" s="2"/>
     </row>
@@ -3559,7 +3559,7 @@
         <v>Implemented</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>299</v>
+        <v>142</v>
       </c>
       <c r="F118" s="2"/>
     </row>
@@ -3575,7 +3575,7 @@
         <v>Implemented</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>38</v>
+        <v>299</v>
       </c>
       <c r="F119" s="2"/>
     </row>
@@ -3591,7 +3591,7 @@
         <v>Implemented</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="F120" s="2"/>
     </row>
@@ -3607,7 +3607,7 @@
         <v>Implemented</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F121" s="2"/>
     </row>
@@ -3623,7 +3623,7 @@
         <v>Implemented</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>387</v>
+        <v>147</v>
       </c>
       <c r="F122" s="2"/>
     </row>
@@ -3639,7 +3639,7 @@
         <v>Implemented</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>41</v>
+        <v>387</v>
       </c>
       <c r="F123" s="2"/>
     </row>
@@ -3655,7 +3655,7 @@
         <v>Implemented</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>238</v>
+        <v>41</v>
       </c>
       <c r="F124" s="2"/>
     </row>
@@ -3671,7 +3671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>301</v>
+        <v>238</v>
       </c>
       <c r="F125" s="2"/>
     </row>
@@ -3687,7 +3687,7 @@
         <v>Implemented</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>151</v>
+        <v>301</v>
       </c>
       <c r="F126" s="2"/>
     </row>
@@ -3703,7 +3703,7 @@
         <v>Implemented</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F127" s="2"/>
     </row>
@@ -3719,7 +3719,7 @@
         <v>Implemented</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F128" s="2"/>
     </row>
@@ -3735,7 +3735,7 @@
         <v>Implemented</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F129" s="2"/>
     </row>
@@ -3751,7 +3751,7 @@
         <v>Implemented</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>52</v>
+        <v>157</v>
       </c>
       <c r="F130" s="2"/>
     </row>
@@ -3767,7 +3767,7 @@
         <v>Implemented</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F131" s="2"/>
     </row>
@@ -3783,7 +3783,7 @@
         <v>Implemented</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>245</v>
+        <v>53</v>
       </c>
       <c r="F132" s="2"/>
     </row>
@@ -3799,7 +3799,7 @@
         <v>Implemented</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>388</v>
+        <v>245</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -3815,7 +3815,7 @@
         <v>Implemented</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>54</v>
+        <v>388</v>
       </c>
       <c r="F134" s="2"/>
     </row>
@@ -3831,7 +3831,7 @@
         <v>Implemented</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F135" s="2"/>
     </row>
@@ -3847,7 +3847,7 @@
         <v>Implemented</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F136" s="2"/>
     </row>
@@ -3863,7 +3863,7 @@
         <v>Implemented</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -3879,7 +3879,7 @@
         <v>Implemented</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>158</v>
+        <v>335</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -3895,7 +3895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>306</v>
+        <v>58</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -3911,7 +3911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>249</v>
+        <v>336</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -3927,7 +3927,7 @@
         <v>Implemented</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>250</v>
+        <v>158</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -3943,7 +3943,7 @@
         <v>Implemented</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>163</v>
+        <v>337</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -3959,7 +3959,7 @@
         <v>Implemented</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>73</v>
+        <v>306</v>
       </c>
       <c r="F143" s="2"/>
     </row>
@@ -3975,7 +3975,7 @@
         <v>Implemented</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>74</v>
+        <v>338</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -3991,7 +3991,7 @@
         <v>Implemented</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>164</v>
+        <v>249</v>
       </c>
       <c r="F145" s="2"/>
     </row>
@@ -4007,7 +4007,7 @@
         <v>Implemented</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F146" s="2"/>
     </row>
@@ -4023,7 +4023,7 @@
         <v>Implemented</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>76</v>
+        <v>163</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4039,7 +4039,7 @@
         <v>Implemented</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>165</v>
+        <v>73</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4055,7 +4055,7 @@
         <v>Implemented</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>255</v>
+        <v>74</v>
       </c>
       <c r="F149" s="2"/>
     </row>
@@ -4071,7 +4071,7 @@
         <v>Implemented</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4086,7 +4086,7 @@
         <v>Implemented</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>79</v>
+        <v>340</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>Implemented</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>169</v>
+        <v>253</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4116,7 +4116,7 @@
         <v>Implemented</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4131,7 +4131,7 @@
         <v>Implemented</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>257</v>
+        <v>341</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4146,7 +4146,7 @@
         <v>Implemented</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>259</v>
+        <v>165</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
         <v>Implemented</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4176,7 +4176,7 @@
         <v>Implemented</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>263</v>
+        <v>168</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
         <v>Implemented</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>173</v>
+        <v>79</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4206,7 +4206,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>311</v>
+        <v>169</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>312</v>
+        <v>80</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>89</v>
+        <v>257</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4251,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>90</v>
+        <v>262</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>313</v>
+        <v>263</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,7 +4296,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>91</v>
+        <v>173</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>93</v>
+        <v>311</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,7 +4326,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>94</v>
+        <v>312</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4356,7 +4356,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,7 +4371,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>178</v>
+        <v>90</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,7 +4386,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>270</v>
+        <v>313</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>179</v>
+        <v>91</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,7 +4431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>271</v>
+        <v>94</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4446,7 +4446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>100</v>
+        <v>269</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>101</v>
+        <v>178</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4491,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>183</v>
+        <v>270</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4506,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>318</v>
+        <v>179</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4521,7 +4521,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>274</v>
+        <v>98</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4536,7 +4536,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>106</v>
+        <v>271</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,7 +4551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,7 +4566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>187</v>
+        <v>100</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>392</v>
+        <v>101</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +4611,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>322</v>
+        <v>274</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +4641,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>195</v>
+        <v>106</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,7 +4656,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>278</v>
+        <v>392</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +4701,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>365</v>
+        <v>189</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4716,7 +4716,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>366</v>
+        <v>190</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4731,7 +4731,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>367</v>
+        <v>322</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4746,7 +4746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>393</v>
+        <v>195</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4761,7 +4761,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4776,7 +4776,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>280</v>
+        <v>197</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>201</v>
+        <v>365</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,7 +4821,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>204</v>
+        <v>366</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4836,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>282</v>
+        <v>367</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4851,7 +4851,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>207</v>
+        <v>393</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4866,7 +4866,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>285</v>
+        <v>199</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,7 +4881,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>377</v>
+        <v>280</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4896,7 +4896,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>378</v>
+        <v>281</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4911,7 +4911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>287</v>
+        <v>201</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4941,7 +4941,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>209</v>
+        <v>282</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>385</v>
+        <v>207</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4971,7 +4971,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>210</v>
+        <v>285</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,7 +4986,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>212</v>
+        <v>377</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,7 +5001,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>288</v>
+        <v>378</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5016,7 +5016,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>213</v>
+        <v>287</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5031,7 +5031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>118</v>
+        <v>208</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>125</v>
+        <v>209</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5061,7 +5061,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>291</v>
+        <v>385</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,7 +5076,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,7 +5091,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>20</v>
+        <v>212</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>21</v>
+        <v>288</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,7 +5121,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>129</v>
+        <v>213</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,7 +5136,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>235</v>
+        <v>125</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5166,7 +5166,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>239</v>
+        <v>291</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,7 +5181,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>150</v>
+        <v>225</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5211,7 +5211,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5226,7 +5226,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,7 +5256,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5271,7 +5271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>69</v>
+        <v>239</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>309</v>
+        <v>150</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5302,7 +5302,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5318,7 +5318,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5334,7 +5334,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5350,7 +5350,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5366,7 +5366,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>324</v>
+        <v>248</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5382,7 +5382,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>373</v>
+        <v>69</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5398,7 +5398,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>221</v>
+        <v>309</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5414,7 +5414,7 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>297</v>
+        <v>78</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5430,7 +5430,7 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5446,7 +5446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>37</v>
+        <v>181</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5462,7 +5462,7 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>247</v>
+        <v>182</v>
       </c>
       <c r="F242" s="2"/>
     </row>
@@ -5478,7 +5478,7 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>66</v>
+        <v>324</v>
       </c>
       <c r="F243" s="2"/>
     </row>
@@ -5494,7 +5494,7 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>67</v>
+        <v>373</v>
       </c>
       <c r="F244" s="2"/>
     </row>
@@ -5510,7 +5510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>161</v>
+        <v>221</v>
       </c>
       <c r="F245" s="2"/>
     </row>
@@ -5526,7 +5526,7 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>167</v>
+        <v>297</v>
       </c>
       <c r="F246" s="2"/>
     </row>
@@ -5542,7 +5542,7 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="F247" s="2"/>
     </row>
@@ -5558,7 +5558,7 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>260</v>
+        <v>37</v>
       </c>
       <c r="F248" s="2"/>
     </row>
@@ -5574,7 +5574,7 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>82</v>
+        <v>247</v>
       </c>
       <c r="F249" s="2"/>
     </row>
@@ -5590,7 +5590,7 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5606,7 +5606,7 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>310</v>
+        <v>67</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5622,7 +5622,7 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5638,7 +5638,7 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>92</v>
+        <v>167</v>
       </c>
       <c r="F253" s="2"/>
     </row>
@@ -5654,7 +5654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>97</v>
+        <v>256</v>
       </c>
       <c r="F254" s="2"/>
     </row>
@@ -5670,7 +5670,7 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>319</v>
+        <v>260</v>
       </c>
       <c r="F255" s="2"/>
     </row>
@@ -5686,7 +5686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>275</v>
+        <v>82</v>
       </c>
       <c r="F256" s="2"/>
     </row>
@@ -5702,7 +5702,7 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="F257" s="2"/>
     </row>
@@ -5718,7 +5718,7 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>109</v>
+        <v>310</v>
       </c>
       <c r="F258" s="2"/>
     </row>
@@ -5734,7 +5734,7 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>188</v>
+        <v>84</v>
       </c>
       <c r="F259" s="2"/>
     </row>
@@ -5750,7 +5750,7 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>202</v>
+        <v>92</v>
       </c>
       <c r="F260" s="2"/>
     </row>
@@ -5766,7 +5766,7 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>203</v>
+        <v>97</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -5782,7 +5782,7 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>18</v>
+        <v>319</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -5798,7 +5798,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>17</v>
+        <v>275</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5814,7 +5814,7 @@
         <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="F264" s="2"/>
     </row>
@@ -5830,7 +5830,7 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="F265" s="2"/>
     </row>
@@ -5846,7 +5846,7 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -5862,7 +5862,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>133</v>
+        <v>202</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5878,7 +5878,7 @@
         <v>Implemented</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>134</v>
+        <v>203</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5894,7 +5894,7 @@
         <v>Implemented</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -5910,7 +5910,7 @@
         <v>Implemented</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -5926,7 +5926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>333</v>
+        <v>19</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -5942,7 +5942,7 @@
         <v>Implemented</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -5958,7 +5958,7 @@
         <v>Implemented</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>43</v>
+        <v>224</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -5974,7 +5974,7 @@
         <v>Implemented</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>246</v>
+        <v>133</v>
       </c>
       <c r="F274" s="2"/>
     </row>
@@ -5990,7 +5990,7 @@
         <v>Implemented</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>308</v>
+        <v>134</v>
       </c>
       <c r="F275" s="2"/>
     </row>
@@ -6006,7 +6006,7 @@
         <v>Implemented</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>261</v>
+        <v>36</v>
       </c>
       <c r="F276" s="2"/>
     </row>
@@ -6022,7 +6022,7 @@
         <v>Implemented</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>314</v>
+        <v>140</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -6038,7 +6038,7 @@
         <v>Implemented</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>268</v>
+        <v>333</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -6054,7 +6054,7 @@
         <v>Implemented</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>316</v>
+        <v>148</v>
       </c>
       <c r="F279" s="2"/>
     </row>
@@ -6067,10 +6067,10 @@
       </c>
       <c r="C280" t="str">
         <f>IF(COUNTIF(D:D,$A280)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
       <c r="F280" s="2"/>
     </row>
@@ -6083,10 +6083,10 @@
       </c>
       <c r="C281" t="str">
         <f>IF(COUNTIF(D:D,$A281)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>186</v>
+        <v>246</v>
       </c>
       <c r="F281" s="2"/>
     </row>
@@ -6099,10 +6099,10 @@
       </c>
       <c r="C282" t="str">
         <f>IF(COUNTIF(D:D,$A282)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>112</v>
+        <v>308</v>
       </c>
       <c r="F282" s="2"/>
     </row>
@@ -6115,10 +6115,10 @@
       </c>
       <c r="C283" t="str">
         <f>IF(COUNTIF(D:D,$A283)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="F283" s="2"/>
     </row>
@@ -6131,10 +6131,10 @@
       </c>
       <c r="C284" t="str">
         <f>IF(COUNTIF(D:D,$A284)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>113</v>
+        <v>314</v>
       </c>
       <c r="F284" s="2"/>
     </row>
@@ -6147,10 +6147,10 @@
       </c>
       <c r="C285" t="str">
         <f>IF(COUNTIF(D:D,$A285)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>362</v>
+        <v>268</v>
       </c>
       <c r="F285" s="2"/>
     </row>
@@ -6163,10 +6163,10 @@
       </c>
       <c r="C286" t="str">
         <f>IF(COUNTIF(D:D,$A286)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>375</v>
+        <v>316</v>
       </c>
       <c r="F286" s="2"/>
     </row>
@@ -6182,7 +6182,7 @@
         <v>Missing</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="F287" s="2"/>
     </row>
@@ -6198,7 +6198,7 @@
         <v>Missing</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>9</v>
+        <v>186</v>
       </c>
       <c r="F288" s="2"/>
     </row>
@@ -6214,7 +6214,7 @@
         <v>Missing</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>214</v>
+        <v>112</v>
       </c>
       <c r="F289" s="2"/>
     </row>
@@ -6230,7 +6230,7 @@
         <v>Missing</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>23</v>
+        <v>277</v>
       </c>
       <c r="F290" s="2"/>
     </row>
@@ -6246,7 +6246,7 @@
         <v>Missing</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>298</v>
+        <v>113</v>
       </c>
       <c r="F291" s="2"/>
     </row>
@@ -6262,7 +6262,7 @@
         <v>Missing</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>145</v>
+        <v>362</v>
       </c>
       <c r="F292" s="2"/>
     </row>
@@ -6278,7 +6278,7 @@
         <v>Missing</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>300</v>
+        <v>375</v>
       </c>
       <c r="F293" s="2"/>
     </row>
@@ -6294,7 +6294,7 @@
         <v>Missing</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="F294" s="2"/>
     </row>
@@ -6310,7 +6310,7 @@
         <v>Missing</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>302</v>
+        <v>9</v>
       </c>
       <c r="F295" s="2"/>
     </row>
@@ -6326,7 +6326,7 @@
         <v>Missing</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="F296" s="2"/>
     </row>
@@ -6342,7 +6342,7 @@
         <v>Missing</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F297" s="2"/>
     </row>
@@ -6358,7 +6358,7 @@
         <v>Missing</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>48</v>
+        <v>298</v>
       </c>
       <c r="F298" s="2"/>
     </row>
@@ -6374,7 +6374,7 @@
         <v>Missing</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F299" s="2"/>
     </row>
@@ -6390,7 +6390,7 @@
         <v>Missing</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="F300" s="2"/>
     </row>
@@ -6406,7 +6406,7 @@
         <v>Missing</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="F301" s="2"/>
     </row>
@@ -6422,7 +6422,7 @@
         <v>Missing</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>254</v>
+        <v>302</v>
       </c>
       <c r="F302" s="2"/>
     </row>
@@ -6438,7 +6438,7 @@
         <v>Implemented</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>166</v>
+        <v>242</v>
       </c>
       <c r="F303" s="2"/>
     </row>
@@ -6454,7 +6454,7 @@
         <v>Implemented</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>400</v>
+        <v>45</v>
       </c>
       <c r="F304" s="2"/>
     </row>
@@ -6470,7 +6470,7 @@
         <v>Implemented</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>258</v>
+        <v>48</v>
       </c>
       <c r="F305" s="2"/>
     </row>
@@ -6486,7 +6486,7 @@
         <v>Implemented</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="F306" s="2"/>
     </row>
@@ -6502,7 +6502,7 @@
         <v>Implemented</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>198</v>
+        <v>50</v>
       </c>
       <c r="F307" s="2"/>
     </row>
@@ -6518,7 +6518,7 @@
         <v>Implemented</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>371</v>
+        <v>64</v>
       </c>
       <c r="F308" s="2"/>
     </row>
@@ -6534,7 +6534,7 @@
         <v>Implemented</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>205</v>
+        <v>254</v>
       </c>
       <c r="F309" s="2"/>
     </row>
@@ -6550,7 +6550,7 @@
         <v>Implemented</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>383</v>
+        <v>166</v>
       </c>
       <c r="F310" s="2"/>
     </row>
@@ -6566,7 +6566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>384</v>
+        <v>400</v>
       </c>
       <c r="F311" s="2"/>
     </row>
@@ -6582,7 +6582,7 @@
         <v>Implemented</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
       <c r="F312" s="2"/>
     </row>
@@ -6598,7 +6598,7 @@
         <v>Implemented</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="F313" s="2"/>
     </row>
@@ -6614,7 +6614,7 @@
         <v>Implemented</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
       <c r="F314" s="2"/>
     </row>
@@ -6630,7 +6630,7 @@
         <v>Implemented</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>141</v>
+        <v>371</v>
       </c>
       <c r="F315" s="2"/>
     </row>
@@ -6646,7 +6646,7 @@
         <v>Implemented</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="F316" s="2"/>
     </row>
@@ -6662,7 +6662,7 @@
         <v>Implemented</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>39</v>
+        <v>383</v>
       </c>
       <c r="F317" s="2"/>
     </row>
@@ -6678,7 +6678,7 @@
         <v>Implemented</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>40</v>
+        <v>384</v>
       </c>
       <c r="F318" s="2"/>
     </row>
@@ -6694,7 +6694,7 @@
         <v>Implemented</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>241</v>
+        <v>292</v>
       </c>
       <c r="F319" s="2"/>
     </row>
@@ -6710,7 +6710,7 @@
         <v>Implemented</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="F320" s="2"/>
     </row>
@@ -6726,7 +6726,7 @@
         <v>Implemented</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -6742,7 +6742,7 @@
         <v>Implemented</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6758,7 +6758,7 @@
         <v>Implemented</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>315</v>
+        <v>236</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6774,7 +6774,7 @@
         <v>Implemented</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="F324" s="2"/>
     </row>
@@ -6790,7 +6790,7 @@
         <v>Implemented</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>103</v>
+        <v>40</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
@@ -6805,7 +6805,7 @@
         <v>Implemented</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>185</v>
+        <v>241</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
@@ -6820,7 +6820,7 @@
         <v>Implemented</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>107</v>
+        <v>153</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -6835,7 +6835,7 @@
         <v>Implemented</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>276</v>
+        <v>62</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
@@ -6850,7 +6850,7 @@
         <v>Implemented</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>397</v>
+        <v>87</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -6865,7 +6865,7 @@
         <v>Implemented</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>114</v>
+        <v>315</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
@@ -6880,7 +6880,7 @@
         <v>Implemented</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>368</v>
+        <v>177</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -6895,7 +6895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>200</v>
+        <v>103</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
@@ -6910,7 +6910,7 @@
         <v>Implemented</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>325</v>
+        <v>185</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
@@ -6925,7 +6925,7 @@
         <v>Implemented</v>
       </c>
       <c r="D334" s="2" t="s">
-        <v>286</v>
+        <v>107</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
@@ -6940,7 +6940,7 @@
         <v>Implemented</v>
       </c>
       <c r="D335" s="2" t="s">
-        <v>376</v>
+        <v>276</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
@@ -6955,7 +6955,7 @@
         <v>Implemented</v>
       </c>
       <c r="D336" s="2" t="s">
-        <v>124</v>
+        <v>397</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -6970,7 +6970,7 @@
         <v>Implemented</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -6985,7 +6985,7 @@
         <v>Implemented</v>
       </c>
       <c r="D338" s="2" t="s">
-        <v>220</v>
+        <v>368</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -7000,7 +7000,7 @@
         <v>Implemented</v>
       </c>
       <c r="D339" s="2" t="s">
-        <v>127</v>
+        <v>200</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -7015,7 +7015,7 @@
         <v>Implemented</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>296</v>
+        <v>325</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -7030,7 +7030,7 @@
         <v>Implemented</v>
       </c>
       <c r="D341" s="2" t="s">
-        <v>27</v>
+        <v>286</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -7045,7 +7045,7 @@
         <v>Implemented</v>
       </c>
       <c r="D342" s="2" t="s">
-        <v>30</v>
+        <v>376</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -7060,7 +7060,7 @@
         <v>Implemented</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>230</v>
+        <v>124</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -7075,7 +7075,7 @@
         <v>Implemented</v>
       </c>
       <c r="D344" s="2" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -7090,7 +7090,7 @@
         <v>Implemented</v>
       </c>
       <c r="D345" s="2" t="s">
-        <v>42</v>
+        <v>220</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
@@ -7105,7 +7105,7 @@
         <v>Implemented</v>
       </c>
       <c r="D346" s="2" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
@@ -7120,7 +7120,7 @@
         <v>Implemented</v>
       </c>
       <c r="D347" s="2" t="s">
-        <v>244</v>
+        <v>296</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
@@ -7135,7 +7135,7 @@
         <v>Implemented</v>
       </c>
       <c r="D348" s="2" t="s">
-        <v>305</v>
+        <v>27</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -7150,7 +7150,7 @@
         <v>Implemented</v>
       </c>
       <c r="D349" s="2" t="s">
-        <v>334</v>
+        <v>30</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
@@ -7165,7 +7165,7 @@
         <v>Implemented</v>
       </c>
       <c r="D350" s="2" t="s">
-        <v>63</v>
+        <v>230</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
@@ -7180,7 +7180,7 @@
         <v>Implemented</v>
       </c>
       <c r="D351" s="2" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -7195,7 +7195,7 @@
         <v>Implemented</v>
       </c>
       <c r="D352" s="2" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
@@ -7210,7 +7210,7 @@
         <v>Implemented</v>
       </c>
       <c r="D353" s="2" t="s">
-        <v>265</v>
+        <v>44</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
@@ -7225,7 +7225,7 @@
         <v>Implemented</v>
       </c>
       <c r="D354" s="2" t="s">
-        <v>180</v>
+        <v>244</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
@@ -7240,7 +7240,7 @@
         <v>Implemented</v>
       </c>
       <c r="D355" s="2" t="s">
-        <v>111</v>
+        <v>305</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
@@ -7255,7 +7255,7 @@
         <v>Implemented</v>
       </c>
       <c r="D356" s="2" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
@@ -7270,7 +7270,7 @@
         <v>Implemented</v>
       </c>
       <c r="D357" s="2" t="s">
-        <v>191</v>
+        <v>63</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
@@ -7285,7 +7285,7 @@
         <v>Implemented</v>
       </c>
       <c r="D358" s="2" t="s">
-        <v>283</v>
+        <v>162</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -7300,7 +7300,7 @@
         <v>Implemented</v>
       </c>
       <c r="D359" s="2" t="s">
-        <v>379</v>
+        <v>77</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -7315,7 +7315,7 @@
         <v>Implemented</v>
       </c>
       <c r="D360" s="2" t="s">
-        <v>381</v>
+        <v>265</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
@@ -7330,7 +7330,7 @@
         <v>Implemented</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
@@ -7345,7 +7345,7 @@
         <v>Implemented</v>
       </c>
       <c r="D362" s="2" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
@@ -7360,7 +7360,7 @@
         <v>Implemented</v>
       </c>
       <c r="D363" s="2" t="s">
-        <v>151</v>
+        <v>320</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
@@ -7375,7 +7375,7 @@
         <v>Implemented</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>245</v>
+        <v>191</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
@@ -7390,7 +7390,7 @@
         <v>Implemented</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>198</v>
+        <v>283</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
@@ -7405,7 +7405,7 @@
         <v>Implemented</v>
       </c>
       <c r="D366" s="2" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
@@ -7420,7 +7420,7 @@
         <v>Implemented</v>
       </c>
       <c r="D367" s="2" t="s">
-        <v>114</v>
+        <v>381</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -7435,7 +7435,7 @@
         <v>Implemented</v>
       </c>
       <c r="D368" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -7450,7 +7450,7 @@
         <v>Implemented</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7465,7 +7465,7 @@
         <v>Implemented</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
@@ -7480,7 +7480,7 @@
         <v>Implemented</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
@@ -7495,7 +7495,7 @@
         <v>Implemented</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>154</v>
+        <v>198</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
@@ -7510,7 +7510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D373" s="2" t="s">
-        <v>173</v>
+        <v>394</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
@@ -7525,7 +7525,7 @@
         <v>Implemented</v>
       </c>
       <c r="D374" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -7540,7 +7540,7 @@
         <v>Implemented</v>
       </c>
       <c r="D375" s="2" t="s">
-        <v>161</v>
+        <v>44</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -7555,7 +7555,7 @@
         <v>Implemented</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>203</v>
+        <v>63</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
@@ -7570,7 +7570,7 @@
         <v>Implemented</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
@@ -7585,7 +7585,7 @@
         <v>Implemented</v>
       </c>
       <c r="D378" s="2" t="s">
-        <v>134</v>
+        <v>228</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
@@ -7600,7 +7600,7 @@
         <v>Implemented</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
@@ -7615,7 +7615,7 @@
         <v>Implemented</v>
       </c>
       <c r="D380" s="2" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
@@ -7630,7 +7630,7 @@
         <v>Implemented</v>
       </c>
       <c r="D381" s="2" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
@@ -7644,6 +7644,9 @@
         <f>IF(COUNTIF(D:D,$A382)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D382" s="2" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
@@ -7656,144 +7659,172 @@
         <f>IF(COUNTIF(D:D,$A383)&gt;0,"Implemented","Missing")</f>
         <v>Implemented</v>
       </c>
+      <c r="D383" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D384" s="2" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
     </row>
     <row r="385" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D385" s="2" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
     </row>
     <row r="386" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D386" s="2" t="s">
-        <v>234</v>
+        <v>130</v>
       </c>
     </row>
     <row r="387" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D387" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="388" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D388" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="391" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D391" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="392" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D392" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="393" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D393" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="394" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D394" s="2" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D420" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D421" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D422" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D423" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D424" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D425" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D426" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="427" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D427" s="2" t="s">
-        <v>115</v>
+        <v>231</v>
       </c>
     </row>
     <row r="428" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D428" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="429" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D429" s="2" t="s">
-        <v>144</v>
+        <v>65</v>
       </c>
     </row>
     <row r="430" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D430" s="2" t="s">
-        <v>382</v>
+        <v>66</v>
       </c>
     </row>
     <row r="431" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D431" s="2" t="s">
-        <v>156</v>
+        <v>42</v>
       </c>
     </row>
     <row r="432" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D432" s="2" t="s">
-        <v>215</v>
+        <v>54</v>
       </c>
     </row>
     <row r="433" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D433" s="2" t="s">
-        <v>253</v>
+        <v>57</v>
       </c>
     </row>
     <row r="434" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D434" s="2" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
     <row r="435" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D435" s="2" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
     </row>
     <row r="436" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D436" s="2" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
     </row>
     <row r="437" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D437" s="2" t="s">
-        <v>155</v>
+        <v>382</v>
       </c>
     </row>
     <row r="438" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D438" s="2" t="s">
-        <v>227</v>
+        <v>156</v>
       </c>
     </row>
     <row r="439" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D439" s="2" t="s">
-        <v>85</v>
+        <v>215</v>
       </c>
     </row>
     <row r="440" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D440" s="2" t="s">
-        <v>123</v>
+        <v>253</v>
       </c>
     </row>
     <row r="441" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D441" s="2" t="s">
-        <v>238</v>
+        <v>132</v>
       </c>
     </row>
     <row r="442" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D442" s="2" t="s">
-        <v>366</v>
+        <v>167</v>
       </c>
     </row>
     <row r="443" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D443" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D444" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D445" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="446" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D446" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="447" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D447" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="448" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D448" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="449" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D449" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="450" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D450" s="2" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- implemented the following legendary cards: Ragnaros the Firelord, Sylvanas Windrunner, The Beast, The Black Knight, Tinkmaster Overspark, Ysera, Tirion Fordring - with this commit ALL cards except the Naxxramas Adventure cards have been implemented - introduced summon stack to make minions which summon other minions work correctly
</commit_message>
<xml_diff>
--- a/card_checklist.xlsx
+++ b/card_checklist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$367</definedName>
+    <definedName name="implemented_cards" localSheetId="0">Tabelle1!$D$2:$E$383</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="401">
   <si>
     <t>Cardname</t>
   </si>
@@ -1605,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K450"/>
+  <dimension ref="A1:K466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C284" sqref="C284"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="K8">
         <f>COUNTIF(C:C,"Implemented")</f>
-        <v>366</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="K9">
         <f>COUNTIF(C:C,"Missing")</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -4206,7 +4206,7 @@
         <v>Implemented</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>169</v>
+        <v>343</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>Implemented</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>80</v>
+        <v>169</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>Implemented</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>257</v>
+        <v>80</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4251,7 @@
         <v>Implemented</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>259</v>
+        <v>344</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>Implemented</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>Implemented</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,7 +4296,7 @@
         <v>Implemented</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>173</v>
+        <v>262</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
         <v>Implemented</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,7 +4326,7 @@
         <v>Implemented</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>312</v>
+        <v>263</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <v>Implemented</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4356,7 +4356,7 @@
         <v>Implemented</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>266</v>
+        <v>311</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,7 +4371,7 @@
         <v>Implemented</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>90</v>
+        <v>312</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,7 +4386,7 @@
         <v>Implemented</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>313</v>
+        <v>89</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>Implemented</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>91</v>
+        <v>266</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>Implemented</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,7 +4431,7 @@
         <v>Implemented</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>94</v>
+        <v>313</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4446,7 +4446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>95</v>
+        <v>346</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
         <v>Implemented</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>269</v>
+        <v>91</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
         <v>Implemented</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>178</v>
+        <v>93</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4491,7 @@
         <v>Implemented</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>270</v>
+        <v>347</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4506,7 @@
         <v>Implemented</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>179</v>
+        <v>94</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4521,7 +4521,7 @@
         <v>Implemented</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4536,7 +4536,7 @@
         <v>Implemented</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>271</v>
+        <v>390</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,7 +4551,7 @@
         <v>Implemented</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>99</v>
+        <v>348</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,7 +4566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>100</v>
+        <v>269</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
         <v>Implemented</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>101</v>
+        <v>178</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>Implemented</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>183</v>
+        <v>270</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +4611,7 @@
         <v>Implemented</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>318</v>
+        <v>179</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>Implemented</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>274</v>
+        <v>350</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +4641,7 @@
         <v>Implemented</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,7 +4656,7 @@
         <v>Implemented</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>110</v>
+        <v>271</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>Implemented</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>187</v>
+        <v>99</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>392</v>
+        <v>100</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +4701,7 @@
         <v>Implemented</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>189</v>
+        <v>101</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4716,7 +4716,7 @@
         <v>Implemented</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4731,7 +4731,7 @@
         <v>Implemented</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4746,7 +4746,7 @@
         <v>Implemented</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>195</v>
+        <v>274</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4761,7 +4761,7 @@
         <v>Implemented</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>196</v>
+        <v>106</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4776,7 +4776,7 @@
         <v>Implemented</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>197</v>
+        <v>110</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>Implemented</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>278</v>
+        <v>187</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>Implemented</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>365</v>
+        <v>392</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,7 +4821,7 @@
         <v>Implemented</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>366</v>
+        <v>189</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4836,7 @@
         <v>Implemented</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>367</v>
+        <v>190</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4851,7 +4851,7 @@
         <v>Implemented</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>393</v>
+        <v>322</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4866,7 +4866,7 @@
         <v>Implemented</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,7 +4881,7 @@
         <v>Implemented</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>280</v>
+        <v>196</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4896,7 +4896,7 @@
         <v>Implemented</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>281</v>
+        <v>197</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4911,7 +4911,7 @@
         <v>Implemented</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>201</v>
+        <v>278</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>204</v>
+        <v>365</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4941,7 +4941,7 @@
         <v>Implemented</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>282</v>
+        <v>366</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>Implemented</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>207</v>
+        <v>367</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4971,7 +4971,7 @@
         <v>Implemented</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>285</v>
+        <v>393</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,7 +4986,7 @@
         <v>Implemented</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>377</v>
+        <v>199</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,7 +5001,7 @@
         <v>Implemented</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>378</v>
+        <v>280</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5016,7 +5016,7 @@
         <v>Implemented</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5031,7 +5031,7 @@
         <v>Implemented</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>208</v>
+        <v>351</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>Implemented</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5061,7 +5061,7 @@
         <v>Implemented</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>385</v>
+        <v>352</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,7 +5076,7 @@
         <v>Implemented</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>210</v>
+        <v>353</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,7 +5091,7 @@
         <v>Implemented</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
         <v>Implemented</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>288</v>
+        <v>354</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,7 +5121,7 @@
         <v>Implemented</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>213</v>
+        <v>282</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,7 +5136,7 @@
         <v>Implemented</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
         <v>Implemented</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>125</v>
+        <v>285</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5166,7 +5166,7 @@
         <v>Implemented</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>291</v>
+        <v>377</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,7 +5181,7 @@
         <v>Implemented</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>225</v>
+        <v>378</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>Implemented</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>20</v>
+        <v>287</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5211,7 +5211,7 @@
         <v>Implemented</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5226,7 +5226,7 @@
         <v>Implemented</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>129</v>
+        <v>209</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>Implemented</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>31</v>
+        <v>385</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,7 +5256,7 @@
         <v>Implemented</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5271,7 +5271,7 @@
         <v>Implemented</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>Implemented</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>150</v>
+        <v>288</v>
       </c>
       <c r="F231" s="2"/>
     </row>
@@ -5302,7 +5302,7 @@
         <v>Implemented</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>57</v>
+        <v>213</v>
       </c>
       <c r="F232" s="2"/>
     </row>
@@ -5318,7 +5318,7 @@
         <v>Implemented</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>59</v>
+        <v>356</v>
       </c>
       <c r="F233" s="2"/>
     </row>
@@ -5334,7 +5334,7 @@
         <v>Implemented</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="F234" s="2"/>
     </row>
@@ -5350,7 +5350,7 @@
         <v>Implemented</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="F235" s="2"/>
     </row>
@@ -5366,7 +5366,7 @@
         <v>Implemented</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>248</v>
+        <v>291</v>
       </c>
       <c r="F236" s="2"/>
     </row>
@@ -5382,7 +5382,7 @@
         <v>Implemented</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>69</v>
+        <v>225</v>
       </c>
       <c r="F237" s="2"/>
     </row>
@@ -5398,7 +5398,7 @@
         <v>Implemented</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>309</v>
+        <v>20</v>
       </c>
       <c r="F238" s="2"/>
     </row>
@@ -5414,7 +5414,7 @@
         <v>Implemented</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5430,7 +5430,7 @@
         <v>Implemented</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5446,7 +5446,7 @@
         <v>Implemented</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>181</v>
+        <v>31</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5462,7 +5462,7 @@
         <v>Implemented</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>182</v>
+        <v>235</v>
       </c>
       <c r="F242" s="2"/>
     </row>
@@ -5478,7 +5478,7 @@
         <v>Implemented</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>324</v>
+        <v>239</v>
       </c>
       <c r="F243" s="2"/>
     </row>
@@ -5494,7 +5494,7 @@
         <v>Implemented</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>373</v>
+        <v>150</v>
       </c>
       <c r="F244" s="2"/>
     </row>
@@ -5510,7 +5510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>221</v>
+        <v>57</v>
       </c>
       <c r="F245" s="2"/>
     </row>
@@ -5526,7 +5526,7 @@
         <v>Implemented</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>297</v>
+        <v>59</v>
       </c>
       <c r="F246" s="2"/>
     </row>
@@ -5542,7 +5542,7 @@
         <v>Implemented</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="F247" s="2"/>
     </row>
@@ -5558,7 +5558,7 @@
         <v>Implemented</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="F248" s="2"/>
     </row>
@@ -5574,7 +5574,7 @@
         <v>Implemented</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F249" s="2"/>
     </row>
@@ -5590,7 +5590,7 @@
         <v>Implemented</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5606,7 +5606,7 @@
         <v>Implemented</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>67</v>
+        <v>309</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5622,7 +5622,7 @@
         <v>Implemented</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>161</v>
+        <v>78</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5638,7 +5638,7 @@
         <v>Implemented</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="F253" s="2"/>
     </row>
@@ -5654,7 +5654,7 @@
         <v>Implemented</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>256</v>
+        <v>181</v>
       </c>
       <c r="F254" s="2"/>
     </row>
@@ -5670,7 +5670,7 @@
         <v>Implemented</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>260</v>
+        <v>182</v>
       </c>
       <c r="F255" s="2"/>
     </row>
@@ -5686,7 +5686,7 @@
         <v>Implemented</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="F256" s="2"/>
     </row>
@@ -5702,7 +5702,7 @@
         <v>Implemented</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>83</v>
+        <v>355</v>
       </c>
       <c r="F257" s="2"/>
     </row>
@@ -5718,7 +5718,7 @@
         <v>Implemented</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>310</v>
+        <v>373</v>
       </c>
       <c r="F258" s="2"/>
     </row>
@@ -5734,7 +5734,7 @@
         <v>Implemented</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>84</v>
+        <v>221</v>
       </c>
       <c r="F259" s="2"/>
     </row>
@@ -5750,7 +5750,7 @@
         <v>Implemented</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>92</v>
+        <v>297</v>
       </c>
       <c r="F260" s="2"/>
     </row>
@@ -5766,7 +5766,7 @@
         <v>Implemented</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -5782,7 +5782,7 @@
         <v>Implemented</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>319</v>
+        <v>37</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -5798,7 +5798,7 @@
         <v>Implemented</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5814,7 +5814,7 @@
         <v>Implemented</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="F264" s="2"/>
     </row>
@@ -5830,7 +5830,7 @@
         <v>Implemented</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>109</v>
+        <v>67</v>
       </c>
       <c r="F265" s="2"/>
     </row>
@@ -5846,7 +5846,7 @@
         <v>Implemented</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -5862,7 +5862,7 @@
         <v>Implemented</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5878,7 +5878,7 @@
         <v>Implemented</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>203</v>
+        <v>256</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5894,7 +5894,7 @@
         <v>Implemented</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>18</v>
+        <v>260</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -5910,7 +5910,7 @@
         <v>Implemented</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -5926,7 +5926,7 @@
         <v>Implemented</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -5942,7 +5942,7 @@
         <v>Implemented</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>128</v>
+        <v>310</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -5958,7 +5958,7 @@
         <v>Implemented</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>224</v>
+        <v>84</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -5974,7 +5974,7 @@
         <v>Implemented</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="F274" s="2"/>
     </row>
@@ -5990,7 +5990,7 @@
         <v>Implemented</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>134</v>
+        <v>97</v>
       </c>
       <c r="F275" s="2"/>
     </row>
@@ -6006,7 +6006,7 @@
         <v>Implemented</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>36</v>
+        <v>349</v>
       </c>
       <c r="F276" s="2"/>
     </row>
@@ -6022,7 +6022,7 @@
         <v>Implemented</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>140</v>
+        <v>319</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -6038,7 +6038,7 @@
         <v>Implemented</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>333</v>
+        <v>275</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -6054,7 +6054,7 @@
         <v>Implemented</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="F279" s="2"/>
     </row>
@@ -6070,7 +6070,7 @@
         <v>Implemented</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="F280" s="2"/>
     </row>
@@ -6086,7 +6086,7 @@
         <v>Implemented</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>246</v>
+        <v>188</v>
       </c>
       <c r="F281" s="2"/>
     </row>
@@ -6102,7 +6102,7 @@
         <v>Implemented</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>308</v>
+        <v>202</v>
       </c>
       <c r="F282" s="2"/>
     </row>
@@ -6118,7 +6118,7 @@
         <v>Implemented</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>261</v>
+        <v>203</v>
       </c>
       <c r="F283" s="2"/>
     </row>
@@ -6134,7 +6134,7 @@
         <v>Implemented</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>314</v>
+        <v>18</v>
       </c>
       <c r="F284" s="2"/>
     </row>
@@ -6150,7 +6150,7 @@
         <v>Implemented</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>268</v>
+        <v>17</v>
       </c>
       <c r="F285" s="2"/>
     </row>
@@ -6166,7 +6166,7 @@
         <v>Implemented</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>316</v>
+        <v>19</v>
       </c>
       <c r="F286" s="2"/>
     </row>
@@ -6179,10 +6179,10 @@
       </c>
       <c r="C287" t="str">
         <f>IF(COUNTIF(D:D,$A287)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="F287" s="2"/>
     </row>
@@ -6195,10 +6195,10 @@
       </c>
       <c r="C288" t="str">
         <f>IF(COUNTIF(D:D,$A288)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>186</v>
+        <v>224</v>
       </c>
       <c r="F288" s="2"/>
     </row>
@@ -6211,10 +6211,10 @@
       </c>
       <c r="C289" t="str">
         <f>IF(COUNTIF(D:D,$A289)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="F289" s="2"/>
     </row>
@@ -6227,10 +6227,10 @@
       </c>
       <c r="C290" t="str">
         <f>IF(COUNTIF(D:D,$A290)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>277</v>
+        <v>134</v>
       </c>
       <c r="F290" s="2"/>
     </row>
@@ -6243,10 +6243,10 @@
       </c>
       <c r="C291" t="str">
         <f>IF(COUNTIF(D:D,$A291)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>113</v>
+        <v>36</v>
       </c>
       <c r="F291" s="2"/>
     </row>
@@ -6259,10 +6259,10 @@
       </c>
       <c r="C292" t="str">
         <f>IF(COUNTIF(D:D,$A292)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>362</v>
+        <v>140</v>
       </c>
       <c r="F292" s="2"/>
     </row>
@@ -6275,10 +6275,10 @@
       </c>
       <c r="C293" t="str">
         <f>IF(COUNTIF(D:D,$A293)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>375</v>
+        <v>333</v>
       </c>
       <c r="F293" s="2"/>
     </row>
@@ -6291,10 +6291,10 @@
       </c>
       <c r="C294" t="str">
         <f>IF(COUNTIF(D:D,$A294)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="F294" s="2"/>
     </row>
@@ -6307,10 +6307,10 @@
       </c>
       <c r="C295" t="str">
         <f>IF(COUNTIF(D:D,$A295)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F295" s="2"/>
     </row>
@@ -6323,10 +6323,10 @@
       </c>
       <c r="C296" t="str">
         <f>IF(COUNTIF(D:D,$A296)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="F296" s="2"/>
     </row>
@@ -6339,10 +6339,10 @@
       </c>
       <c r="C297" t="str">
         <f>IF(COUNTIF(D:D,$A297)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>23</v>
+        <v>308</v>
       </c>
       <c r="F297" s="2"/>
     </row>
@@ -6355,10 +6355,10 @@
       </c>
       <c r="C298" t="str">
         <f>IF(COUNTIF(D:D,$A298)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="F298" s="2"/>
     </row>
@@ -6371,10 +6371,10 @@
       </c>
       <c r="C299" t="str">
         <f>IF(COUNTIF(D:D,$A299)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>145</v>
+        <v>314</v>
       </c>
       <c r="F299" s="2"/>
     </row>
@@ -6387,10 +6387,10 @@
       </c>
       <c r="C300" t="str">
         <f>IF(COUNTIF(D:D,$A300)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>300</v>
+        <v>268</v>
       </c>
       <c r="F300" s="2"/>
     </row>
@@ -6403,10 +6403,10 @@
       </c>
       <c r="C301" t="str">
         <f>IF(COUNTIF(D:D,$A301)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>146</v>
+        <v>316</v>
       </c>
       <c r="F301" s="2"/>
     </row>
@@ -6419,10 +6419,10 @@
       </c>
       <c r="C302" t="str">
         <f>IF(COUNTIF(D:D,$A302)&gt;0,"Implemented","Missing")</f>
-        <v>Missing</v>
+        <v>Implemented</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>302</v>
+        <v>104</v>
       </c>
       <c r="F302" s="2"/>
     </row>
@@ -6438,7 +6438,7 @@
         <v>Implemented</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>242</v>
+        <v>186</v>
       </c>
       <c r="F303" s="2"/>
     </row>
@@ -6454,7 +6454,7 @@
         <v>Implemented</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="F304" s="2"/>
     </row>
@@ -6470,7 +6470,7 @@
         <v>Implemented</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>48</v>
+        <v>277</v>
       </c>
       <c r="F305" s="2"/>
     </row>
@@ -6486,7 +6486,7 @@
         <v>Implemented</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>155</v>
+        <v>113</v>
       </c>
       <c r="F306" s="2"/>
     </row>
@@ -6502,7 +6502,7 @@
         <v>Implemented</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>50</v>
+        <v>362</v>
       </c>
       <c r="F307" s="2"/>
     </row>
@@ -6518,7 +6518,7 @@
         <v>Implemented</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>64</v>
+        <v>375</v>
       </c>
       <c r="F308" s="2"/>
     </row>
@@ -6534,7 +6534,7 @@
         <v>Implemented</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>254</v>
+        <v>116</v>
       </c>
       <c r="F309" s="2"/>
     </row>
@@ -6550,7 +6550,7 @@
         <v>Implemented</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>166</v>
+        <v>9</v>
       </c>
       <c r="F310" s="2"/>
     </row>
@@ -6566,7 +6566,7 @@
         <v>Implemented</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>400</v>
+        <v>214</v>
       </c>
       <c r="F311" s="2"/>
     </row>
@@ -6582,7 +6582,7 @@
         <v>Implemented</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>258</v>
+        <v>23</v>
       </c>
       <c r="F312" s="2"/>
     </row>
@@ -6598,7 +6598,7 @@
         <v>Implemented</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>102</v>
+        <v>298</v>
       </c>
       <c r="F313" s="2"/>
     </row>
@@ -6614,7 +6614,7 @@
         <v>Implemented</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>198</v>
+        <v>145</v>
       </c>
       <c r="F314" s="2"/>
     </row>
@@ -6630,7 +6630,7 @@
         <v>Implemented</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>371</v>
+        <v>300</v>
       </c>
       <c r="F315" s="2"/>
     </row>
@@ -6646,7 +6646,7 @@
         <v>Implemented</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="F316" s="2"/>
     </row>
@@ -6662,7 +6662,7 @@
         <v>Implemented</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>383</v>
+        <v>302</v>
       </c>
       <c r="F317" s="2"/>
     </row>
@@ -6678,7 +6678,7 @@
         <v>Implemented</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>384</v>
+        <v>242</v>
       </c>
       <c r="F318" s="2"/>
     </row>
@@ -6694,7 +6694,7 @@
         <v>Implemented</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>292</v>
+        <v>45</v>
       </c>
       <c r="F319" s="2"/>
     </row>
@@ -6710,7 +6710,7 @@
         <v>Implemented</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>130</v>
+        <v>48</v>
       </c>
       <c r="F320" s="2"/>
     </row>
@@ -6726,7 +6726,7 @@
         <v>Implemented</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -6742,7 +6742,7 @@
         <v>Implemented</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>141</v>
+        <v>50</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6758,7 +6758,7 @@
         <v>Implemented</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>236</v>
+        <v>64</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6774,7 +6774,7 @@
         <v>Implemented</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>39</v>
+        <v>254</v>
       </c>
       <c r="F324" s="2"/>
     </row>
@@ -6790,7 +6790,7 @@
         <v>Implemented</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>40</v>
+        <v>166</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
@@ -6805,7 +6805,7 @@
         <v>Implemented</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>241</v>
+        <v>400</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
@@ -6820,7 +6820,7 @@
         <v>Implemented</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>153</v>
+        <v>258</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -6835,7 +6835,7 @@
         <v>Implemented</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
@@ -6850,7 +6850,7 @@
         <v>Implemented</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>87</v>
+        <v>198</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -6865,7 +6865,7 @@
         <v>Implemented</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>315</v>
+        <v>371</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
@@ -6880,7 +6880,7 @@
         <v>Implemented</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -6895,7 +6895,7 @@
         <v>Implemented</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>103</v>
+        <v>383</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
@@ -6910,7 +6910,7 @@
         <v>Implemented</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>185</v>
+        <v>384</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
@@ -6925,7 +6925,7 @@
         <v>Implemented</v>
       </c>
       <c r="D334" s="2" t="s">
-        <v>107</v>
+        <v>292</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
@@ -6940,7 +6940,7 @@
         <v>Implemented</v>
       </c>
       <c r="D335" s="2" t="s">
-        <v>276</v>
+        <v>130</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
@@ -6955,7 +6955,7 @@
         <v>Implemented</v>
       </c>
       <c r="D336" s="2" t="s">
-        <v>397</v>
+        <v>33</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -6970,7 +6970,7 @@
         <v>Implemented</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -6985,7 +6985,7 @@
         <v>Implemented</v>
       </c>
       <c r="D338" s="2" t="s">
-        <v>368</v>
+        <v>236</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -7000,7 +7000,7 @@
         <v>Implemented</v>
       </c>
       <c r="D339" s="2" t="s">
-        <v>200</v>
+        <v>39</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -7015,7 +7015,7 @@
         <v>Implemented</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>325</v>
+        <v>40</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -7030,7 +7030,7 @@
         <v>Implemented</v>
       </c>
       <c r="D341" s="2" t="s">
-        <v>286</v>
+        <v>241</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -7045,7 +7045,7 @@
         <v>Implemented</v>
       </c>
       <c r="D342" s="2" t="s">
-        <v>376</v>
+        <v>153</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -7060,7 +7060,7 @@
         <v>Implemented</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -7075,7 +7075,7 @@
         <v>Implemented</v>
       </c>
       <c r="D344" s="2" t="s">
-        <v>15</v>
+        <v>342</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -7090,7 +7090,7 @@
         <v>Implemented</v>
       </c>
       <c r="D345" s="2" t="s">
-        <v>220</v>
+        <v>87</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
@@ -7105,7 +7105,7 @@
         <v>Implemented</v>
       </c>
       <c r="D346" s="2" t="s">
-        <v>127</v>
+        <v>315</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
@@ -7120,7 +7120,7 @@
         <v>Implemented</v>
       </c>
       <c r="D347" s="2" t="s">
-        <v>296</v>
+        <v>177</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
@@ -7135,7 +7135,7 @@
         <v>Implemented</v>
       </c>
       <c r="D348" s="2" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -7150,7 +7150,7 @@
         <v>Implemented</v>
       </c>
       <c r="D349" s="2" t="s">
-        <v>30</v>
+        <v>185</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
@@ -7165,7 +7165,7 @@
         <v>Implemented</v>
       </c>
       <c r="D350" s="2" t="s">
-        <v>230</v>
+        <v>107</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
@@ -7180,7 +7180,7 @@
         <v>Implemented</v>
       </c>
       <c r="D351" s="2" t="s">
-        <v>136</v>
+        <v>276</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -7195,7 +7195,7 @@
         <v>Implemented</v>
       </c>
       <c r="D352" s="2" t="s">
-        <v>42</v>
+        <v>397</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
@@ -7210,7 +7210,7 @@
         <v>Implemented</v>
       </c>
       <c r="D353" s="2" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
@@ -7225,7 +7225,7 @@
         <v>Implemented</v>
       </c>
       <c r="D354" s="2" t="s">
-        <v>244</v>
+        <v>368</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
@@ -7240,7 +7240,7 @@
         <v>Implemented</v>
       </c>
       <c r="D355" s="2" t="s">
-        <v>305</v>
+        <v>200</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
@@ -7255,7 +7255,7 @@
         <v>Implemented</v>
       </c>
       <c r="D356" s="2" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
@@ -7270,7 +7270,7 @@
         <v>Implemented</v>
       </c>
       <c r="D357" s="2" t="s">
-        <v>63</v>
+        <v>286</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
@@ -7285,7 +7285,7 @@
         <v>Implemented</v>
       </c>
       <c r="D358" s="2" t="s">
-        <v>162</v>
+        <v>376</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -7300,7 +7300,7 @@
         <v>Implemented</v>
       </c>
       <c r="D359" s="2" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -7315,7 +7315,7 @@
         <v>Implemented</v>
       </c>
       <c r="D360" s="2" t="s">
-        <v>265</v>
+        <v>15</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
@@ -7330,7 +7330,7 @@
         <v>Implemented</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
@@ -7345,7 +7345,7 @@
         <v>Implemented</v>
       </c>
       <c r="D362" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
@@ -7360,7 +7360,7 @@
         <v>Implemented</v>
       </c>
       <c r="D363" s="2" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
@@ -7375,7 +7375,7 @@
         <v>Implemented</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
@@ -7390,7 +7390,7 @@
         <v>Implemented</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>283</v>
+        <v>30</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
@@ -7405,7 +7405,7 @@
         <v>Implemented</v>
       </c>
       <c r="D366" s="2" t="s">
-        <v>379</v>
+        <v>230</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
@@ -7420,7 +7420,7 @@
         <v>Implemented</v>
       </c>
       <c r="D367" s="2" t="s">
-        <v>381</v>
+        <v>136</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -7435,7 +7435,7 @@
         <v>Implemented</v>
       </c>
       <c r="D368" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -7450,7 +7450,7 @@
         <v>Implemented</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>137</v>
+        <v>44</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7465,7 +7465,7 @@
         <v>Implemented</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>151</v>
+        <v>244</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
@@ -7480,7 +7480,7 @@
         <v>Implemented</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>245</v>
+        <v>305</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
@@ -7495,7 +7495,7 @@
         <v>Implemented</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>198</v>
+        <v>334</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
@@ -7510,7 +7510,7 @@
         <v>Implemented</v>
       </c>
       <c r="D373" s="2" t="s">
-        <v>394</v>
+        <v>63</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
@@ -7525,7 +7525,7 @@
         <v>Implemented</v>
       </c>
       <c r="D374" s="2" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -7540,7 +7540,7 @@
         <v>Implemented</v>
       </c>
       <c r="D375" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -7555,7 +7555,7 @@
         <v>Implemented</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>63</v>
+        <v>265</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
@@ -7570,7 +7570,7 @@
         <v>Implemented</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>122</v>
+        <v>180</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
@@ -7585,7 +7585,7 @@
         <v>Implemented</v>
       </c>
       <c r="D378" s="2" t="s">
-        <v>228</v>
+        <v>111</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
@@ -7600,7 +7600,7 @@
         <v>Implemented</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>154</v>
+        <v>320</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
@@ -7615,7 +7615,7 @@
         <v>Implemented</v>
       </c>
       <c r="D380" s="2" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
@@ -7630,7 +7630,7 @@
         <v>Implemented</v>
       </c>
       <c r="D381" s="2" t="s">
-        <v>150</v>
+        <v>283</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
@@ -7645,7 +7645,7 @@
         <v>Implemented</v>
       </c>
       <c r="D382" s="2" t="s">
-        <v>161</v>
+        <v>379</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
@@ -7660,171 +7660,251 @@
         <v>Implemented</v>
       </c>
       <c r="D383" s="2" t="s">
-        <v>203</v>
+        <v>381</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D384" s="2" t="s">
-        <v>133</v>
+        <v>32</v>
       </c>
     </row>
     <row r="385" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D385" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="386" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D386" s="2" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
     </row>
     <row r="387" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D387" s="2" t="s">
-        <v>124</v>
+        <v>245</v>
       </c>
     </row>
     <row r="388" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D388" s="2" t="s">
-        <v>92</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="389" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D389" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="390" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D390" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="391" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D391" s="2" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
     </row>
     <row r="392" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D392" s="2" t="s">
-        <v>160</v>
+        <v>63</v>
       </c>
     </row>
     <row r="393" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D393" s="2" t="s">
-        <v>234</v>
+        <v>122</v>
       </c>
     </row>
     <row r="394" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D394" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="395" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D395" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="396" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D396" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="397" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D397" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="398" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D398" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="399" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D399" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="400" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D400" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="401" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D401" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="402" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D402" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="403" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D403" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="404" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D404" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="407" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D407" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="408" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D408" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="409" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D409" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="410" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D410" s="2" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D427" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D428" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D429" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D430" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D431" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D432" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D433" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D434" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D435" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D436" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D437" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D438" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D439" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D440" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D441" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D442" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="443" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D443" s="2" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="444" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D444" s="2" t="s">
-        <v>155</v>
+        <v>31</v>
       </c>
     </row>
     <row r="445" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D445" s="2" t="s">
-        <v>227</v>
+        <v>65</v>
       </c>
     </row>
     <row r="446" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D446" s="2" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="447" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D447" s="2" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
     </row>
     <row r="448" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D448" s="2" t="s">
-        <v>238</v>
+        <v>54</v>
       </c>
     </row>
     <row r="449" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D449" s="2" t="s">
-        <v>366</v>
+        <v>57</v>
       </c>
     </row>
     <row r="450" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D450" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="451" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D451" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="452" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D452" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="453" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D453" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="454" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D454" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="455" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D455" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="456" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D456" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="457" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D457" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="458" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D458" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="459" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D459" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="460" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D460" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="461" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D461" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="462" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D462" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="463" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D463" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="464" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D464" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="465" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D465" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="466" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D466" s="2" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>